<commit_message>
updated xl: btech-62-sem-2/4, bca-62-sem4
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 62 (btech-62)/4/1.xlsx
+++ b/raw/time_tables/B.Tech 62 (btech-62)/4/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fileserver2\time table\JIIT Time Table EVEN 2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\TT_27 jan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5323F501-85CB-408D-B8C8-A9446183B1D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DFC6E4-FBED-42A9-A258-2FE1B9972DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IV" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="579">
   <si>
     <t>B.Tech IV SEMESTER-EVEN SEM 2026</t>
   </si>
@@ -862,15 +862,9 @@
     <t>PB1,B2(25B16CS211)-CL21,22,23/BS,PAG,SMS</t>
   </si>
   <si>
-    <t>PB5,B6(CS222)-CL05,06/SYN,SUD,NIY</t>
-  </si>
-  <si>
     <t>PB10 (CS221) – CL07/AMT,SHV</t>
   </si>
   <si>
-    <t>PB1,B2(CS224)-CL02,03/TAJ,ATI,SHG</t>
-  </si>
-  <si>
     <t>PB11,B12(CS224)-CL11,12/ALK,AMT,TAJ</t>
   </si>
   <si>
@@ -886,9 +880,6 @@
     <t>LA17,A18(25B11MA231)-G9/MKB</t>
   </si>
   <si>
-    <t>LB10-B14(CS211)-FF9/NET</t>
-  </si>
-  <si>
     <t>LC1-C3(12BT311)-G6/SAJ</t>
   </si>
   <si>
@@ -988,9 +979,6 @@
     <t>LB9,B10 (CS223)-FF1/RJM</t>
   </si>
   <si>
-    <t>LB7,B8 (CS221)-FF8/KJ</t>
-  </si>
-  <si>
     <t>LB9,B10 (CS221)-FF9/DL</t>
   </si>
   <si>
@@ -1303,9 +1291,6 @@
     <t>TC2(BT211)-TS16/VGU, SBT</t>
   </si>
   <si>
-    <t>TB11 (CS221) – TS13/KJ</t>
-  </si>
-  <si>
     <t>TG1(25B11MA231)-TS16/GA</t>
   </si>
   <si>
@@ -1387,15 +1372,9 @@
     <t>LB(CS242)-G3/AYS</t>
   </si>
   <si>
-    <t>PMinor(24B15CS245)-CL01/MSI</t>
-  </si>
-  <si>
     <t>PMinor(24B15CS244)-CL02/AYS</t>
   </si>
   <si>
-    <t>PMinor(24B15CS245)-CL02/MSI</t>
-  </si>
-  <si>
     <t>PMinor(24B15CS244)-CL03/AYS</t>
   </si>
   <si>
@@ -1450,9 +1429,6 @@
     <t>TA1(15B11EC411)-TS13/RRJ</t>
   </si>
   <si>
-    <t>PB3,B14(CS221)-CL02,03/IC,TRN,KJ,MKT</t>
-  </si>
-  <si>
     <t>LB14,B16 (CS223)-FF9/PSO</t>
   </si>
   <si>
@@ -1531,9 +1507,6 @@
     <t>LA15,A16(25B21EC213)-FF8/KUL</t>
   </si>
   <si>
-    <t>PB16(CS221)-CL324/SHJ,TKT</t>
-  </si>
-  <si>
     <t>PG1(25B15MA233)-CL324/RSA</t>
   </si>
   <si>
@@ -1646,9 +1619,6 @@
   </si>
   <si>
     <t>PB7,B8(CS224)-CL13,14/AKM,DEP,ASI</t>
-  </si>
-  <si>
-    <t>PB14,B16(CS224)-CL14,15/AKM,SLK,ATI</t>
   </si>
   <si>
     <r>
@@ -1956,9 +1926,6 @@
     <t>PB11,12(CS221)-CL21, CL22 /TKT,VRN, MKT, RJM</t>
   </si>
   <si>
-    <t>PB1,B2,B4(CS221)-CL10,11,12/AST,TRN,TAJ,RJM</t>
-  </si>
-  <si>
     <t>PB7(CS221)-CL07/KJ,AST</t>
   </si>
   <si>
@@ -1966,9 +1933,6 @@
   </si>
   <si>
     <t>LG1,G2 (CS222)-CS5/AKM</t>
-  </si>
-  <si>
-    <t>TB16 (CS221) – TR326/TKT</t>
   </si>
   <si>
     <t>LG1,G2(MA222)-CS4/DCS</t>
@@ -2096,6 +2060,55 @@
         <family val="1"/>
       </rPr>
       <t>/MO</t>
+    </r>
+  </si>
+  <si>
+    <t>PB1,B2(CS224)-CL02,03/SLK,ATI,SHG</t>
+  </si>
+  <si>
+    <t>PB5,B6(CS222)-CL05,06/SYN,NIY</t>
+  </si>
+  <si>
+    <t>PB14(CS224)-CL14/AKM,ATI</t>
+  </si>
+  <si>
+    <t>TB11 (CS221) – TS13/TKT</t>
+  </si>
+  <si>
+    <t>PB1,B2,B4(CS221)-CL10,11,12/AST,TRN,TAJ,RJM,KJ</t>
+  </si>
+  <si>
+    <t>PB3,B14(CS221)-CL02,03/TRN,KJ,MKT</t>
+  </si>
+  <si>
+    <t>PMinor(24B15CS245)-CL01/NET</t>
+  </si>
+  <si>
+    <t>PMinor(24B15CS245)-CL324/NET</t>
+  </si>
+  <si>
+    <t>LB10-B14(CS211)-LT3/NET</t>
+  </si>
+  <si>
+    <r>
+      <t>LB7,B8 (CS221)-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>G8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/KJ</t>
     </r>
   </si>
 </sst>
@@ -2269,7 +2282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2407,11 +2420,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2636,9 +2662,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2659,26 +2682,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2691,11 +2694,114 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -2703,126 +2809,73 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3046,10 +3099,10 @@
   <dimension ref="A1:AA1060"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3070,18 +3123,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="122"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="114"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
@@ -3100,7 +3153,7 @@
     </row>
     <row r="2" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>1</v>
@@ -3143,7 +3196,7 @@
       <c r="Y2" s="9"/>
     </row>
     <row r="3" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="131" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="12"/>
@@ -3154,8 +3207,8 @@
       <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>426</v>
+      <c r="G3" s="96" t="s">
+        <v>575</v>
       </c>
       <c r="I3" s="69" t="s">
         <v>15</v>
@@ -3180,24 +3233,24 @@
       <c r="Y3" s="9"/>
     </row>
     <row r="4" spans="1:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="112"/>
+      <c r="A4" s="103"/>
       <c r="C4" s="77" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="F4" s="111" t="s">
+        <v>473</v>
+      </c>
+      <c r="F4" s="124" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="I4" s="69" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="K4" s="71"/>
       <c r="L4" s="9"/>
@@ -3216,28 +3269,28 @@
       <c r="Y4" s="9"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
-      <c r="C5" s="102" t="s">
-        <v>549</v>
+      <c r="A5" s="103"/>
+      <c r="C5" s="93" t="s">
+        <v>538</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E5" s="69" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="112"/>
-      <c r="G5" s="128" t="s">
-        <v>431</v>
-      </c>
-      <c r="H5" s="103" t="s">
-        <v>327</v>
+      <c r="F5" s="103"/>
+      <c r="G5" s="104" t="s">
+        <v>424</v>
+      </c>
+      <c r="H5" s="94" t="s">
+        <v>323</v>
       </c>
       <c r="I5" s="69" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="69" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -3256,25 +3309,25 @@
       <c r="Y5" s="9"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
+      <c r="A6" s="103"/>
       <c r="C6" s="2" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F6" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="129"/>
+      <c r="G6" s="105"/>
       <c r="H6" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="I6" s="93" t="s">
-        <v>269</v>
+        <v>262</v>
+      </c>
+      <c r="I6" s="141" t="s">
+        <v>266</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -3293,12 +3346,12 @@
       <c r="Y6" s="9"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
+      <c r="A7" s="103"/>
       <c r="C7" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>25</v>
@@ -3306,9 +3359,9 @@
       <c r="F7" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="129"/>
+      <c r="G7" s="105"/>
       <c r="H7" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I7" s="69" t="s">
         <v>21</v>
@@ -3331,22 +3384,22 @@
       <c r="Y7" s="9"/>
     </row>
     <row r="8" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="112"/>
+      <c r="A8" s="103"/>
       <c r="C8" s="4" t="s">
         <v>229</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="E8" s="93" t="s">
-        <v>255</v>
+        <v>475</v>
+      </c>
+      <c r="E8" s="141" t="s">
+        <v>253</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>521</v>
-      </c>
-      <c r="G8" s="129"/>
+        <v>511</v>
+      </c>
+      <c r="G8" s="105"/>
       <c r="H8" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -3365,22 +3418,22 @@
       <c r="Y8" s="9"/>
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
+      <c r="A9" s="103"/>
       <c r="C9" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="E9" s="93" t="s">
-        <v>256</v>
+        <v>319</v>
+      </c>
+      <c r="E9" s="141" t="s">
+        <v>254</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="G9" s="129"/>
+        <v>331</v>
+      </c>
+      <c r="G9" s="105"/>
       <c r="H9" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I9" s="3"/>
       <c r="K9" s="9"/>
@@ -3400,19 +3453,19 @@
       <c r="Y9" s="9"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
+      <c r="A10" s="103"/>
       <c r="D10" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E10" s="69" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G10" s="129"/>
+        <v>322</v>
+      </c>
+      <c r="G10" s="105"/>
       <c r="H10" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="16"/>
@@ -3433,17 +3486,17 @@
       <c r="AA10" s="17"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
+      <c r="A11" s="103"/>
       <c r="C11" s="4" t="s">
         <v>241</v>
       </c>
       <c r="E11" s="69" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="G11" s="129"/>
+        <v>412</v>
+      </c>
+      <c r="G11" s="105"/>
       <c r="H11" s="69"/>
       <c r="K11" s="9"/>
       <c r="L11" s="16"/>
@@ -3464,20 +3517,20 @@
       <c r="AA11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="112"/>
+      <c r="A12" s="103"/>
       <c r="C12" s="77"/>
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="G12" s="129"/>
+        <v>415</v>
+      </c>
+      <c r="G12" s="105"/>
       <c r="H12" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I12" s="94" t="s">
-        <v>390</v>
+      <c r="I12" s="142" t="s">
+        <v>386</v>
       </c>
       <c r="J12" s="69"/>
       <c r="K12" s="9"/>
@@ -3499,22 +3552,22 @@
       <c r="AA12" s="17"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
+      <c r="A13" s="103"/>
       <c r="C13" s="67" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="E13" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="87" t="s">
-        <v>498</v>
-      </c>
-      <c r="G13" s="129"/>
+      <c r="F13" s="86" t="s">
+        <v>489</v>
+      </c>
+      <c r="G13" s="105"/>
       <c r="H13" s="4" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="J13" s="69"/>
       <c r="K13" s="9"/>
@@ -3536,24 +3589,24 @@
       <c r="AA13" s="17"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
+      <c r="A14" s="103"/>
       <c r="C14" s="2" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="E14" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="129"/>
+      <c r="G14" s="105"/>
       <c r="H14" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="I14" s="113" t="s">
-        <v>568</v>
-      </c>
-      <c r="J14" s="112"/>
+        <v>434</v>
+      </c>
+      <c r="I14" s="126" t="s">
+        <v>556</v>
+      </c>
+      <c r="J14" s="103"/>
       <c r="K14" s="9"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -3573,7 +3626,7 @@
       <c r="AA14" s="17"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
+      <c r="A15" s="103"/>
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
@@ -3581,16 +3634,16 @@
         <v>70</v>
       </c>
       <c r="F15" s="69" t="s">
-        <v>262</v>
-      </c>
-      <c r="G15" s="129"/>
-      <c r="H15" s="86" t="s">
-        <v>532</v>
-      </c>
-      <c r="I15" s="113" t="s">
-        <v>569</v>
-      </c>
-      <c r="J15" s="112"/>
+        <v>259</v>
+      </c>
+      <c r="G15" s="105"/>
+      <c r="H15" s="85" t="s">
+        <v>522</v>
+      </c>
+      <c r="I15" s="126" t="s">
+        <v>557</v>
+      </c>
+      <c r="J15" s="103"/>
       <c r="K15" s="9"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -3610,19 +3663,19 @@
       <c r="AA15" s="17"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
+      <c r="A16" s="103"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F16" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="G16" s="129"/>
-      <c r="I16" s="113" t="s">
+        <v>260</v>
+      </c>
+      <c r="G16" s="105"/>
+      <c r="I16" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="112"/>
+      <c r="J16" s="103"/>
       <c r="K16" s="9"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -3642,20 +3695,20 @@
       <c r="AA16" s="17"/>
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
+      <c r="A17" s="103"/>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G17" s="129"/>
+        <v>353</v>
+      </c>
+      <c r="E17" s="96" t="s">
+        <v>577</v>
+      </c>
+      <c r="G17" s="105"/>
       <c r="H17" s="72"/>
-      <c r="I17" s="105" t="s">
-        <v>347</v>
-      </c>
-      <c r="J17" s="106"/>
+      <c r="I17" s="108" t="s">
+        <v>343</v>
+      </c>
+      <c r="J17" s="101"/>
       <c r="K17" s="9"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
@@ -3675,13 +3728,13 @@
       <c r="AA17" s="17"/>
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
+      <c r="A18" s="103"/>
       <c r="C18" s="4"/>
-      <c r="G18" s="129"/>
-      <c r="I18" s="105" t="s">
+      <c r="G18" s="105"/>
+      <c r="I18" s="108" t="s">
         <v>187</v>
       </c>
-      <c r="J18" s="106"/>
+      <c r="J18" s="101"/>
       <c r="K18" s="9"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
@@ -3701,17 +3754,17 @@
       <c r="AA18" s="17"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
+      <c r="A19" s="103"/>
       <c r="C19" s="4"/>
-      <c r="E19" s="95" t="s">
-        <v>488</v>
+      <c r="E19" s="143" t="s">
+        <v>479</v>
       </c>
       <c r="F19" s="69"/>
-      <c r="G19" s="129"/>
-      <c r="I19" s="105" t="s">
+      <c r="G19" s="105"/>
+      <c r="I19" s="108" t="s">
         <v>213</v>
       </c>
-      <c r="J19" s="106"/>
+      <c r="J19" s="101"/>
       <c r="K19" s="9"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -3731,19 +3784,19 @@
       <c r="AA19" s="17"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
+      <c r="A20" s="103"/>
       <c r="C20" s="4"/>
       <c r="D20" s="73" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>260</v>
-      </c>
-      <c r="G20" s="129"/>
-      <c r="I20" s="105" t="s">
+        <v>257</v>
+      </c>
+      <c r="G20" s="105"/>
+      <c r="I20" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="J20" s="106"/>
+      <c r="J20" s="101"/>
       <c r="K20" s="9"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
@@ -3763,19 +3816,19 @@
       <c r="AA20" s="17"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
+      <c r="A21" s="103"/>
       <c r="C21" s="4"/>
       <c r="E21" s="4" t="s">
         <v>235</v>
       </c>
       <c r="F21" s="69" t="s">
-        <v>570</v>
-      </c>
-      <c r="G21" s="129"/>
-      <c r="H21" s="105" t="s">
+        <v>558</v>
+      </c>
+      <c r="G21" s="105"/>
+      <c r="H21" s="108" t="s">
         <v>200</v>
       </c>
-      <c r="I21" s="106"/>
+      <c r="I21" s="101"/>
       <c r="K21" s="9"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
@@ -3795,18 +3848,18 @@
       <c r="AA21" s="17"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112"/>
+      <c r="A22" s="103"/>
       <c r="C22" s="4"/>
       <c r="E22" s="4" t="s">
         <v>239</v>
       </c>
       <c r="F22" s="69"/>
-      <c r="G22" s="129"/>
+      <c r="G22" s="105"/>
       <c r="H22" s="72"/>
-      <c r="I22" s="105" t="s">
+      <c r="I22" s="108" t="s">
         <v>217</v>
       </c>
-      <c r="J22" s="106"/>
+      <c r="J22" s="101"/>
       <c r="K22" s="9"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
@@ -3826,18 +3879,18 @@
       <c r="AA22" s="17"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="112"/>
+      <c r="A23" s="103"/>
       <c r="C23" s="4"/>
       <c r="E23" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F23" s="69"/>
-      <c r="G23" s="129"/>
+      <c r="G23" s="105"/>
       <c r="H23" s="72"/>
-      <c r="I23" s="105" t="s">
+      <c r="I23" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="J23" s="106"/>
+      <c r="J23" s="101"/>
       <c r="K23" s="9"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
@@ -3856,13 +3909,13 @@
       <c r="AA23" s="17"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="112"/>
+      <c r="A24" s="103"/>
       <c r="C24" s="4"/>
       <c r="F24" s="69"/>
-      <c r="G24" s="129"/>
+      <c r="G24" s="105"/>
       <c r="H24" s="72"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="122"/>
+      <c r="I24" s="113"/>
+      <c r="J24" s="114"/>
       <c r="K24" s="9"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
@@ -3881,15 +3934,15 @@
       <c r="AA24" s="17"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="112"/>
+      <c r="A25" s="103"/>
       <c r="C25" s="4"/>
       <c r="F25" s="69"/>
-      <c r="G25" s="129"/>
+      <c r="G25" s="105"/>
       <c r="H25" s="72"/>
-      <c r="I25" s="105" t="s">
-        <v>525</v>
-      </c>
-      <c r="J25" s="106"/>
+      <c r="I25" s="108" t="s">
+        <v>515</v>
+      </c>
+      <c r="J25" s="101"/>
       <c r="K25" s="9"/>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
@@ -3908,15 +3961,15 @@
       <c r="AA25" s="17"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="112"/>
+      <c r="A26" s="103"/>
       <c r="C26" s="4"/>
       <c r="F26" s="69"/>
-      <c r="G26" s="129"/>
+      <c r="G26" s="105"/>
       <c r="H26" s="72"/>
-      <c r="I26" s="105" t="s">
-        <v>578</v>
-      </c>
-      <c r="J26" s="106"/>
+      <c r="I26" s="108" t="s">
+        <v>566</v>
+      </c>
+      <c r="J26" s="101"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
@@ -3933,14 +3986,14 @@
       <c r="Y26" s="9"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="112"/>
+      <c r="A27" s="103"/>
       <c r="C27" s="4"/>
       <c r="F27" s="69"/>
-      <c r="G27" s="129"/>
-      <c r="H27" s="105" t="s">
-        <v>579</v>
-      </c>
-      <c r="I27" s="106"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="108" t="s">
+        <v>567</v>
+      </c>
+      <c r="I27" s="101"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -3957,10 +4010,10 @@
       <c r="Y27" s="9"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="112"/>
+      <c r="A28" s="103"/>
       <c r="C28" s="4"/>
       <c r="F28" s="69"/>
-      <c r="G28" s="130"/>
+      <c r="G28" s="132"/>
       <c r="H28" s="72"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -4004,7 +4057,7 @@
       <c r="Y29" s="9"/>
     </row>
     <row r="30" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="118" t="s">
+      <c r="A30" s="98" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="12"/>
@@ -4015,13 +4068,13 @@
         <v>12</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H30" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="J30" s="69" t="s">
         <v>30</v>
@@ -4042,21 +4095,21 @@
       <c r="Y30" s="9"/>
     </row>
     <row r="31" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="119"/>
+      <c r="A31" s="99"/>
       <c r="C31" s="69" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="D31" s="69" t="s">
         <v>32</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="F31" s="111" t="s">
+        <v>270</v>
+      </c>
+      <c r="F31" s="124" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="I31" s="69" t="s">
         <v>33</v>
@@ -4080,22 +4133,22 @@
       <c r="Y31" s="9"/>
     </row>
     <row r="32" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="119"/>
+      <c r="A32" s="99"/>
       <c r="C32" s="69" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>274</v>
-      </c>
-      <c r="F32" s="112"/>
+        <v>271</v>
+      </c>
+      <c r="F32" s="103"/>
       <c r="G32" s="2" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>36</v>
@@ -4119,25 +4172,25 @@
       <c r="Y32" s="9"/>
     </row>
     <row r="33" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="119"/>
+      <c r="A33" s="99"/>
       <c r="C33" s="69" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F33" s="69" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -4155,26 +4208,26 @@
       <c r="Y33" s="9"/>
     </row>
     <row r="34" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="119"/>
+      <c r="A34" s="99"/>
       <c r="C34" s="23" t="s">
-        <v>358</v>
-      </c>
-      <c r="D34" s="93" t="s">
-        <v>333</v>
+        <v>354</v>
+      </c>
+      <c r="D34" s="141" t="s">
+        <v>329</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="I34" s="93" t="s">
+        <v>469</v>
+      </c>
+      <c r="I34" s="141" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="2" t="s">
@@ -4198,27 +4251,24 @@
       <c r="AA34" s="17"/>
     </row>
     <row r="35" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="119"/>
+      <c r="A35" s="99"/>
       <c r="C35" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D35" s="93" t="s">
-        <v>332</v>
+        <v>268</v>
+      </c>
+      <c r="D35" s="141" t="s">
+        <v>328</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="F35" s="111" t="s">
-        <v>521</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>428</v>
+        <v>273</v>
+      </c>
+      <c r="F35" s="124" t="s">
+        <v>511</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="I35" s="93" t="s">
-        <v>286</v>
+        <v>470</v>
+      </c>
+      <c r="I35" s="141" t="s">
+        <v>283</v>
       </c>
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
@@ -4238,22 +4288,22 @@
       <c r="AA35" s="17"/>
     </row>
     <row r="36" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="119"/>
+      <c r="A36" s="99"/>
       <c r="D36" s="69" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="F36" s="112"/>
+        <v>274</v>
+      </c>
+      <c r="F36" s="103"/>
       <c r="G36" s="2" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
@@ -4273,25 +4323,25 @@
       <c r="AA36" s="17"/>
     </row>
     <row r="37" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="119"/>
+      <c r="A37" s="99"/>
       <c r="C37" s="24"/>
       <c r="D37" s="69" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G37" s="128" t="s">
-        <v>431</v>
+        <v>275</v>
+      </c>
+      <c r="G37" s="104" t="s">
+        <v>424</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="I37" s="90" t="s">
-        <v>435</v>
+        <v>281</v>
+      </c>
+      <c r="I37" s="144" t="s">
+        <v>428</v>
       </c>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
@@ -4311,23 +4361,21 @@
       <c r="AA37" s="17"/>
     </row>
     <row r="38" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="119"/>
+      <c r="A38" s="99"/>
       <c r="D38" s="23" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="G38" s="129"/>
+        <v>413</v>
+      </c>
+      <c r="G38" s="105"/>
       <c r="H38" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I38" s="90" t="s">
-        <v>550</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="I38" s="89"/>
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
@@ -4346,20 +4394,20 @@
       <c r="AA38" s="17"/>
     </row>
     <row r="39" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="119"/>
+      <c r="A39" s="99"/>
       <c r="D39" s="69"/>
       <c r="E39" s="24" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="G39" s="129"/>
+        <v>416</v>
+      </c>
+      <c r="G39" s="105"/>
       <c r="H39" s="2" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="I39" s="73" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="J39" s="72" t="s">
         <v>230</v>
@@ -4383,14 +4431,14 @@
       <c r="AA39" s="17"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="119"/>
+      <c r="A40" s="99"/>
       <c r="E40" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="F40" s="87" t="s">
-        <v>498</v>
-      </c>
-      <c r="G40" s="129"/>
+        <v>483</v>
+      </c>
+      <c r="F40" s="86" t="s">
+        <v>489</v>
+      </c>
+      <c r="G40" s="105"/>
       <c r="J40" s="72" t="s">
         <v>232</v>
       </c>
@@ -4413,18 +4461,18 @@
       <c r="AA40" s="17"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="119"/>
+      <c r="A41" s="99"/>
       <c r="E41" s="69"/>
       <c r="F41" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="G41" s="129"/>
+        <v>258</v>
+      </c>
+      <c r="G41" s="105"/>
       <c r="H41" s="1" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="72" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
@@ -4445,16 +4493,16 @@
       <c r="AA41" s="17"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="119"/>
+      <c r="A42" s="99"/>
       <c r="D42" s="4" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="F42" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G42" s="129"/>
+        <v>276</v>
+      </c>
+      <c r="G42" s="105"/>
       <c r="H42" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="7"/>
@@ -4477,17 +4525,17 @@
       <c r="AA42" s="17"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="119"/>
+      <c r="A43" s="99"/>
       <c r="D43" s="4" t="s">
         <v>238</v>
       </c>
       <c r="E43" s="69"/>
       <c r="F43" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="G43" s="129"/>
+        <v>277</v>
+      </c>
+      <c r="G43" s="105"/>
       <c r="J43" s="69" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
@@ -4506,22 +4554,23 @@
       <c r="Y43" s="9"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="119"/>
+      <c r="A44" s="99"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="91" t="s">
-        <v>539</v>
-      </c>
+      <c r="C44" s="153" t="s">
+        <v>529</v>
+      </c>
+      <c r="D44" s="154"/>
       <c r="E44" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G44" s="129"/>
+      <c r="G44" s="105"/>
       <c r="H44" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="I44" s="105" t="s">
+        <v>355</v>
+      </c>
+      <c r="I44" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="J44" s="106"/>
+      <c r="J44" s="101"/>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
@@ -4539,23 +4588,23 @@
       <c r="Y44" s="9"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="119"/>
+      <c r="A45" s="99"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="105" t="s">
+      <c r="C45" s="108" t="s">
         <v>189</v>
       </c>
-      <c r="D45" s="106"/>
+      <c r="D45" s="101"/>
       <c r="F45" s="79" t="s">
-        <v>524</v>
-      </c>
-      <c r="G45" s="129"/>
+        <v>514</v>
+      </c>
+      <c r="G45" s="105"/>
       <c r="H45" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="I45" s="105" t="s">
+        <v>356</v>
+      </c>
+      <c r="I45" s="108" t="s">
         <v>210</v>
       </c>
-      <c r="J45" s="106"/>
+      <c r="J45" s="101"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
@@ -4573,20 +4622,20 @@
       <c r="Y45" s="9"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="119"/>
+      <c r="A46" s="99"/>
       <c r="B46" s="6"/>
       <c r="C46" s="109" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="D46" s="110"/>
       <c r="E46" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G46" s="129"/>
-      <c r="I46" s="105" t="s">
+      <c r="G46" s="105"/>
+      <c r="I46" s="108" t="s">
         <v>190</v>
       </c>
-      <c r="J46" s="106"/>
+      <c r="J46" s="101"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
@@ -4604,20 +4653,20 @@
       <c r="Y46" s="9"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="119"/>
+      <c r="A47" s="99"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="105" t="s">
+      <c r="C47" s="108" t="s">
         <v>227</v>
       </c>
-      <c r="D47" s="106"/>
-      <c r="E47" s="94" t="s">
-        <v>391</v>
-      </c>
-      <c r="G47" s="129"/>
-      <c r="I47" s="105" t="s">
-        <v>515</v>
-      </c>
-      <c r="J47" s="106"/>
+      <c r="D47" s="101"/>
+      <c r="E47" s="142" t="s">
+        <v>387</v>
+      </c>
+      <c r="G47" s="105"/>
+      <c r="I47" s="108" t="s">
+        <v>505</v>
+      </c>
+      <c r="J47" s="101"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
@@ -4635,20 +4684,20 @@
       <c r="Y47" s="9"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="119"/>
-      <c r="C48" s="105" t="s">
-        <v>490</v>
-      </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="94" t="s">
-        <v>392</v>
+      <c r="A48" s="99"/>
+      <c r="C48" s="108" t="s">
+        <v>481</v>
+      </c>
+      <c r="D48" s="101"/>
+      <c r="E48" s="142" t="s">
+        <v>388</v>
       </c>
       <c r="F48" s="69"/>
-      <c r="G48" s="129"/>
-      <c r="I48" s="105" t="s">
-        <v>253</v>
-      </c>
-      <c r="J48" s="106"/>
+      <c r="G48" s="105"/>
+      <c r="I48" s="115" t="s">
+        <v>569</v>
+      </c>
+      <c r="J48" s="116"/>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
@@ -4666,21 +4715,21 @@
       <c r="Y48" s="9"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="119"/>
+      <c r="A49" s="99"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="145" t="s">
-        <v>526</v>
-      </c>
-      <c r="D49" s="146"/>
-      <c r="E49" s="105" t="s">
-        <v>464</v>
-      </c>
-      <c r="F49" s="106"/>
-      <c r="G49" s="129"/>
-      <c r="I49" s="105" t="s">
-        <v>251</v>
-      </c>
-      <c r="J49" s="106"/>
+      <c r="C49" s="106" t="s">
+        <v>516</v>
+      </c>
+      <c r="D49" s="107"/>
+      <c r="E49" s="108" t="s">
+        <v>456</v>
+      </c>
+      <c r="F49" s="101"/>
+      <c r="G49" s="105"/>
+      <c r="I49" s="115" t="s">
+        <v>570</v>
+      </c>
+      <c r="J49" s="116"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
@@ -4698,19 +4747,19 @@
       <c r="Y49" s="9"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="119"/>
+      <c r="A50" s="99"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="105" t="s">
-        <v>491</v>
-      </c>
-      <c r="D50" s="106"/>
+      <c r="C50" s="108" t="s">
+        <v>482</v>
+      </c>
+      <c r="D50" s="101"/>
       <c r="E50" s="69"/>
       <c r="F50" s="69"/>
-      <c r="G50" s="129"/>
-      <c r="I50" s="105" t="s">
-        <v>493</v>
-      </c>
-      <c r="J50" s="106"/>
+      <c r="G50" s="105"/>
+      <c r="I50" s="108" t="s">
+        <v>484</v>
+      </c>
+      <c r="J50" s="101"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
@@ -4728,15 +4777,15 @@
       <c r="Y50" s="9"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="119"/>
+      <c r="A51" s="99"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="105" t="s">
-        <v>512</v>
-      </c>
-      <c r="D51" s="106"/>
+      <c r="C51" s="158" t="s">
+        <v>503</v>
+      </c>
+      <c r="D51" s="157"/>
       <c r="E51" s="69"/>
       <c r="F51" s="69"/>
-      <c r="G51" s="129"/>
+      <c r="G51" s="105"/>
       <c r="I51" s="70"/>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -4755,17 +4804,17 @@
       <c r="Y51" s="9"/>
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="120"/>
-      <c r="C52" s="105" t="s">
+      <c r="A52" s="100"/>
+      <c r="C52" s="108" t="s">
         <v>188</v>
       </c>
-      <c r="D52" s="106"/>
+      <c r="D52" s="101"/>
       <c r="E52" s="69"/>
       <c r="F52" s="69"/>
-      <c r="G52" s="129"/>
+      <c r="G52" s="105"/>
       <c r="H52" s="25"/>
-      <c r="I52" s="131"/>
-      <c r="J52" s="132"/>
+      <c r="I52" s="122"/>
+      <c r="J52" s="123"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
@@ -4789,7 +4838,7 @@
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="129"/>
+      <c r="G53" s="105"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
@@ -4810,11 +4859,11 @@
       <c r="Y53" s="9"/>
     </row>
     <row r="54" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="107" t="s">
+      <c r="A54" s="133" t="s">
         <v>40</v>
       </c>
       <c r="B54" s="27"/>
-      <c r="G54" s="129"/>
+      <c r="G54" s="105"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -4832,8 +4881,8 @@
       <c r="Y54" s="9"/>
     </row>
     <row r="55" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="108"/>
-      <c r="G55" s="129"/>
+      <c r="A55" s="134"/>
+      <c r="G55" s="105"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -4851,7 +4900,7 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="56" spans="1:27" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="108"/>
+      <c r="A56" s="134"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -4877,18 +4926,18 @@
       <c r="Y56" s="9"/>
     </row>
     <row r="57" spans="1:27" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="108"/>
+      <c r="A57" s="134"/>
       <c r="D57" s="69" t="s">
         <v>46</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F57" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="128" t="s">
-        <v>431</v>
+      <c r="G57" s="104" t="s">
+        <v>424</v>
       </c>
       <c r="H57" s="28" t="s">
         <v>10</v>
@@ -4913,9 +4962,9 @@
       <c r="Y57" s="13"/>
     </row>
     <row r="58" spans="1:27" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="108"/>
-      <c r="C58" s="96" t="s">
-        <v>361</v>
+      <c r="A58" s="134"/>
+      <c r="C58" s="145" t="s">
+        <v>357</v>
       </c>
       <c r="D58" s="69" t="s">
         <v>49</v>
@@ -4923,9 +4972,9 @@
       <c r="E58" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G58" s="129"/>
+      <c r="G58" s="105"/>
       <c r="H58" s="23" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="I58" s="69" t="s">
         <v>51</v>
@@ -4950,28 +4999,28 @@
       <c r="Y58" s="13"/>
     </row>
     <row r="59" spans="1:27" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="108"/>
+      <c r="A59" s="134"/>
       <c r="C59" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="D59" s="141" t="s">
+        <v>284</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>457</v>
+      </c>
+      <c r="F59" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="G59" s="105"/>
+      <c r="H59" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="D59" s="93" t="s">
-        <v>287</v>
-      </c>
-      <c r="E59" s="23" t="s">
-        <v>465</v>
-      </c>
-      <c r="F59" s="69" t="s">
-        <v>343</v>
-      </c>
-      <c r="G59" s="129"/>
-      <c r="H59" s="23" t="s">
-        <v>367</v>
-      </c>
       <c r="I59" s="23" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="K59" s="80"/>
       <c r="L59" s="80"/>
@@ -4992,9 +5041,9 @@
       <c r="AA59" s="81"/>
     </row>
     <row r="60" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="108"/>
+      <c r="A60" s="134"/>
       <c r="C60" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D60" s="69" t="s">
         <v>32</v>
@@ -5003,15 +5052,15 @@
       <c r="F60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G60" s="129"/>
+      <c r="G60" s="105"/>
       <c r="H60" s="23" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I60" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="J60" s="93" t="s">
-        <v>528</v>
+      <c r="J60" s="141" t="s">
+        <v>518</v>
       </c>
       <c r="K60" s="80"/>
       <c r="L60" s="80"/>
@@ -5032,25 +5081,25 @@
       <c r="AA60" s="81"/>
     </row>
     <row r="61" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="108"/>
+      <c r="A61" s="134"/>
       <c r="C61" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="D61" s="93" t="s">
+        <v>361</v>
+      </c>
+      <c r="D61" s="141" t="s">
+        <v>285</v>
+      </c>
+      <c r="E61" s="145" t="s">
         <v>288</v>
       </c>
-      <c r="E61" s="96" t="s">
-        <v>291</v>
-      </c>
       <c r="F61" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="G61" s="129"/>
+        <v>289</v>
+      </c>
+      <c r="G61" s="105"/>
       <c r="H61" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="I61" s="93" t="s">
-        <v>294</v>
+        <v>564</v>
+      </c>
+      <c r="I61" s="141" t="s">
+        <v>290</v>
       </c>
       <c r="J61" s="24" t="s">
         <v>53</v>
@@ -5074,28 +5123,28 @@
       <c r="AA61" s="81"/>
     </row>
     <row r="62" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="108"/>
+      <c r="A62" s="134"/>
       <c r="C62" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="D62" s="93" t="s">
-        <v>289</v>
+        <v>442</v>
+      </c>
+      <c r="D62" s="141" t="s">
+        <v>286</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>573</v>
-      </c>
-      <c r="F62" s="89" t="s">
-        <v>534</v>
-      </c>
-      <c r="G62" s="129"/>
+        <v>561</v>
+      </c>
+      <c r="F62" s="88" t="s">
+        <v>524</v>
+      </c>
+      <c r="G62" s="105"/>
       <c r="H62" s="23" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="I62" s="69" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="K62" s="80"/>
       <c r="L62" s="80"/>
@@ -5116,23 +5165,23 @@
       <c r="AA62" s="81"/>
     </row>
     <row r="63" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="108"/>
+      <c r="A63" s="134"/>
       <c r="C63" s="23" t="s">
         <v>240</v>
       </c>
       <c r="D63" s="69" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E63" s="23"/>
       <c r="F63" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="G63" s="129"/>
+      <c r="G63" s="105"/>
       <c r="H63" s="23" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="K63" s="80"/>
       <c r="L63" s="80"/>
@@ -5153,22 +5202,22 @@
       <c r="AA63" s="81"/>
     </row>
     <row r="64" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="108"/>
-      <c r="C64" s="96" t="s">
-        <v>395</v>
+      <c r="A64" s="134"/>
+      <c r="C64" s="145" t="s">
+        <v>391</v>
       </c>
       <c r="D64" s="69" t="s">
-        <v>341</v>
-      </c>
-      <c r="G64" s="129"/>
+        <v>337</v>
+      </c>
+      <c r="G64" s="105"/>
       <c r="H64" s="23" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="J64" s="23" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="K64" s="80"/>
       <c r="L64" s="80"/>
@@ -5189,7 +5238,7 @@
       <c r="AA64" s="81"/>
     </row>
     <row r="65" spans="1:27" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="108"/>
+      <c r="A65" s="134"/>
       <c r="D65" s="23" t="s">
         <v>39</v>
       </c>
@@ -5197,11 +5246,11 @@
         <v>25</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>558</v>
-      </c>
-      <c r="G65" s="129"/>
+        <v>546</v>
+      </c>
+      <c r="G65" s="105"/>
       <c r="H65" s="23" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I65" s="23"/>
       <c r="K65" s="80"/>
@@ -5223,24 +5272,24 @@
       <c r="AA65" s="81"/>
     </row>
     <row r="66" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="108"/>
+      <c r="A66" s="134"/>
       <c r="B66" s="82"/>
-      <c r="C66" s="97" t="s">
-        <v>411</v>
-      </c>
-      <c r="D66" s="93" t="s">
-        <v>572</v>
+      <c r="C66" s="146" t="s">
+        <v>406</v>
+      </c>
+      <c r="D66" s="141" t="s">
+        <v>560</v>
       </c>
       <c r="E66" s="41"/>
       <c r="F66" s="23" t="s">
-        <v>557</v>
-      </c>
-      <c r="G66" s="129"/>
+        <v>545</v>
+      </c>
+      <c r="G66" s="105"/>
       <c r="H66" s="23" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="K66" s="80"/>
       <c r="L66" s="80"/>
@@ -5261,25 +5310,25 @@
       <c r="AA66" s="81"/>
     </row>
     <row r="67" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="108"/>
-      <c r="C67" s="96" t="s">
-        <v>556</v>
+      <c r="A67" s="134"/>
+      <c r="C67" s="145" t="s">
+        <v>544</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="F67" s="23" t="s">
-        <v>559</v>
-      </c>
-      <c r="G67" s="129"/>
+        <v>547</v>
+      </c>
+      <c r="G67" s="105"/>
       <c r="H67" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I67" s="69" t="s">
         <v>45</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="K67" s="80"/>
       <c r="L67" s="80"/>
@@ -5300,25 +5349,25 @@
       <c r="AA67" s="81"/>
     </row>
     <row r="68" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="108"/>
-      <c r="C68" s="91" t="s">
-        <v>538</v>
+      <c r="A68" s="134"/>
+      <c r="C68" s="90" t="s">
+        <v>528</v>
       </c>
       <c r="D68" s="67" t="s">
-        <v>519</v>
-      </c>
-      <c r="F68" s="98" t="s">
-        <v>410</v>
-      </c>
-      <c r="G68" s="129"/>
+        <v>509</v>
+      </c>
+      <c r="F68" s="147" t="s">
+        <v>405</v>
+      </c>
+      <c r="G68" s="105"/>
       <c r="H68" s="23" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>571</v>
-      </c>
-      <c r="J68" s="98" t="s">
-        <v>408</v>
+        <v>559</v>
+      </c>
+      <c r="J68" s="147" t="s">
+        <v>403</v>
       </c>
       <c r="K68" s="80"/>
       <c r="L68" s="80"/>
@@ -5339,15 +5388,15 @@
       <c r="AA68" s="81"/>
     </row>
     <row r="69" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="108"/>
+      <c r="A69" s="134"/>
       <c r="B69" s="83"/>
-      <c r="C69" s="116" t="s">
+      <c r="C69" s="135" t="s">
         <v>203</v>
       </c>
-      <c r="D69" s="117"/>
+      <c r="D69" s="136"/>
       <c r="G69" s="69"/>
       <c r="H69" s="23" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
@@ -5366,22 +5415,22 @@
       <c r="Y69" s="13"/>
     </row>
     <row r="70" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="108"/>
+      <c r="A70" s="134"/>
       <c r="B70" s="83"/>
-      <c r="C70" s="105" t="s">
+      <c r="C70" s="108" t="s">
         <v>191</v>
       </c>
-      <c r="D70" s="106"/>
-      <c r="G70" s="148" t="s">
-        <v>505</v>
+      <c r="D70" s="101"/>
+      <c r="G70" s="111" t="s">
+        <v>496</v>
       </c>
       <c r="H70" s="23" t="s">
-        <v>373</v>
-      </c>
-      <c r="I70" s="105" t="s">
+        <v>369</v>
+      </c>
+      <c r="I70" s="108" t="s">
         <v>192</v>
       </c>
-      <c r="J70" s="106"/>
+      <c r="J70" s="101"/>
       <c r="K70" s="13"/>
       <c r="L70" s="13"/>
       <c r="M70" s="13"/>
@@ -5399,24 +5448,24 @@
       <c r="Y70" s="13"/>
     </row>
     <row r="71" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="108"/>
+      <c r="A71" s="134"/>
       <c r="B71" s="83"/>
-      <c r="C71" s="105" t="s">
+      <c r="C71" s="108" t="s">
         <v>211</v>
       </c>
-      <c r="D71" s="106"/>
-      <c r="E71" s="105" t="s">
-        <v>471</v>
-      </c>
-      <c r="F71" s="106"/>
-      <c r="G71" s="149"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="108" t="s">
+        <v>463</v>
+      </c>
+      <c r="F71" s="101"/>
+      <c r="G71" s="112"/>
       <c r="H71" s="23" t="s">
-        <v>433</v>
-      </c>
-      <c r="I71" s="105" t="s">
+        <v>426</v>
+      </c>
+      <c r="I71" s="108" t="s">
         <v>207</v>
       </c>
-      <c r="J71" s="106"/>
+      <c r="J71" s="101"/>
       <c r="K71" s="13"/>
       <c r="L71" s="13"/>
       <c r="M71" s="13"/>
@@ -5434,26 +5483,26 @@
       <c r="Y71" s="13"/>
     </row>
     <row r="72" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="108"/>
+      <c r="A72" s="134"/>
       <c r="B72" s="83"/>
       <c r="C72" s="109" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="D72" s="110"/>
-      <c r="E72" s="105" t="s">
+      <c r="E72" s="108" t="s">
         <v>228</v>
       </c>
-      <c r="F72" s="106"/>
-      <c r="G72" s="104" t="s">
-        <v>553</v>
+      <c r="F72" s="101"/>
+      <c r="G72" s="95" t="s">
+        <v>541</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="I72" s="105" t="s">
+        <v>384</v>
+      </c>
+      <c r="I72" s="108" t="s">
         <v>214</v>
       </c>
-      <c r="J72" s="106"/>
+      <c r="J72" s="101"/>
       <c r="K72" s="13"/>
       <c r="L72" s="13"/>
       <c r="M72" s="13"/>
@@ -5471,24 +5520,24 @@
       <c r="Y72" s="13"/>
     </row>
     <row r="73" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="108"/>
+      <c r="A73" s="134"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="105" t="s">
+      <c r="C73" s="108" t="s">
         <v>224</v>
       </c>
-      <c r="D73" s="106"/>
-      <c r="E73" s="105" t="s">
-        <v>254</v>
-      </c>
-      <c r="F73" s="106"/>
+      <c r="D73" s="101"/>
+      <c r="E73" s="108" t="s">
+        <v>252</v>
+      </c>
+      <c r="F73" s="101"/>
       <c r="G73" s="69"/>
-      <c r="H73" s="84" t="s">
-        <v>527</v>
-      </c>
-      <c r="I73" s="105" t="s">
-        <v>516</v>
-      </c>
-      <c r="J73" s="106"/>
+      <c r="H73" s="148" t="s">
+        <v>517</v>
+      </c>
+      <c r="I73" s="108" t="s">
+        <v>506</v>
+      </c>
+      <c r="J73" s="101"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -5506,16 +5555,16 @@
       <c r="Y73" s="9"/>
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="108"/>
-      <c r="E74" s="105" t="s">
-        <v>513</v>
-      </c>
-      <c r="F74" s="106"/>
+      <c r="A74" s="134"/>
+      <c r="E74" s="115" t="s">
+        <v>571</v>
+      </c>
+      <c r="F74" s="116"/>
       <c r="G74" s="69"/>
-      <c r="I74" s="105" t="s">
+      <c r="I74" s="108" t="s">
         <v>218</v>
       </c>
-      <c r="J74" s="106"/>
+      <c r="J74" s="101"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -5533,19 +5582,19 @@
       <c r="Y74" s="9"/>
     </row>
     <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="108"/>
+      <c r="A75" s="134"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="105"/>
-      <c r="D75" s="106"/>
-      <c r="E75" s="121" t="s">
+      <c r="C75" s="108"/>
+      <c r="D75" s="101"/>
+      <c r="E75" s="113" t="s">
         <v>249</v>
       </c>
-      <c r="F75" s="122"/>
+      <c r="F75" s="114"/>
       <c r="G75" s="69"/>
-      <c r="I75" s="136" t="s">
-        <v>459</v>
-      </c>
-      <c r="J75" s="106"/>
+      <c r="I75" s="106" t="s">
+        <v>451</v>
+      </c>
+      <c r="J75" s="107"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -5563,17 +5612,17 @@
       <c r="Y75" s="9"/>
     </row>
     <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="108"/>
+      <c r="A76" s="134"/>
       <c r="B76" s="6"/>
       <c r="C76" s="70"/>
       <c r="D76" s="71"/>
-      <c r="E76" s="105" t="s">
-        <v>438</v>
-      </c>
-      <c r="F76" s="106"/>
+      <c r="E76" s="108" t="s">
+        <v>431</v>
+      </c>
+      <c r="F76" s="101"/>
       <c r="G76" s="69"/>
-      <c r="J76" s="92" t="s">
-        <v>464</v>
+      <c r="J76" s="91" t="s">
+        <v>456</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
@@ -5618,27 +5667,27 @@
       <c r="Y77" s="9"/>
     </row>
     <row r="78" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="118" t="s">
+      <c r="A78" s="98" t="s">
         <v>55</v>
       </c>
       <c r="B78" s="12"/>
       <c r="C78" s="15" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D78" s="69" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G78" s="147" t="s">
-        <v>430</v>
+      <c r="G78" s="102" t="s">
+        <v>423</v>
       </c>
       <c r="H78" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="69" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -5659,9 +5708,9 @@
       <c r="AA78" s="9"/>
     </row>
     <row r="79" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="119"/>
-      <c r="C79" s="85" t="s">
-        <v>451</v>
+      <c r="A79" s="99"/>
+      <c r="C79" s="84" t="s">
+        <v>443</v>
       </c>
       <c r="D79" s="69" t="s">
         <v>58</v>
@@ -5670,11 +5719,11 @@
         <v>19</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="G79" s="112"/>
+        <v>342</v>
+      </c>
+      <c r="G79" s="103"/>
       <c r="H79" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I79" s="69" t="s">
         <v>33</v>
@@ -5698,7 +5747,7 @@
       <c r="AA79" s="9"/>
     </row>
     <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="119"/>
+      <c r="A80" s="99"/>
       <c r="C80" s="2" t="s">
         <v>62</v>
       </c>
@@ -5711,9 +5760,9 @@
       <c r="F80" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G80" s="112"/>
+      <c r="G80" s="103"/>
       <c r="H80" s="4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="I80" s="15" t="s">
         <v>59</v>
@@ -5738,25 +5787,25 @@
       <c r="Y80" s="9"/>
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="119"/>
-      <c r="C81" s="93" t="s">
-        <v>291</v>
+      <c r="A81" s="99"/>
+      <c r="C81" s="141" t="s">
+        <v>288</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="G81" s="112"/>
+        <v>293</v>
+      </c>
+      <c r="G81" s="103"/>
       <c r="H81" s="4" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="I81" s="69" t="s">
         <v>49</v>
       </c>
       <c r="J81" s="69" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
@@ -5775,25 +5824,25 @@
       <c r="Y81" s="9"/>
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="119"/>
+      <c r="A82" s="99"/>
       <c r="C82" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D82" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E82" s="96" t="s">
-        <v>255</v>
-      </c>
-      <c r="F82" s="93" t="s">
-        <v>293</v>
-      </c>
-      <c r="G82" s="112"/>
+      <c r="E82" s="145" t="s">
+        <v>253</v>
+      </c>
+      <c r="F82" s="141" t="s">
+        <v>578</v>
+      </c>
+      <c r="G82" s="103"/>
       <c r="H82" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -5811,22 +5860,22 @@
       <c r="Y82" s="9"/>
     </row>
     <row r="83" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="119"/>
-      <c r="D83" s="93" t="s">
-        <v>290</v>
+      <c r="A83" s="99"/>
+      <c r="D83" s="141" t="s">
+        <v>287</v>
       </c>
       <c r="E83" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="G83" s="112"/>
+        <v>295</v>
+      </c>
+      <c r="G83" s="103"/>
       <c r="H83" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="I83" s="93" t="s">
-        <v>288</v>
+        <v>565</v>
+      </c>
+      <c r="I83" s="141" t="s">
+        <v>285</v>
       </c>
       <c r="J83" s="69" t="s">
         <v>20</v>
@@ -5848,28 +5897,28 @@
       <c r="Y83" s="9"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="119"/>
+      <c r="A84" s="99"/>
       <c r="C84" s="4" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="G84" s="112"/>
+        <v>296</v>
+      </c>
+      <c r="G84" s="103"/>
       <c r="H84" s="73" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J84" s="69" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
@@ -5888,28 +5937,28 @@
       <c r="Y84" s="9"/>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="119"/>
+      <c r="A85" s="99"/>
       <c r="C85" s="4" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="G85" s="112"/>
+        <v>297</v>
+      </c>
+      <c r="G85" s="103"/>
       <c r="H85" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
@@ -5928,25 +5977,25 @@
       <c r="Y85" s="9"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="119"/>
+      <c r="A86" s="99"/>
       <c r="C86" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="E86" s="90" t="s">
-        <v>398</v>
+        <v>549</v>
+      </c>
+      <c r="E86" s="149" t="s">
+        <v>572</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="G86" s="112"/>
+        <v>540</v>
+      </c>
+      <c r="G86" s="103"/>
       <c r="H86" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="K86" s="31"/>
       <c r="L86" s="31"/>
@@ -5967,22 +6016,22 @@
       <c r="AA86" s="31"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="119"/>
+      <c r="A87" s="99"/>
       <c r="E87" s="73" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="G87" s="112"/>
+        <v>395</v>
+      </c>
+      <c r="G87" s="103"/>
       <c r="H87" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="L87" s="31"/>
       <c r="M87" s="31"/>
@@ -6002,17 +6051,17 @@
       <c r="AA87" s="31"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="119"/>
+      <c r="A88" s="99"/>
       <c r="C88" s="2"/>
-      <c r="E88" s="90" t="s">
-        <v>535</v>
+      <c r="E88" s="89" t="s">
+        <v>525</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="G88" s="112"/>
+      <c r="G88" s="103"/>
       <c r="H88" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="L88" s="16"/>
       <c r="M88" s="16"/>
@@ -6032,19 +6081,19 @@
       <c r="AA88" s="17"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="119"/>
+      <c r="A89" s="99"/>
       <c r="B89" s="29"/>
       <c r="G89" s="2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="I89" s="73" t="s">
         <v>231</v>
       </c>
       <c r="J89" s="69" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="L89" s="16"/>
       <c r="M89" s="16"/>
@@ -6064,19 +6113,19 @@
       <c r="AA89" s="17"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="119"/>
-      <c r="C90" s="136" t="s">
-        <v>511</v>
-      </c>
-      <c r="D90" s="106"/>
+      <c r="A90" s="99"/>
+      <c r="C90" s="106" t="s">
+        <v>502</v>
+      </c>
+      <c r="D90" s="107"/>
       <c r="G90" s="2" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="I90" s="90" t="s">
-        <v>536</v>
+        <v>382</v>
+      </c>
+      <c r="I90" s="89" t="s">
+        <v>526</v>
       </c>
       <c r="K90" s="16"/>
       <c r="L90" s="16"/>
@@ -6097,16 +6146,16 @@
       <c r="AA90" s="17"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="119"/>
-      <c r="C91" s="136" t="s">
-        <v>252</v>
-      </c>
-      <c r="D91" s="144"/>
+      <c r="A91" s="99"/>
+      <c r="C91" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="D91" s="152"/>
       <c r="H91" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="I91" s="73" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="K91" s="16"/>
       <c r="L91" s="16"/>
@@ -6127,11 +6176,11 @@
       <c r="AA91" s="17"/>
     </row>
     <row r="92" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="119"/>
+      <c r="A92" s="99"/>
       <c r="E92" s="61"/>
       <c r="G92" s="32"/>
       <c r="H92" s="4" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="J92" s="69"/>
       <c r="K92" s="16"/>
@@ -6153,13 +6202,13 @@
       <c r="AA92" s="17"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="119"/>
-      <c r="C93" s="86" t="s">
-        <v>530</v>
+      <c r="A93" s="99"/>
+      <c r="C93" s="85" t="s">
+        <v>520</v>
       </c>
       <c r="G93" s="32"/>
       <c r="H93" s="78" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="J93" s="69"/>
       <c r="K93" s="9"/>
@@ -6179,22 +6228,22 @@
       <c r="Y93" s="9"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="119"/>
+      <c r="A94" s="99"/>
       <c r="B94" s="6"/>
-      <c r="C94" s="105" t="s">
+      <c r="C94" s="108" t="s">
         <v>204</v>
       </c>
-      <c r="D94" s="106"/>
-      <c r="E94" s="105" t="s">
+      <c r="D94" s="101"/>
+      <c r="E94" s="108" t="s">
         <v>216</v>
       </c>
-      <c r="F94" s="106"/>
+      <c r="F94" s="101"/>
       <c r="G94" s="32"/>
       <c r="H94" s="69"/>
-      <c r="I94" s="105" t="s">
+      <c r="I94" s="108" t="s">
         <v>193</v>
       </c>
-      <c r="J94" s="106"/>
+      <c r="J94" s="101"/>
       <c r="K94" s="9"/>
       <c r="L94" s="9"/>
       <c r="M94" s="9"/>
@@ -6212,22 +6261,22 @@
       <c r="Y94" s="9"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="119"/>
+      <c r="A95" s="99"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="105" t="s">
-        <v>469</v>
-      </c>
-      <c r="D95" s="106"/>
-      <c r="E95" s="105" t="s">
+      <c r="C95" s="108" t="s">
+        <v>461</v>
+      </c>
+      <c r="D95" s="101"/>
+      <c r="E95" s="108" t="s">
         <v>225</v>
       </c>
-      <c r="F95" s="106"/>
+      <c r="F95" s="101"/>
       <c r="G95" s="32"/>
       <c r="H95" s="69"/>
-      <c r="I95" s="105" t="s">
+      <c r="I95" s="108" t="s">
         <v>215</v>
       </c>
-      <c r="J95" s="106"/>
+      <c r="J95" s="101"/>
       <c r="K95" s="9"/>
       <c r="L95" s="9"/>
       <c r="M95" s="9"/>
@@ -6245,21 +6294,21 @@
       <c r="Y95" s="9"/>
     </row>
     <row r="96" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="119"/>
+      <c r="A96" s="99"/>
       <c r="B96" s="6"/>
-      <c r="C96" s="105" t="s">
+      <c r="C96" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="D96" s="106"/>
-      <c r="E96" s="113" t="s">
-        <v>565</v>
-      </c>
-      <c r="F96" s="112"/>
+      <c r="D96" s="101"/>
+      <c r="E96" s="126" t="s">
+        <v>553</v>
+      </c>
+      <c r="F96" s="103"/>
       <c r="G96" s="32"/>
-      <c r="H96" s="105" t="s">
-        <v>575</v>
-      </c>
-      <c r="I96" s="106"/>
+      <c r="H96" s="108" t="s">
+        <v>563</v>
+      </c>
+      <c r="I96" s="101"/>
       <c r="J96" s="61"/>
       <c r="K96" s="9"/>
       <c r="L96" s="9"/>
@@ -6278,22 +6327,22 @@
       <c r="Y96" s="9"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="119"/>
+      <c r="A97" s="99"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="105" t="s">
-        <v>514</v>
-      </c>
-      <c r="D97" s="106"/>
-      <c r="E97" s="113" t="s">
-        <v>564</v>
-      </c>
-      <c r="F97" s="112"/>
+      <c r="C97" s="108" t="s">
+        <v>504</v>
+      </c>
+      <c r="D97" s="101"/>
+      <c r="E97" s="126" t="s">
+        <v>552</v>
+      </c>
+      <c r="F97" s="103"/>
       <c r="G97" s="32"/>
       <c r="H97" s="69"/>
-      <c r="I97" s="136" t="s">
-        <v>545</v>
-      </c>
-      <c r="J97" s="106"/>
+      <c r="I97" s="106" t="s">
+        <v>535</v>
+      </c>
+      <c r="J97" s="107"/>
       <c r="K97" s="9"/>
       <c r="L97" s="9"/>
       <c r="M97" s="9"/>
@@ -6311,20 +6360,20 @@
       <c r="Y97" s="9"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="119"/>
+      <c r="A98" s="99"/>
       <c r="B98" s="6"/>
-      <c r="C98" s="105" t="s">
+      <c r="C98" s="108" t="s">
         <v>223</v>
       </c>
-      <c r="D98" s="106"/>
-      <c r="E98" s="113" t="s">
+      <c r="D98" s="101"/>
+      <c r="E98" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="F98" s="112"/>
+      <c r="F98" s="103"/>
       <c r="G98" s="32"/>
       <c r="H98" s="75"/>
-      <c r="I98" s="131"/>
-      <c r="J98" s="132"/>
+      <c r="I98" s="122"/>
+      <c r="J98" s="123"/>
       <c r="K98" s="9"/>
       <c r="L98" s="9"/>
       <c r="M98" s="9"/>
@@ -6342,16 +6391,16 @@
       <c r="Y98" s="9"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="119"/>
+      <c r="A99" s="99"/>
       <c r="B99" s="6"/>
-      <c r="C99" s="121" t="s">
+      <c r="C99" s="113" t="s">
         <v>250</v>
       </c>
-      <c r="D99" s="122"/>
-      <c r="E99" s="121" t="s">
-        <v>412</v>
-      </c>
-      <c r="F99" s="122"/>
+      <c r="D99" s="114"/>
+      <c r="E99" s="113" t="s">
+        <v>407</v>
+      </c>
+      <c r="F99" s="114"/>
       <c r="G99" s="32"/>
       <c r="H99" s="75"/>
       <c r="J99" s="75"/>
@@ -6372,14 +6421,14 @@
       <c r="Y99" s="9"/>
     </row>
     <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="119"/>
+      <c r="A100" s="99"/>
       <c r="B100" s="6"/>
       <c r="C100" s="70"/>
       <c r="D100" s="71"/>
-      <c r="E100" s="105" t="s">
-        <v>494</v>
-      </c>
-      <c r="F100" s="106"/>
+      <c r="E100" s="108" t="s">
+        <v>485</v>
+      </c>
+      <c r="F100" s="101"/>
       <c r="G100" s="32"/>
       <c r="H100" s="75"/>
       <c r="I100" s="75"/>
@@ -6401,14 +6450,14 @@
       <c r="Y100" s="9"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="119"/>
+      <c r="A101" s="99"/>
       <c r="B101" s="6"/>
       <c r="C101" s="70"/>
       <c r="D101" s="71"/>
-      <c r="E101" s="134" t="s">
+      <c r="E101" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="F101" s="134"/>
+      <c r="F101" s="117"/>
       <c r="G101" s="32"/>
       <c r="H101" s="75"/>
       <c r="J101" s="75"/>
@@ -6429,12 +6478,12 @@
       <c r="Y101" s="9"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="120"/>
+      <c r="A102" s="100"/>
       <c r="B102" s="6"/>
       <c r="C102" s="70"/>
       <c r="D102" s="71"/>
-      <c r="E102" s="105"/>
-      <c r="F102" s="106"/>
+      <c r="E102" s="108"/>
+      <c r="F102" s="101"/>
       <c r="G102" s="32"/>
       <c r="H102" s="75"/>
       <c r="J102" s="75"/>
@@ -6507,25 +6556,25 @@
       <c r="X104" s="9"/>
       <c r="Y104" s="9"/>
     </row>
-    <row r="105" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="115" t="s">
+    <row r="105" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="131" t="s">
         <v>65</v>
       </c>
       <c r="B105" s="12"/>
       <c r="C105" s="69" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D105" s="69" t="s">
         <v>17</v>
       </c>
       <c r="E105" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="F105" s="89" t="s">
-        <v>534</v>
-      </c>
-      <c r="G105" s="139" t="s">
-        <v>548</v>
+        <v>351</v>
+      </c>
+      <c r="F105" s="88" t="s">
+        <v>524</v>
+      </c>
+      <c r="G105" s="155" t="s">
+        <v>537</v>
       </c>
       <c r="H105" s="34" t="s">
         <v>66</v>
@@ -6552,10 +6601,10 @@
       <c r="X105" s="9"/>
       <c r="Y105" s="9"/>
     </row>
-    <row r="106" spans="1:27" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="112"/>
+    <row r="106" spans="1:27" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="103"/>
       <c r="C106" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D106" s="69" t="s">
         <v>19</v>
@@ -6566,10 +6615,12 @@
       <c r="F106" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G106" s="140"/>
+      <c r="G106" s="156" t="s">
+        <v>576</v>
+      </c>
       <c r="H106" s="34"/>
       <c r="I106" s="23" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="J106" s="69" t="s">
         <v>68</v>
@@ -6591,24 +6642,24 @@
       <c r="Y106" s="9"/>
     </row>
     <row r="107" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="112"/>
+      <c r="A107" s="103"/>
       <c r="C107" s="69" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D107" s="69" t="s">
         <v>49</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F107" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G107" s="104" t="s">
-        <v>554</v>
+      <c r="G107" s="97" t="s">
+        <v>542</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="I107" s="15" t="s">
         <v>35</v>
@@ -6633,27 +6684,27 @@
       <c r="Y107" s="9"/>
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="112"/>
+      <c r="A108" s="103"/>
       <c r="C108" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G108" s="128" t="s">
-        <v>431</v>
+      <c r="G108" s="104" t="s">
+        <v>424</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="I108" s="101" t="s">
-        <v>541</v>
+        <v>409</v>
+      </c>
+      <c r="I108" s="92" t="s">
+        <v>531</v>
       </c>
       <c r="J108" s="69" t="s">
         <v>38</v>
@@ -6675,22 +6726,22 @@
       <c r="Y108" s="9"/>
     </row>
     <row r="109" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="112"/>
-      <c r="D109" s="93" t="s">
-        <v>307</v>
+      <c r="A109" s="103"/>
+      <c r="D109" s="141" t="s">
+        <v>303</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="G109" s="129"/>
+        <v>447</v>
+      </c>
+      <c r="G109" s="105"/>
       <c r="H109" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="K109" s="9"/>
       <c r="L109" s="9"/>
@@ -6709,17 +6760,17 @@
       <c r="Y109" s="9"/>
     </row>
     <row r="110" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="112"/>
-      <c r="D110" s="93" t="s">
-        <v>353</v>
+      <c r="A110" s="103"/>
+      <c r="D110" s="141" t="s">
+        <v>349</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F110" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G110" s="129"/>
+      <c r="G110" s="105"/>
       <c r="I110" s="69"/>
       <c r="J110" s="69"/>
       <c r="K110" s="16"/>
@@ -6741,14 +6792,14 @@
       <c r="AA110" s="17"/>
     </row>
     <row r="111" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="112"/>
-      <c r="D111" s="93" t="s">
-        <v>454</v>
+      <c r="A111" s="103"/>
+      <c r="D111" s="141" t="s">
+        <v>446</v>
       </c>
       <c r="F111" s="69" t="s">
-        <v>551</v>
-      </c>
-      <c r="G111" s="129"/>
+        <v>539</v>
+      </c>
+      <c r="G111" s="105"/>
       <c r="H111" s="36"/>
       <c r="I111" s="4" t="s">
         <v>233</v>
@@ -6773,11 +6824,11 @@
       <c r="AA111" s="17"/>
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="112"/>
+      <c r="A112" s="103"/>
       <c r="D112" s="23" t="s">
-        <v>354</v>
-      </c>
-      <c r="G112" s="129"/>
+        <v>350</v>
+      </c>
+      <c r="G112" s="105"/>
       <c r="H112" s="36"/>
       <c r="J112" s="2"/>
       <c r="K112" s="16"/>
@@ -6799,12 +6850,12 @@
       <c r="AA112" s="17"/>
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="112"/>
+      <c r="A113" s="103"/>
       <c r="C113" s="69"/>
       <c r="E113" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="G113" s="129"/>
+        <v>399</v>
+      </c>
+      <c r="G113" s="105"/>
       <c r="H113" s="34"/>
       <c r="J113" s="2"/>
       <c r="K113" s="16"/>
@@ -6826,11 +6877,11 @@
       <c r="AA113" s="17"/>
     </row>
     <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="112"/>
+      <c r="A114" s="103"/>
       <c r="E114" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="G114" s="129"/>
+        <v>550</v>
+      </c>
+      <c r="G114" s="105"/>
       <c r="H114" s="36"/>
       <c r="K114" s="16"/>
       <c r="L114" s="16"/>
@@ -6851,15 +6902,15 @@
       <c r="AA114" s="17"/>
     </row>
     <row r="115" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="112"/>
+      <c r="A115" s="103"/>
       <c r="D115" s="69"/>
       <c r="E115" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="G115" s="129"/>
+        <v>439</v>
+      </c>
+      <c r="G115" s="105"/>
       <c r="H115" s="36"/>
       <c r="J115" s="69"/>
       <c r="K115" s="16"/>
@@ -6881,11 +6932,11 @@
       <c r="AA115" s="17"/>
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="112"/>
+      <c r="A116" s="103"/>
       <c r="E116" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="G116" s="129"/>
+        <v>551</v>
+      </c>
+      <c r="G116" s="105"/>
       <c r="H116" s="69" t="s">
         <v>32</v>
       </c>
@@ -6908,22 +6959,22 @@
       <c r="AA116" s="17"/>
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="112"/>
+      <c r="A117" s="103"/>
       <c r="B117" s="6"/>
-      <c r="C117" s="105"/>
-      <c r="D117" s="106"/>
-      <c r="E117" s="105" t="s">
+      <c r="C117" s="108"/>
+      <c r="D117" s="101"/>
+      <c r="E117" s="108" t="s">
         <v>208</v>
       </c>
-      <c r="F117" s="106"/>
-      <c r="G117" s="129"/>
+      <c r="F117" s="101"/>
+      <c r="G117" s="105"/>
       <c r="H117" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I117" s="105" t="s">
+      <c r="I117" s="108" t="s">
         <v>194</v>
       </c>
-      <c r="J117" s="106"/>
+      <c r="J117" s="101"/>
       <c r="K117" s="16"/>
       <c r="L117" s="16"/>
       <c r="M117" s="16"/>
@@ -6943,15 +6994,15 @@
       <c r="AA117" s="17"/>
     </row>
     <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="112"/>
-      <c r="C118" s="86" t="s">
-        <v>531</v>
-      </c>
-      <c r="G118" s="129"/>
-      <c r="H118" s="141" t="s">
-        <v>467</v>
-      </c>
-      <c r="I118" s="142"/>
+      <c r="A118" s="103"/>
+      <c r="C118" s="85" t="s">
+        <v>521</v>
+      </c>
+      <c r="G118" s="105"/>
+      <c r="H118" s="115" t="s">
+        <v>459</v>
+      </c>
+      <c r="I118" s="116"/>
       <c r="K118" s="16"/>
       <c r="L118" s="16"/>
       <c r="M118" s="16"/>
@@ -6971,21 +7022,21 @@
       <c r="AA118" s="17"/>
     </row>
     <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="112"/>
+      <c r="A119" s="103"/>
       <c r="B119" s="6"/>
-      <c r="C119" s="105" t="s">
-        <v>466</v>
-      </c>
-      <c r="D119" s="106"/>
-      <c r="E119" s="105" t="s">
+      <c r="C119" s="108" t="s">
+        <v>458</v>
+      </c>
+      <c r="D119" s="101"/>
+      <c r="E119" s="108" t="s">
         <v>222</v>
       </c>
-      <c r="F119" s="106"/>
-      <c r="G119" s="129"/>
-      <c r="I119" s="105" t="s">
+      <c r="F119" s="101"/>
+      <c r="G119" s="105"/>
+      <c r="I119" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="J119" s="106"/>
+      <c r="J119" s="101"/>
       <c r="K119" s="16"/>
       <c r="L119" s="16"/>
       <c r="M119" s="16"/>
@@ -7005,22 +7056,22 @@
       <c r="AA119" s="17"/>
     </row>
     <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="112"/>
+      <c r="A120" s="103"/>
       <c r="B120" s="6"/>
-      <c r="C120" s="105" t="s">
-        <v>472</v>
-      </c>
-      <c r="D120" s="106"/>
-      <c r="E120" s="121" t="s">
-        <v>419</v>
-      </c>
-      <c r="F120" s="122"/>
+      <c r="C120" s="108" t="s">
+        <v>464</v>
+      </c>
+      <c r="D120" s="101"/>
+      <c r="E120" s="113" t="s">
+        <v>414</v>
+      </c>
+      <c r="F120" s="114"/>
       <c r="G120" s="35"/>
       <c r="H120" s="36"/>
-      <c r="I120" s="105" t="s">
+      <c r="I120" s="108" t="s">
         <v>212</v>
       </c>
-      <c r="J120" s="106"/>
+      <c r="J120" s="101"/>
       <c r="K120" s="16"/>
       <c r="L120" s="16"/>
       <c r="M120" s="16"/>
@@ -7040,22 +7091,22 @@
       <c r="AA120" s="17"/>
     </row>
     <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="112"/>
+      <c r="A121" s="103"/>
       <c r="B121" s="6"/>
-      <c r="C121" s="105" t="s">
-        <v>468</v>
-      </c>
-      <c r="D121" s="106"/>
-      <c r="E121" s="136" t="s">
-        <v>547</v>
-      </c>
-      <c r="F121" s="106"/>
+      <c r="C121" s="108" t="s">
+        <v>460</v>
+      </c>
+      <c r="D121" s="101"/>
+      <c r="E121" s="106" t="s">
+        <v>536</v>
+      </c>
+      <c r="F121" s="107"/>
       <c r="G121" s="35"/>
       <c r="H121" s="36"/>
-      <c r="I121" s="105" t="s">
+      <c r="I121" s="108" t="s">
         <v>219</v>
       </c>
-      <c r="J121" s="106"/>
+      <c r="J121" s="101"/>
       <c r="K121" s="16"/>
       <c r="L121" s="16"/>
       <c r="M121" s="16"/>
@@ -7075,16 +7126,16 @@
       <c r="AA121" s="17"/>
     </row>
     <row r="122" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="112"/>
+      <c r="A122" s="103"/>
       <c r="B122" s="6"/>
-      <c r="C122" s="105" t="s">
+      <c r="C122" s="108" t="s">
         <v>202</v>
       </c>
-      <c r="D122" s="106"/>
-      <c r="E122" s="105" t="s">
-        <v>439</v>
-      </c>
-      <c r="F122" s="106"/>
+      <c r="D122" s="101"/>
+      <c r="E122" s="108" t="s">
+        <v>432</v>
+      </c>
+      <c r="F122" s="101"/>
       <c r="G122" s="35"/>
       <c r="H122" s="36"/>
       <c r="K122" s="16"/>
@@ -7106,22 +7157,20 @@
       <c r="AA122" s="17"/>
     </row>
     <row r="123" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="112"/>
+      <c r="A123" s="103"/>
       <c r="B123" s="6"/>
-      <c r="C123" s="105" t="s">
+      <c r="C123" s="108" t="s">
         <v>221</v>
       </c>
-      <c r="D123" s="106"/>
-      <c r="E123" s="134" t="s">
-        <v>475</v>
-      </c>
-      <c r="F123" s="112"/>
+      <c r="D123" s="101"/>
+      <c r="E123" s="117" t="s">
+        <v>466</v>
+      </c>
+      <c r="F123" s="103"/>
       <c r="G123" s="35"/>
       <c r="H123" s="36"/>
-      <c r="I123" s="136" t="s">
-        <v>474</v>
-      </c>
-      <c r="J123" s="106"/>
+      <c r="I123" s="106"/>
+      <c r="J123" s="107"/>
       <c r="K123" s="16"/>
       <c r="L123" s="16"/>
       <c r="M123" s="16"/>
@@ -7141,20 +7190,20 @@
       <c r="AA123" s="17"/>
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="112"/>
+      <c r="A124" s="103"/>
       <c r="B124" s="6"/>
-      <c r="C124" s="136" t="s">
-        <v>546</v>
-      </c>
-      <c r="D124" s="106"/>
+      <c r="C124" s="139" t="s">
+        <v>573</v>
+      </c>
+      <c r="D124" s="119"/>
       <c r="G124" s="35"/>
-      <c r="H124" s="90" t="s">
-        <v>434</v>
-      </c>
-      <c r="I124" s="136" t="s">
-        <v>447</v>
-      </c>
-      <c r="J124" s="106"/>
+      <c r="H124" s="144" t="s">
+        <v>427</v>
+      </c>
+      <c r="I124" s="139" t="s">
+        <v>574</v>
+      </c>
+      <c r="J124" s="116"/>
       <c r="K124" s="16"/>
       <c r="L124" s="16"/>
       <c r="M124" s="16"/>
@@ -7174,16 +7223,16 @@
       <c r="AA124" s="17"/>
     </row>
     <row r="125" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="112"/>
+      <c r="A125" s="103"/>
       <c r="B125" s="6"/>
-      <c r="C125" s="105"/>
-      <c r="D125" s="106"/>
+      <c r="C125" s="108"/>
+      <c r="D125" s="101"/>
       <c r="G125" s="35"/>
       <c r="H125" s="73"/>
-      <c r="I125" s="143" t="s">
-        <v>495</v>
-      </c>
-      <c r="J125" s="132"/>
+      <c r="I125" s="140" t="s">
+        <v>486</v>
+      </c>
+      <c r="J125" s="123"/>
       <c r="K125" s="16"/>
       <c r="L125" s="16"/>
       <c r="M125" s="16"/>
@@ -7203,10 +7252,10 @@
       <c r="AA125" s="17"/>
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="112"/>
+      <c r="A126" s="103"/>
       <c r="B126" s="6"/>
-      <c r="C126" s="105"/>
-      <c r="D126" s="106"/>
+      <c r="C126" s="108"/>
+      <c r="D126" s="101"/>
       <c r="G126" s="35"/>
       <c r="H126" s="36"/>
       <c r="K126" s="16"/>
@@ -7228,7 +7277,7 @@
       <c r="AA126" s="17"/>
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="112"/>
+      <c r="A127" s="103"/>
       <c r="B127" s="6"/>
       <c r="C127" s="70"/>
       <c r="D127" s="71"/>
@@ -7306,12 +7355,12 @@
       <c r="Y129" s="9"/>
     </row>
     <row r="130" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="118" t="s">
+      <c r="A130" s="98" t="s">
         <v>73</v>
       </c>
       <c r="B130" s="74"/>
       <c r="C130" s="23" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>74</v>
@@ -7343,9 +7392,9 @@
       <c r="Y130" s="9"/>
     </row>
     <row r="131" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="119"/>
+      <c r="A131" s="99"/>
       <c r="C131" s="23" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>77</v>
@@ -7354,8 +7403,8 @@
         <v>67</v>
       </c>
       <c r="H131" s="11"/>
-      <c r="I131" s="135"/>
-      <c r="J131" s="112"/>
+      <c r="I131" s="127"/>
+      <c r="J131" s="103"/>
       <c r="K131" s="9"/>
       <c r="L131" s="9"/>
       <c r="M131" s="9"/>
@@ -7373,15 +7422,15 @@
       <c r="Y131" s="9"/>
     </row>
     <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="119"/>
+      <c r="A132" s="99"/>
       <c r="C132" s="23" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D132" s="79" t="s">
-        <v>542</v>
-      </c>
-      <c r="F132" s="89" t="s">
-        <v>533</v>
+        <v>532</v>
+      </c>
+      <c r="F132" s="88" t="s">
+        <v>523</v>
       </c>
       <c r="H132" s="11"/>
       <c r="I132" s="41"/>
@@ -7403,15 +7452,15 @@
       <c r="Y132" s="9"/>
     </row>
     <row r="133" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="119"/>
+      <c r="A133" s="99"/>
       <c r="C133" s="23" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D133" s="69" t="s">
         <v>21</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H133" s="11"/>
       <c r="I133" s="11"/>
@@ -7433,12 +7482,12 @@
       <c r="Y133" s="9"/>
     </row>
     <row r="134" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="119"/>
+      <c r="A134" s="99"/>
       <c r="C134" s="15" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>64</v>
@@ -7463,15 +7512,15 @@
       <c r="Y134" s="9"/>
     </row>
     <row r="135" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="119"/>
+      <c r="A135" s="99"/>
       <c r="C135" s="23" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="I135" s="42"/>
       <c r="J135" s="75"/>
@@ -7492,15 +7541,15 @@
       <c r="Y135" s="9"/>
     </row>
     <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="119"/>
+      <c r="A136" s="99"/>
       <c r="C136" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E136" s="93" t="s">
-        <v>487</v>
+        <v>313</v>
+      </c>
+      <c r="E136" s="141" t="s">
+        <v>478</v>
       </c>
       <c r="G136" s="2"/>
       <c r="I136" s="43"/>
@@ -7522,15 +7571,15 @@
       <c r="Y136" s="9"/>
     </row>
     <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="119"/>
-      <c r="C137" s="111" t="s">
-        <v>555</v>
+      <c r="A137" s="99"/>
+      <c r="C137" s="124" t="s">
+        <v>543</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E137" s="94" t="s">
-        <v>406</v>
+        <v>314</v>
+      </c>
+      <c r="E137" s="142" t="s">
+        <v>401</v>
       </c>
       <c r="G137" s="2"/>
       <c r="I137" s="43"/>
@@ -7552,15 +7601,15 @@
       <c r="Y137" s="9"/>
     </row>
     <row r="138" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="119"/>
-      <c r="C138" s="112"/>
+      <c r="A138" s="99"/>
+      <c r="C138" s="103"/>
       <c r="D138" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E138" s="105" t="s">
+        <v>326</v>
+      </c>
+      <c r="E138" s="108" t="s">
         <v>201</v>
       </c>
-      <c r="F138" s="106"/>
+      <c r="F138" s="101"/>
       <c r="G138" s="2"/>
       <c r="H138" s="43"/>
       <c r="I138" s="43"/>
@@ -7582,14 +7631,14 @@
       <c r="Y138" s="9"/>
     </row>
     <row r="139" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="119"/>
+      <c r="A139" s="99"/>
       <c r="C139" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="F139" s="113" t="s">
-        <v>501</v>
-      </c>
-      <c r="G139" s="112"/>
+      <c r="F139" s="126" t="s">
+        <v>492</v>
+      </c>
+      <c r="G139" s="103"/>
       <c r="H139" s="43"/>
       <c r="I139" s="43"/>
       <c r="J139" s="11"/>
@@ -7610,14 +7659,14 @@
       <c r="Y139" s="9"/>
     </row>
     <row r="140" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="119"/>
+      <c r="A140" s="99"/>
       <c r="C140" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="F140" s="114" t="s">
+      <c r="F140" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="G140" s="112"/>
+      <c r="G140" s="103"/>
       <c r="H140" s="43"/>
       <c r="I140" s="43"/>
       <c r="J140" s="11"/>
@@ -7638,15 +7687,15 @@
       <c r="Y140" s="9"/>
     </row>
     <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="119"/>
-      <c r="C141" s="99" t="s">
-        <v>409</v>
+      <c r="A141" s="99"/>
+      <c r="C141" s="150" t="s">
+        <v>404</v>
       </c>
       <c r="E141" s="61"/>
-      <c r="F141" s="114" t="s">
+      <c r="F141" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="G141" s="112"/>
+      <c r="G141" s="103"/>
       <c r="H141" s="43"/>
       <c r="I141" s="43"/>
       <c r="J141" s="11"/>
@@ -7667,9 +7716,9 @@
       <c r="Y141" s="9"/>
     </row>
     <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="119"/>
-      <c r="E142" s="86" t="s">
-        <v>529</v>
+      <c r="A142" s="99"/>
+      <c r="E142" s="85" t="s">
+        <v>519</v>
       </c>
       <c r="G142" s="35"/>
       <c r="H142" s="43"/>
@@ -7692,12 +7741,12 @@
       <c r="Y142" s="9"/>
     </row>
     <row r="143" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="119"/>
+      <c r="A143" s="99"/>
       <c r="C143" s="2"/>
-      <c r="D143" s="105" t="s">
+      <c r="D143" s="108" t="s">
         <v>209</v>
       </c>
-      <c r="E143" s="106"/>
+      <c r="E143" s="101"/>
       <c r="H143" s="43"/>
       <c r="I143" s="43"/>
       <c r="J143" s="11"/>
@@ -7718,16 +7767,16 @@
       <c r="Y143" s="9"/>
     </row>
     <row r="144" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="119"/>
+      <c r="A144" s="99"/>
       <c r="C144" s="2"/>
-      <c r="D144" s="105" t="s">
+      <c r="D144" s="108" t="s">
         <v>196</v>
       </c>
-      <c r="E144" s="106"/>
-      <c r="F144" s="121" t="s">
+      <c r="E144" s="101"/>
+      <c r="F144" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="G144" s="122"/>
+      <c r="G144" s="114"/>
       <c r="H144" s="43"/>
       <c r="I144" s="43"/>
       <c r="J144" s="11"/>
@@ -7748,16 +7797,16 @@
       <c r="Y144" s="9"/>
     </row>
     <row r="145" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="119"/>
+      <c r="A145" s="99"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="137" t="s">
+      <c r="D145" s="120" t="s">
         <v>197</v>
       </c>
-      <c r="E145" s="138"/>
-      <c r="F145" s="121" t="s">
-        <v>422</v>
-      </c>
-      <c r="G145" s="122"/>
+      <c r="E145" s="121"/>
+      <c r="F145" s="113" t="s">
+        <v>417</v>
+      </c>
+      <c r="G145" s="114"/>
       <c r="H145" s="43"/>
       <c r="I145" s="43"/>
       <c r="J145" s="11"/>
@@ -7778,16 +7827,16 @@
       <c r="Y145" s="9"/>
     </row>
     <row r="146" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="119"/>
+      <c r="A146" s="99"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="105" t="s">
+      <c r="D146" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="E146" s="106"/>
-      <c r="F146" s="123" t="s">
-        <v>497</v>
-      </c>
-      <c r="G146" s="124"/>
+      <c r="E146" s="101"/>
+      <c r="F146" s="137" t="s">
+        <v>488</v>
+      </c>
+      <c r="G146" s="138"/>
       <c r="H146" s="43"/>
       <c r="I146" s="43"/>
       <c r="J146" s="11"/>
@@ -7808,12 +7857,12 @@
       <c r="Y146" s="9"/>
     </row>
     <row r="147" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="119"/>
+      <c r="A147" s="99"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="105" t="s">
+      <c r="D147" s="108" t="s">
         <v>220</v>
       </c>
-      <c r="E147" s="106"/>
+      <c r="E147" s="101"/>
       <c r="H147" s="43"/>
       <c r="I147" s="43"/>
       <c r="J147" s="11"/>
@@ -7834,12 +7883,12 @@
       <c r="Y147" s="9"/>
     </row>
     <row r="148" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="119"/>
+      <c r="A148" s="99"/>
       <c r="C148" s="2"/>
-      <c r="D148" s="109" t="s">
-        <v>496</v>
-      </c>
-      <c r="E148" s="110"/>
+      <c r="D148" s="106" t="s">
+        <v>487</v>
+      </c>
+      <c r="E148" s="107"/>
       <c r="H148" s="43"/>
       <c r="I148" s="43"/>
       <c r="J148" s="11"/>
@@ -7860,12 +7909,12 @@
       <c r="Y148" s="9"/>
     </row>
     <row r="149" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="119"/>
+      <c r="A149" s="99"/>
       <c r="C149" s="2"/>
-      <c r="D149" s="113" t="s">
-        <v>567</v>
-      </c>
-      <c r="E149" s="112"/>
+      <c r="D149" s="126" t="s">
+        <v>555</v>
+      </c>
+      <c r="E149" s="103"/>
       <c r="F149" s="2"/>
       <c r="G149" s="35"/>
       <c r="H149" s="11"/>
@@ -7888,12 +7937,12 @@
       <c r="Y149" s="9"/>
     </row>
     <row r="150" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="119"/>
+      <c r="A150" s="99"/>
       <c r="C150" s="2"/>
-      <c r="D150" s="113" t="s">
-        <v>566</v>
-      </c>
-      <c r="E150" s="112"/>
+      <c r="D150" s="126" t="s">
+        <v>554</v>
+      </c>
+      <c r="E150" s="103"/>
       <c r="F150" s="2"/>
       <c r="G150" s="32"/>
       <c r="H150" s="11"/>
@@ -7916,12 +7965,12 @@
       <c r="Y150" s="9"/>
     </row>
     <row r="151" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="119"/>
+      <c r="A151" s="99"/>
       <c r="C151" s="2"/>
-      <c r="D151" s="113" t="s">
+      <c r="D151" s="126" t="s">
         <v>80</v>
       </c>
-      <c r="E151" s="112"/>
+      <c r="E151" s="103"/>
       <c r="F151" s="2"/>
       <c r="G151" s="32"/>
       <c r="H151" s="11"/>
@@ -7944,12 +7993,12 @@
       <c r="Y151" s="9"/>
     </row>
     <row r="152" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="120"/>
+      <c r="A152" s="100"/>
       <c r="C152" s="2"/>
-      <c r="E152" s="105" t="s">
-        <v>523</v>
-      </c>
-      <c r="F152" s="106"/>
+      <c r="E152" s="108" t="s">
+        <v>513</v>
+      </c>
+      <c r="F152" s="101"/>
       <c r="G152" s="32"/>
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
@@ -8136,10 +8185,10 @@
     <row r="158" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="9"/>
       <c r="B158" s="9"/>
-      <c r="C158" s="100" t="s">
+      <c r="C158" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="D158" s="100" t="s">
+      <c r="D158" s="151" t="s">
         <v>89</v>
       </c>
       <c r="E158" s="53" t="s">
@@ -8228,7 +8277,7 @@
       <c r="H160" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="I160" s="88" t="s">
+      <c r="I160" s="87" t="s">
         <v>140</v>
       </c>
       <c r="K160" s="9"/>
@@ -8443,7 +8492,7 @@
         <v>148</v>
       </c>
       <c r="H166" s="59" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="I166" s="59" t="s">
         <v>149</v>
@@ -8739,7 +8788,7 @@
       <c r="D174" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E174" s="88" t="s">
+      <c r="E174" s="87" t="s">
         <v>128</v>
       </c>
       <c r="F174" s="13"/>
@@ -8783,10 +8832,10 @@
       </c>
       <c r="F175" s="13"/>
       <c r="G175" s="58" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="H175" s="58" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="I175" s="58" t="s">
         <v>173</v>
@@ -8816,10 +8865,10 @@
       <c r="E176" s="13"/>
       <c r="F176" s="13"/>
       <c r="G176" s="58" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="H176" s="58" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I176" s="58" t="s">
         <v>174</v>
@@ -9258,7 +9307,7 @@
       <c r="C192" s="58"/>
       <c r="D192" s="58"/>
       <c r="E192" s="58"/>
-      <c r="F192" s="133"/>
+      <c r="F192" s="125"/>
       <c r="J192" s="13"/>
       <c r="K192" s="9"/>
       <c r="L192" s="9"/>
@@ -9282,7 +9331,7 @@
       <c r="C193" s="58"/>
       <c r="D193" s="58"/>
       <c r="E193" s="58"/>
-      <c r="F193" s="112"/>
+      <c r="F193" s="103"/>
       <c r="J193" s="13"/>
       <c r="K193" s="9"/>
       <c r="L193" s="9"/>
@@ -9333,7 +9382,7 @@
       <c r="C195" s="58"/>
       <c r="D195" s="58"/>
       <c r="E195" s="58"/>
-      <c r="F195" s="133"/>
+      <c r="F195" s="125"/>
       <c r="G195" s="9"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
@@ -9360,7 +9409,7 @@
       <c r="C196" s="58"/>
       <c r="D196" s="58"/>
       <c r="E196" s="58"/>
-      <c r="F196" s="112"/>
+      <c r="F196" s="103"/>
       <c r="G196" s="9"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
@@ -12933,7 +12982,114 @@
     <row r="1059" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1060" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="132">
+  <mergeCells count="131">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="A54:A76"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="F140:G140"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="A105:A127"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="A78:A102"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="F145:G145"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A3:A28"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G5:G28"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="A30:A52"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="F192:F193"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="F139:G139"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="I131:J131"/>
+    <mergeCell ref="I120:J120"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="I117:J117"/>
+    <mergeCell ref="I119:J119"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="I124:J124"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G108:G119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="E138:F138"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="I97:J97"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="I125:J125"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
     <mergeCell ref="A130:A152"/>
     <mergeCell ref="I75:J75"/>
     <mergeCell ref="G78:G88"/>
@@ -12958,114 +13114,6 @@
     <mergeCell ref="I74:J74"/>
     <mergeCell ref="I73:J73"/>
     <mergeCell ref="E76:F76"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="F141:G141"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="G108:G119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="E138:F138"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="G105:G106"/>
-    <mergeCell ref="I97:J97"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="H118:I118"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="I125:J125"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="F192:F193"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="F139:G139"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="I131:J131"/>
-    <mergeCell ref="I120:J120"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="I117:J117"/>
-    <mergeCell ref="I119:J119"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="I124:J124"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:A28"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G5:G28"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A30:A52"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="E152:F152"/>
-    <mergeCell ref="A54:A76"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="F140:G140"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="A105:A127"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="A78:A102"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="F145:G145"/>
-    <mergeCell ref="F146:G146"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: update tt btech 62 sem2,4
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 62 (btech-62)/4/1.xlsx
+++ b/raw/time_tables/B.Tech 62 (btech-62)/4/1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\TT_27 jan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\TT_27 jan\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DFC6E4-FBED-42A9-A258-2FE1B9972DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13067FA-8708-4617-90FC-E59BC59324A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1360,9 +1360,6 @@
     <t>LB(CS212)-G4/SHO</t>
   </si>
   <si>
-    <t>PB(25B16CS212)-CL02,03,04/APJ,SHO</t>
-  </si>
-  <si>
     <t>LB(CS243)-G6/NET</t>
   </si>
   <si>
@@ -1568,9 +1565,6 @@
   </si>
   <si>
     <t>PG1,G2(CS221)-CL10,11/VRN,SHV,DL,RJM</t>
-  </si>
-  <si>
-    <t>PB8(CS221)-CL02/VRN,TKT</t>
   </si>
   <si>
     <t>PB(25B16CS213)-CL17,18/HN,VIK</t>
@@ -1926,9 +1920,6 @@
     <t>PB11,12(CS221)-CL21, CL22 /TKT,VRN, MKT, RJM</t>
   </si>
   <si>
-    <t>PB7(CS221)-CL07/KJ,AST</t>
-  </si>
-  <si>
     <t>LB(CS242)-G4/AYS</t>
   </si>
   <si>
@@ -2110,6 +2101,15 @@
       </rPr>
       <t>/KJ</t>
     </r>
+  </si>
+  <si>
+    <t>PB(25B16CS212)-CL02,03,04/APJ,SHO,KRL</t>
+  </si>
+  <si>
+    <t>PB7(CS221)-CL07/TKT,AST</t>
+  </si>
+  <si>
+    <t>PB8(CS221)-CL02/VRN,KJ</t>
   </si>
 </sst>
 </file>
@@ -2172,7 +2172,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2278,6 +2278,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2437,7 +2443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2700,133 +2706,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2856,26 +2735,168 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3099,10 +3120,10 @@
   <dimension ref="A1:AA1060"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomRight" activeCell="D148" sqref="D148:E148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3123,18 +3144,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="114"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="134"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
@@ -3196,7 +3217,7 @@
       <c r="Y2" s="9"/>
     </row>
     <row r="3" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="127" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="12"/>
@@ -3208,7 +3229,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="96" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="I3" s="69" t="s">
         <v>15</v>
@@ -3233,24 +3254,24 @@
       <c r="Y3" s="9"/>
     </row>
     <row r="4" spans="1:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103"/>
+      <c r="A4" s="122"/>
       <c r="C4" s="77" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="F4" s="124" t="s">
+        <v>472</v>
+      </c>
+      <c r="F4" s="121" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I4" s="69" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K4" s="71"/>
       <c r="L4" s="9"/>
@@ -3269,9 +3290,9 @@
       <c r="Y4" s="9"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
+      <c r="A5" s="122"/>
       <c r="C5" s="93" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>318</v>
@@ -3279,9 +3300,9 @@
       <c r="E5" s="69" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="103"/>
-      <c r="G5" s="104" t="s">
-        <v>424</v>
+      <c r="F5" s="122"/>
+      <c r="G5" s="140" t="s">
+        <v>423</v>
       </c>
       <c r="H5" s="94" t="s">
         <v>323</v>
@@ -3290,7 +3311,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="69" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -3309,12 +3330,12 @@
       <c r="Y5" s="9"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="103"/>
+      <c r="A6" s="122"/>
       <c r="C6" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>321</v>
@@ -3322,11 +3343,11 @@
       <c r="F6" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="105"/>
+      <c r="G6" s="141"/>
       <c r="H6" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="I6" s="141" t="s">
+      <c r="I6" s="98" t="s">
         <v>266</v>
       </c>
       <c r="K6" s="9"/>
@@ -3346,12 +3367,12 @@
       <c r="Y6" s="9"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103"/>
+      <c r="A7" s="122"/>
       <c r="C7" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>25</v>
@@ -3359,7 +3380,7 @@
       <c r="F7" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="105"/>
+      <c r="G7" s="141"/>
       <c r="H7" s="2" t="s">
         <v>263</v>
       </c>
@@ -3384,20 +3405,20 @@
       <c r="Y7" s="9"/>
     </row>
     <row r="8" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
+      <c r="A8" s="122"/>
       <c r="C8" s="4" t="s">
         <v>229</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="E8" s="141" t="s">
+        <v>474</v>
+      </c>
+      <c r="E8" s="98" t="s">
         <v>253</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>511</v>
-      </c>
-      <c r="G8" s="105"/>
+        <v>509</v>
+      </c>
+      <c r="G8" s="141"/>
       <c r="H8" s="2" t="s">
         <v>264</v>
       </c>
@@ -3418,20 +3439,20 @@
       <c r="Y8" s="9"/>
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="103"/>
+      <c r="A9" s="122"/>
       <c r="C9" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E9" s="141" t="s">
+      <c r="E9" s="98" t="s">
         <v>254</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="G9" s="105"/>
+      <c r="G9" s="141"/>
       <c r="H9" s="2" t="s">
         <v>265</v>
       </c>
@@ -3453,7 +3474,7 @@
       <c r="Y9" s="9"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="103"/>
+      <c r="A10" s="122"/>
       <c r="D10" s="1" t="s">
         <v>320</v>
       </c>
@@ -3463,7 +3484,7 @@
       <c r="F10" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="G10" s="105"/>
+      <c r="G10" s="141"/>
       <c r="H10" s="2" t="s">
         <v>325</v>
       </c>
@@ -3486,7 +3507,7 @@
       <c r="AA10" s="17"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="103"/>
+      <c r="A11" s="122"/>
       <c r="C11" s="4" t="s">
         <v>241</v>
       </c>
@@ -3496,7 +3517,7 @@
       <c r="F11" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="G11" s="105"/>
+      <c r="G11" s="141"/>
       <c r="H11" s="69"/>
       <c r="K11" s="9"/>
       <c r="L11" s="16"/>
@@ -3517,7 +3538,7 @@
       <c r="AA11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="103"/>
+      <c r="A12" s="122"/>
       <c r="C12" s="77"/>
       <c r="D12" s="1" t="s">
         <v>24</v>
@@ -3525,11 +3546,11 @@
       <c r="F12" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="G12" s="105"/>
+      <c r="G12" s="141"/>
       <c r="H12" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I12" s="142" t="s">
+      <c r="I12" s="99" t="s">
         <v>386</v>
       </c>
       <c r="J12" s="69"/>
@@ -3552,22 +3573,22 @@
       <c r="AA12" s="17"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="103"/>
+      <c r="A13" s="122"/>
       <c r="C13" s="67" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E13" s="69" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="86" t="s">
-        <v>489</v>
-      </c>
-      <c r="G13" s="105"/>
+        <v>487</v>
+      </c>
+      <c r="G13" s="141"/>
       <c r="H13" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J13" s="69"/>
       <c r="K13" s="9"/>
@@ -3589,24 +3610,24 @@
       <c r="AA13" s="17"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="103"/>
+      <c r="A14" s="122"/>
       <c r="C14" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E14" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="105"/>
+      <c r="G14" s="141"/>
       <c r="H14" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="I14" s="126" t="s">
-        <v>556</v>
-      </c>
-      <c r="J14" s="103"/>
+        <v>433</v>
+      </c>
+      <c r="I14" s="125" t="s">
+        <v>553</v>
+      </c>
+      <c r="J14" s="122"/>
       <c r="K14" s="9"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -3626,7 +3647,7 @@
       <c r="AA14" s="17"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="103"/>
+      <c r="A15" s="122"/>
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
@@ -3636,14 +3657,14 @@
       <c r="F15" s="69" t="s">
         <v>259</v>
       </c>
-      <c r="G15" s="105"/>
+      <c r="G15" s="141"/>
       <c r="H15" s="85" t="s">
-        <v>522</v>
-      </c>
-      <c r="I15" s="126" t="s">
-        <v>557</v>
-      </c>
-      <c r="J15" s="103"/>
+        <v>520</v>
+      </c>
+      <c r="I15" s="125" t="s">
+        <v>554</v>
+      </c>
+      <c r="J15" s="122"/>
       <c r="K15" s="9"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -3663,7 +3684,7 @@
       <c r="AA15" s="17"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="103"/>
+      <c r="A16" s="122"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
         <v>352</v>
@@ -3671,11 +3692,11 @@
       <c r="F16" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="G16" s="105"/>
-      <c r="I16" s="126" t="s">
+      <c r="G16" s="141"/>
+      <c r="I16" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="103"/>
+      <c r="J16" s="122"/>
       <c r="K16" s="9"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -3695,20 +3716,20 @@
       <c r="AA16" s="17"/>
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="103"/>
+      <c r="A17" s="122"/>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
         <v>353</v>
       </c>
       <c r="E17" s="96" t="s">
-        <v>577</v>
-      </c>
-      <c r="G17" s="105"/>
+        <v>574</v>
+      </c>
+      <c r="G17" s="141"/>
       <c r="H17" s="72"/>
-      <c r="I17" s="108" t="s">
+      <c r="I17" s="115" t="s">
         <v>343</v>
       </c>
-      <c r="J17" s="101"/>
+      <c r="J17" s="116"/>
       <c r="K17" s="9"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
@@ -3728,13 +3749,13 @@
       <c r="AA17" s="17"/>
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="103"/>
+      <c r="A18" s="122"/>
       <c r="C18" s="4"/>
-      <c r="G18" s="105"/>
-      <c r="I18" s="108" t="s">
+      <c r="G18" s="141"/>
+      <c r="I18" s="115" t="s">
         <v>187</v>
       </c>
-      <c r="J18" s="101"/>
+      <c r="J18" s="116"/>
       <c r="K18" s="9"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
@@ -3754,17 +3775,17 @@
       <c r="AA18" s="17"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="103"/>
+      <c r="A19" s="122"/>
       <c r="C19" s="4"/>
-      <c r="E19" s="143" t="s">
-        <v>479</v>
+      <c r="E19" s="100" t="s">
+        <v>478</v>
       </c>
       <c r="F19" s="69"/>
-      <c r="G19" s="105"/>
-      <c r="I19" s="108" t="s">
+      <c r="G19" s="141"/>
+      <c r="I19" s="115" t="s">
         <v>213</v>
       </c>
-      <c r="J19" s="101"/>
+      <c r="J19" s="116"/>
       <c r="K19" s="9"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -3784,7 +3805,7 @@
       <c r="AA19" s="17"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="103"/>
+      <c r="A20" s="122"/>
       <c r="C20" s="4"/>
       <c r="D20" s="73" t="s">
         <v>317</v>
@@ -3792,11 +3813,11 @@
       <c r="F20" s="69" t="s">
         <v>257</v>
       </c>
-      <c r="G20" s="105"/>
-      <c r="I20" s="108" t="s">
+      <c r="G20" s="141"/>
+      <c r="I20" s="115" t="s">
         <v>206</v>
       </c>
-      <c r="J20" s="101"/>
+      <c r="J20" s="116"/>
       <c r="K20" s="9"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
@@ -3816,19 +3837,19 @@
       <c r="AA20" s="17"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="103"/>
+      <c r="A21" s="122"/>
       <c r="C21" s="4"/>
       <c r="E21" s="4" t="s">
         <v>235</v>
       </c>
       <c r="F21" s="69" t="s">
-        <v>558</v>
-      </c>
-      <c r="G21" s="105"/>
-      <c r="H21" s="108" t="s">
+        <v>555</v>
+      </c>
+      <c r="G21" s="141"/>
+      <c r="H21" s="115" t="s">
         <v>200</v>
       </c>
-      <c r="I21" s="101"/>
+      <c r="I21" s="116"/>
       <c r="K21" s="9"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
@@ -3848,18 +3869,18 @@
       <c r="AA21" s="17"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="103"/>
+      <c r="A22" s="122"/>
       <c r="C22" s="4"/>
       <c r="E22" s="4" t="s">
         <v>239</v>
       </c>
       <c r="F22" s="69"/>
-      <c r="G22" s="105"/>
+      <c r="G22" s="141"/>
       <c r="H22" s="72"/>
-      <c r="I22" s="108" t="s">
+      <c r="I22" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="J22" s="101"/>
+      <c r="J22" s="116"/>
       <c r="K22" s="9"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
@@ -3879,18 +3900,18 @@
       <c r="AA22" s="17"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="103"/>
+      <c r="A23" s="122"/>
       <c r="C23" s="4"/>
       <c r="E23" s="4" t="s">
         <v>245</v>
       </c>
       <c r="F23" s="69"/>
-      <c r="G23" s="105"/>
+      <c r="G23" s="141"/>
       <c r="H23" s="72"/>
-      <c r="I23" s="108" t="s">
+      <c r="I23" s="115" t="s">
         <v>226</v>
       </c>
-      <c r="J23" s="101"/>
+      <c r="J23" s="116"/>
       <c r="K23" s="9"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
@@ -3909,13 +3930,13 @@
       <c r="AA23" s="17"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
+      <c r="A24" s="122"/>
       <c r="C24" s="4"/>
       <c r="F24" s="69"/>
-      <c r="G24" s="105"/>
+      <c r="G24" s="141"/>
       <c r="H24" s="72"/>
-      <c r="I24" s="113"/>
-      <c r="J24" s="114"/>
+      <c r="I24" s="133"/>
+      <c r="J24" s="134"/>
       <c r="K24" s="9"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
@@ -3934,15 +3955,15 @@
       <c r="AA24" s="17"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="103"/>
+      <c r="A25" s="122"/>
       <c r="C25" s="4"/>
       <c r="F25" s="69"/>
-      <c r="G25" s="105"/>
+      <c r="G25" s="141"/>
       <c r="H25" s="72"/>
-      <c r="I25" s="108" t="s">
-        <v>515</v>
-      </c>
-      <c r="J25" s="101"/>
+      <c r="I25" s="115" t="s">
+        <v>513</v>
+      </c>
+      <c r="J25" s="116"/>
       <c r="K25" s="9"/>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
@@ -3961,15 +3982,15 @@
       <c r="AA25" s="17"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
+      <c r="A26" s="122"/>
       <c r="C26" s="4"/>
       <c r="F26" s="69"/>
-      <c r="G26" s="105"/>
+      <c r="G26" s="141"/>
       <c r="H26" s="72"/>
-      <c r="I26" s="108" t="s">
-        <v>566</v>
-      </c>
-      <c r="J26" s="101"/>
+      <c r="I26" s="115" t="s">
+        <v>563</v>
+      </c>
+      <c r="J26" s="116"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
@@ -3986,14 +4007,14 @@
       <c r="Y26" s="9"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="103"/>
+      <c r="A27" s="122"/>
       <c r="C27" s="4"/>
       <c r="F27" s="69"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="108" t="s">
-        <v>567</v>
-      </c>
-      <c r="I27" s="101"/>
+      <c r="G27" s="141"/>
+      <c r="H27" s="115" t="s">
+        <v>564</v>
+      </c>
+      <c r="I27" s="116"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -4010,10 +4031,10 @@
       <c r="Y27" s="9"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="103"/>
+      <c r="A28" s="122"/>
       <c r="C28" s="4"/>
       <c r="F28" s="69"/>
-      <c r="G28" s="132"/>
+      <c r="G28" s="142"/>
       <c r="H28" s="72"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -4057,7 +4078,7 @@
       <c r="Y29" s="9"/>
     </row>
     <row r="30" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="130" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="12"/>
@@ -4095,9 +4116,9 @@
       <c r="Y30" s="9"/>
     </row>
     <row r="31" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="99"/>
+      <c r="A31" s="131"/>
       <c r="C31" s="69" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D31" s="69" t="s">
         <v>32</v>
@@ -4105,11 +4126,11 @@
       <c r="E31" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="F31" s="124" t="s">
+      <c r="F31" s="121" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I31" s="69" t="s">
         <v>33</v>
@@ -4133,7 +4154,7 @@
       <c r="Y31" s="9"/>
     </row>
     <row r="32" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="99"/>
+      <c r="A32" s="131"/>
       <c r="C32" s="69" t="s">
         <v>324</v>
       </c>
@@ -4143,9 +4164,9 @@
       <c r="E32" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="F32" s="103"/>
+      <c r="F32" s="122"/>
       <c r="G32" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>279</v>
@@ -4172,7 +4193,7 @@
       <c r="Y32" s="9"/>
     </row>
     <row r="33" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="99"/>
+      <c r="A33" s="131"/>
       <c r="C33" s="69" t="s">
         <v>267</v>
       </c>
@@ -4184,13 +4205,13 @@
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>334</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -4208,26 +4229,26 @@
       <c r="Y33" s="9"/>
     </row>
     <row r="34" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="99"/>
+      <c r="A34" s="131"/>
       <c r="C34" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="D34" s="141" t="s">
+      <c r="D34" s="98" t="s">
         <v>329</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F34" s="69" t="s">
         <v>332</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="I34" s="141" t="s">
+        <v>468</v>
+      </c>
+      <c r="I34" s="98" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="2" t="s">
@@ -4251,23 +4272,23 @@
       <c r="AA34" s="17"/>
     </row>
     <row r="35" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="99"/>
+      <c r="A35" s="131"/>
       <c r="C35" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D35" s="141" t="s">
+      <c r="D35" s="98" t="s">
         <v>328</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="F35" s="124" t="s">
-        <v>511</v>
+      <c r="F35" s="121" t="s">
+        <v>509</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="I35" s="141" t="s">
+        <v>469</v>
+      </c>
+      <c r="I35" s="98" t="s">
         <v>283</v>
       </c>
       <c r="K35" s="16"/>
@@ -4288,22 +4309,22 @@
       <c r="AA35" s="17"/>
     </row>
     <row r="36" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="99"/>
+      <c r="A36" s="131"/>
       <c r="D36" s="69" t="s">
         <v>330</v>
       </c>
       <c r="E36" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="F36" s="103"/>
+      <c r="F36" s="122"/>
       <c r="G36" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>280</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
@@ -4323,7 +4344,7 @@
       <c r="AA36" s="17"/>
     </row>
     <row r="37" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
+      <c r="A37" s="131"/>
       <c r="C37" s="24"/>
       <c r="D37" s="69" t="s">
         <v>269</v>
@@ -4334,14 +4355,14 @@
       <c r="F37" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G37" s="104" t="s">
-        <v>424</v>
+      <c r="G37" s="140" t="s">
+        <v>423</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I37" s="144" t="s">
-        <v>428</v>
+      <c r="I37" s="101" t="s">
+        <v>427</v>
       </c>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
@@ -4361,17 +4382,17 @@
       <c r="AA37" s="17"/>
     </row>
     <row r="38" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="99"/>
+      <c r="A38" s="131"/>
       <c r="D38" s="23" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="G38" s="105"/>
+      <c r="G38" s="141"/>
       <c r="H38" s="1" t="s">
         <v>282</v>
       </c>
@@ -4394,17 +4415,17 @@
       <c r="AA38" s="17"/>
     </row>
     <row r="39" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="99"/>
+      <c r="A39" s="131"/>
       <c r="D39" s="69"/>
       <c r="E39" s="24" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="G39" s="105"/>
+      <c r="G39" s="141"/>
       <c r="H39" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I39" s="73" t="s">
         <v>389</v>
@@ -4431,14 +4452,14 @@
       <c r="AA39" s="17"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
+      <c r="A40" s="131"/>
       <c r="E40" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F40" s="86" t="s">
-        <v>489</v>
-      </c>
-      <c r="G40" s="105"/>
+        <v>487</v>
+      </c>
+      <c r="G40" s="141"/>
       <c r="J40" s="72" t="s">
         <v>232</v>
       </c>
@@ -4461,14 +4482,14 @@
       <c r="AA40" s="17"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
+      <c r="A41" s="131"/>
       <c r="E41" s="69"/>
       <c r="F41" s="69" t="s">
         <v>258</v>
       </c>
-      <c r="G41" s="105"/>
+      <c r="G41" s="141"/>
       <c r="H41" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="72" t="s">
@@ -4493,14 +4514,14 @@
       <c r="AA41" s="17"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="99"/>
+      <c r="A42" s="131"/>
       <c r="D42" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F42" s="69" t="s">
         <v>276</v>
       </c>
-      <c r="G42" s="105"/>
+      <c r="G42" s="141"/>
       <c r="H42" s="1" t="s">
         <v>333</v>
       </c>
@@ -4525,7 +4546,7 @@
       <c r="AA42" s="17"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="99"/>
+      <c r="A43" s="131"/>
       <c r="D43" s="4" t="s">
         <v>238</v>
       </c>
@@ -4533,7 +4554,7 @@
       <c r="F43" s="69" t="s">
         <v>277</v>
       </c>
-      <c r="G43" s="105"/>
+      <c r="G43" s="141"/>
       <c r="J43" s="69" t="s">
         <v>278</v>
       </c>
@@ -4554,23 +4575,23 @@
       <c r="Y43" s="9"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="99"/>
+      <c r="A44" s="131"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="153" t="s">
-        <v>529</v>
-      </c>
-      <c r="D44" s="154"/>
+      <c r="C44" s="113" t="s">
+        <v>527</v>
+      </c>
+      <c r="D44" s="114"/>
       <c r="E44" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G44" s="105"/>
+      <c r="G44" s="141"/>
       <c r="H44" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="I44" s="108" t="s">
+      <c r="I44" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="J44" s="101"/>
+      <c r="J44" s="116"/>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
@@ -4588,23 +4609,23 @@
       <c r="Y44" s="9"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="99"/>
+      <c r="A45" s="131"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="108" t="s">
+      <c r="C45" s="115" t="s">
         <v>189</v>
       </c>
-      <c r="D45" s="101"/>
+      <c r="D45" s="116"/>
       <c r="F45" s="79" t="s">
-        <v>514</v>
-      </c>
-      <c r="G45" s="105"/>
+        <v>512</v>
+      </c>
+      <c r="G45" s="141"/>
       <c r="H45" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I45" s="108" t="s">
+      <c r="I45" s="115" t="s">
         <v>210</v>
       </c>
-      <c r="J45" s="101"/>
+      <c r="J45" s="116"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
@@ -4622,20 +4643,20 @@
       <c r="Y45" s="9"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="99"/>
+      <c r="A46" s="131"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="109" t="s">
-        <v>527</v>
-      </c>
-      <c r="D46" s="110"/>
+      <c r="C46" s="123" t="s">
+        <v>525</v>
+      </c>
+      <c r="D46" s="124"/>
       <c r="E46" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G46" s="105"/>
-      <c r="I46" s="108" t="s">
+      <c r="G46" s="141"/>
+      <c r="I46" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="J46" s="101"/>
+      <c r="J46" s="116"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
@@ -4653,20 +4674,20 @@
       <c r="Y46" s="9"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="99"/>
+      <c r="A47" s="131"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="108" t="s">
+      <c r="C47" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="D47" s="101"/>
-      <c r="E47" s="142" t="s">
+      <c r="D47" s="116"/>
+      <c r="E47" s="99" t="s">
         <v>387</v>
       </c>
-      <c r="G47" s="105"/>
-      <c r="I47" s="108" t="s">
-        <v>505</v>
-      </c>
-      <c r="J47" s="101"/>
+      <c r="G47" s="141"/>
+      <c r="I47" s="115" t="s">
+        <v>503</v>
+      </c>
+      <c r="J47" s="116"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
@@ -4684,20 +4705,20 @@
       <c r="Y47" s="9"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="99"/>
-      <c r="C48" s="108" t="s">
-        <v>481</v>
-      </c>
-      <c r="D48" s="101"/>
-      <c r="E48" s="142" t="s">
+      <c r="A48" s="131"/>
+      <c r="C48" s="115" t="s">
+        <v>480</v>
+      </c>
+      <c r="D48" s="116"/>
+      <c r="E48" s="99" t="s">
         <v>388</v>
       </c>
       <c r="F48" s="69"/>
-      <c r="G48" s="105"/>
-      <c r="I48" s="115" t="s">
-        <v>569</v>
-      </c>
-      <c r="J48" s="116"/>
+      <c r="G48" s="141"/>
+      <c r="I48" s="145" t="s">
+        <v>566</v>
+      </c>
+      <c r="J48" s="146"/>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
@@ -4715,21 +4736,21 @@
       <c r="Y48" s="9"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="99"/>
+      <c r="A49" s="131"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="106" t="s">
-        <v>516</v>
-      </c>
-      <c r="D49" s="107"/>
-      <c r="E49" s="108" t="s">
-        <v>456</v>
-      </c>
-      <c r="F49" s="101"/>
-      <c r="G49" s="105"/>
-      <c r="I49" s="115" t="s">
-        <v>570</v>
-      </c>
-      <c r="J49" s="116"/>
+      <c r="C49" s="119" t="s">
+        <v>514</v>
+      </c>
+      <c r="D49" s="120"/>
+      <c r="E49" s="115" t="s">
+        <v>455</v>
+      </c>
+      <c r="F49" s="116"/>
+      <c r="G49" s="141"/>
+      <c r="I49" s="145" t="s">
+        <v>567</v>
+      </c>
+      <c r="J49" s="146"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
@@ -4747,19 +4768,19 @@
       <c r="Y49" s="9"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="99"/>
+      <c r="A50" s="131"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="108" t="s">
-        <v>482</v>
-      </c>
-      <c r="D50" s="101"/>
+      <c r="C50" s="115" t="s">
+        <v>481</v>
+      </c>
+      <c r="D50" s="116"/>
       <c r="E50" s="69"/>
       <c r="F50" s="69"/>
-      <c r="G50" s="105"/>
-      <c r="I50" s="108" t="s">
-        <v>484</v>
-      </c>
-      <c r="J50" s="101"/>
+      <c r="G50" s="141"/>
+      <c r="I50" s="115" t="s">
+        <v>483</v>
+      </c>
+      <c r="J50" s="116"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
@@ -4777,15 +4798,15 @@
       <c r="Y50" s="9"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="99"/>
+      <c r="A51" s="131"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="158" t="s">
-        <v>503</v>
-      </c>
-      <c r="D51" s="157"/>
+      <c r="C51" s="112" t="s">
+        <v>501</v>
+      </c>
+      <c r="D51" s="111"/>
       <c r="E51" s="69"/>
       <c r="F51" s="69"/>
-      <c r="G51" s="105"/>
+      <c r="G51" s="141"/>
       <c r="I51" s="70"/>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -4804,17 +4825,17 @@
       <c r="Y51" s="9"/>
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="100"/>
-      <c r="C52" s="108" t="s">
+      <c r="A52" s="132"/>
+      <c r="C52" s="115" t="s">
         <v>188</v>
       </c>
-      <c r="D52" s="101"/>
+      <c r="D52" s="116"/>
       <c r="E52" s="69"/>
       <c r="F52" s="69"/>
-      <c r="G52" s="105"/>
+      <c r="G52" s="141"/>
       <c r="H52" s="25"/>
-      <c r="I52" s="122"/>
-      <c r="J52" s="123"/>
+      <c r="I52" s="143"/>
+      <c r="J52" s="144"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
@@ -4838,7 +4859,7 @@
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="105"/>
+      <c r="G53" s="141"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
@@ -4859,11 +4880,11 @@
       <c r="Y53" s="9"/>
     </row>
     <row r="54" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="117" t="s">
         <v>40</v>
       </c>
       <c r="B54" s="27"/>
-      <c r="G54" s="105"/>
+      <c r="G54" s="141"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -4881,8 +4902,8 @@
       <c r="Y54" s="9"/>
     </row>
     <row r="55" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="134"/>
-      <c r="G55" s="105"/>
+      <c r="A55" s="118"/>
+      <c r="G55" s="141"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -4900,7 +4921,7 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="56" spans="1:27" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="134"/>
+      <c r="A56" s="118"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -4926,7 +4947,7 @@
       <c r="Y56" s="9"/>
     </row>
     <row r="57" spans="1:27" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="134"/>
+      <c r="A57" s="118"/>
       <c r="D57" s="69" t="s">
         <v>46</v>
       </c>
@@ -4936,8 +4957,8 @@
       <c r="F57" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="104" t="s">
-        <v>424</v>
+      <c r="G57" s="140" t="s">
+        <v>423</v>
       </c>
       <c r="H57" s="28" t="s">
         <v>10</v>
@@ -4962,8 +4983,8 @@
       <c r="Y57" s="13"/>
     </row>
     <row r="58" spans="1:27" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="134"/>
-      <c r="C58" s="145" t="s">
+      <c r="A58" s="118"/>
+      <c r="C58" s="102" t="s">
         <v>357</v>
       </c>
       <c r="D58" s="69" t="s">
@@ -4972,7 +4993,7 @@
       <c r="E58" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G58" s="105"/>
+      <c r="G58" s="141"/>
       <c r="H58" s="23" t="s">
         <v>362</v>
       </c>
@@ -4999,28 +5020,28 @@
       <c r="Y58" s="13"/>
     </row>
     <row r="59" spans="1:27" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="134"/>
+      <c r="A59" s="118"/>
       <c r="C59" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="D59" s="141" t="s">
+      <c r="D59" s="98" t="s">
         <v>284</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F59" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="G59" s="105"/>
+      <c r="G59" s="141"/>
       <c r="H59" s="23" t="s">
         <v>363</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K59" s="80"/>
       <c r="L59" s="80"/>
@@ -5041,7 +5062,7 @@
       <c r="AA59" s="81"/>
     </row>
     <row r="60" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="134"/>
+      <c r="A60" s="118"/>
       <c r="C60" s="4" t="s">
         <v>360</v>
       </c>
@@ -5052,15 +5073,15 @@
       <c r="F60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G60" s="105"/>
+      <c r="G60" s="141"/>
       <c r="H60" s="23" t="s">
         <v>364</v>
       </c>
       <c r="I60" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="J60" s="141" t="s">
-        <v>518</v>
+      <c r="J60" s="98" t="s">
+        <v>516</v>
       </c>
       <c r="K60" s="80"/>
       <c r="L60" s="80"/>
@@ -5081,24 +5102,24 @@
       <c r="AA60" s="81"/>
     </row>
     <row r="61" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="134"/>
+      <c r="A61" s="118"/>
       <c r="C61" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="D61" s="141" t="s">
+      <c r="D61" s="98" t="s">
         <v>285</v>
       </c>
-      <c r="E61" s="145" t="s">
+      <c r="E61" s="102" t="s">
         <v>288</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G61" s="105"/>
+      <c r="G61" s="141"/>
       <c r="H61" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="I61" s="141" t="s">
+        <v>561</v>
+      </c>
+      <c r="I61" s="98" t="s">
         <v>290</v>
       </c>
       <c r="J61" s="24" t="s">
@@ -5123,28 +5144,28 @@
       <c r="AA61" s="81"/>
     </row>
     <row r="62" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="134"/>
+      <c r="A62" s="118"/>
       <c r="C62" s="23" t="s">
-        <v>442</v>
-      </c>
-      <c r="D62" s="141" t="s">
+        <v>441</v>
+      </c>
+      <c r="D62" s="98" t="s">
         <v>286</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="F62" s="88" t="s">
-        <v>524</v>
-      </c>
-      <c r="G62" s="105"/>
+        <v>522</v>
+      </c>
+      <c r="G62" s="141"/>
       <c r="H62" s="23" t="s">
         <v>365</v>
       </c>
       <c r="I62" s="69" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K62" s="80"/>
       <c r="L62" s="80"/>
@@ -5165,7 +5186,7 @@
       <c r="AA62" s="81"/>
     </row>
     <row r="63" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="134"/>
+      <c r="A63" s="118"/>
       <c r="C63" s="23" t="s">
         <v>240</v>
       </c>
@@ -5176,7 +5197,7 @@
       <c r="F63" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="G63" s="105"/>
+      <c r="G63" s="141"/>
       <c r="H63" s="23" t="s">
         <v>366</v>
       </c>
@@ -5202,19 +5223,19 @@
       <c r="AA63" s="81"/>
     </row>
     <row r="64" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="134"/>
-      <c r="C64" s="145" t="s">
+      <c r="A64" s="118"/>
+      <c r="C64" s="102" t="s">
         <v>391</v>
       </c>
       <c r="D64" s="69" t="s">
         <v>337</v>
       </c>
-      <c r="G64" s="105"/>
+      <c r="G64" s="141"/>
       <c r="H64" s="23" t="s">
         <v>367</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J64" s="23" t="s">
         <v>291</v>
@@ -5238,7 +5259,7 @@
       <c r="AA64" s="81"/>
     </row>
     <row r="65" spans="1:27" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="134"/>
+      <c r="A65" s="118"/>
       <c r="D65" s="23" t="s">
         <v>39</v>
       </c>
@@ -5246,9 +5267,9 @@
         <v>25</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>546</v>
-      </c>
-      <c r="G65" s="105"/>
+        <v>543</v>
+      </c>
+      <c r="G65" s="141"/>
       <c r="H65" s="23" t="s">
         <v>368</v>
       </c>
@@ -5272,19 +5293,19 @@
       <c r="AA65" s="81"/>
     </row>
     <row r="66" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="134"/>
+      <c r="A66" s="118"/>
       <c r="B66" s="82"/>
-      <c r="C66" s="146" t="s">
+      <c r="C66" s="103" t="s">
         <v>406</v>
       </c>
-      <c r="D66" s="141" t="s">
-        <v>560</v>
+      <c r="D66" s="98" t="s">
+        <v>557</v>
       </c>
       <c r="E66" s="41"/>
       <c r="F66" s="23" t="s">
-        <v>545</v>
-      </c>
-      <c r="G66" s="105"/>
+        <v>542</v>
+      </c>
+      <c r="G66" s="141"/>
       <c r="H66" s="23" t="s">
         <v>370</v>
       </c>
@@ -5310,17 +5331,17 @@
       <c r="AA66" s="81"/>
     </row>
     <row r="67" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="134"/>
-      <c r="C67" s="145" t="s">
+      <c r="A67" s="118"/>
+      <c r="C67" s="102" t="s">
+        <v>541</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="F67" s="23" t="s">
         <v>544</v>
       </c>
-      <c r="D67" s="23" t="s">
-        <v>437</v>
-      </c>
-      <c r="F67" s="23" t="s">
-        <v>547</v>
-      </c>
-      <c r="G67" s="105"/>
+      <c r="G67" s="141"/>
       <c r="H67" s="23" t="s">
         <v>371</v>
       </c>
@@ -5328,7 +5349,7 @@
         <v>45</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K67" s="80"/>
       <c r="L67" s="80"/>
@@ -5349,24 +5370,24 @@
       <c r="AA67" s="81"/>
     </row>
     <row r="68" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="134"/>
+      <c r="A68" s="118"/>
       <c r="C68" s="90" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D68" s="67" t="s">
-        <v>509</v>
-      </c>
-      <c r="F68" s="147" t="s">
+        <v>507</v>
+      </c>
+      <c r="F68" s="104" t="s">
         <v>405</v>
       </c>
-      <c r="G68" s="105"/>
+      <c r="G68" s="141"/>
       <c r="H68" s="23" t="s">
         <v>372</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>559</v>
-      </c>
-      <c r="J68" s="147" t="s">
+        <v>556</v>
+      </c>
+      <c r="J68" s="104" t="s">
         <v>403</v>
       </c>
       <c r="K68" s="80"/>
@@ -5388,12 +5409,12 @@
       <c r="AA68" s="81"/>
     </row>
     <row r="69" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="134"/>
+      <c r="A69" s="118"/>
       <c r="B69" s="83"/>
-      <c r="C69" s="135" t="s">
+      <c r="C69" s="128" t="s">
         <v>203</v>
       </c>
-      <c r="D69" s="136"/>
+      <c r="D69" s="129"/>
       <c r="G69" s="69"/>
       <c r="H69" s="23" t="s">
         <v>373</v>
@@ -5415,22 +5436,22 @@
       <c r="Y69" s="13"/>
     </row>
     <row r="70" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="134"/>
+      <c r="A70" s="118"/>
       <c r="B70" s="83"/>
-      <c r="C70" s="108" t="s">
+      <c r="C70" s="115" t="s">
         <v>191</v>
       </c>
-      <c r="D70" s="101"/>
-      <c r="G70" s="111" t="s">
-        <v>496</v>
+      <c r="D70" s="116"/>
+      <c r="G70" s="157" t="s">
+        <v>494</v>
       </c>
       <c r="H70" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="I70" s="108" t="s">
+      <c r="I70" s="115" t="s">
         <v>192</v>
       </c>
-      <c r="J70" s="101"/>
+      <c r="J70" s="116"/>
       <c r="K70" s="13"/>
       <c r="L70" s="13"/>
       <c r="M70" s="13"/>
@@ -5448,24 +5469,24 @@
       <c r="Y70" s="13"/>
     </row>
     <row r="71" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="134"/>
+      <c r="A71" s="118"/>
       <c r="B71" s="83"/>
-      <c r="C71" s="108" t="s">
+      <c r="C71" s="115" t="s">
         <v>211</v>
       </c>
-      <c r="D71" s="101"/>
-      <c r="E71" s="108" t="s">
-        <v>463</v>
-      </c>
-      <c r="F71" s="101"/>
-      <c r="G71" s="112"/>
+      <c r="D71" s="116"/>
+      <c r="E71" s="115" t="s">
+        <v>462</v>
+      </c>
+      <c r="F71" s="116"/>
+      <c r="G71" s="158"/>
       <c r="H71" s="23" t="s">
-        <v>426</v>
-      </c>
-      <c r="I71" s="108" t="s">
+        <v>425</v>
+      </c>
+      <c r="I71" s="115" t="s">
         <v>207</v>
       </c>
-      <c r="J71" s="101"/>
+      <c r="J71" s="116"/>
       <c r="K71" s="13"/>
       <c r="L71" s="13"/>
       <c r="M71" s="13"/>
@@ -5483,26 +5504,26 @@
       <c r="Y71" s="13"/>
     </row>
     <row r="72" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="134"/>
+      <c r="A72" s="118"/>
       <c r="B72" s="83"/>
-      <c r="C72" s="109" t="s">
-        <v>530</v>
-      </c>
-      <c r="D72" s="110"/>
-      <c r="E72" s="108" t="s">
+      <c r="C72" s="123" t="s">
+        <v>528</v>
+      </c>
+      <c r="D72" s="124"/>
+      <c r="E72" s="115" t="s">
         <v>228</v>
       </c>
-      <c r="F72" s="101"/>
+      <c r="F72" s="116"/>
       <c r="G72" s="95" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="I72" s="108" t="s">
+      <c r="I72" s="115" t="s">
         <v>214</v>
       </c>
-      <c r="J72" s="101"/>
+      <c r="J72" s="116"/>
       <c r="K72" s="13"/>
       <c r="L72" s="13"/>
       <c r="M72" s="13"/>
@@ -5520,24 +5541,24 @@
       <c r="Y72" s="13"/>
     </row>
     <row r="73" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="134"/>
+      <c r="A73" s="118"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="108" t="s">
+      <c r="C73" s="115" t="s">
         <v>224</v>
       </c>
-      <c r="D73" s="101"/>
-      <c r="E73" s="108" t="s">
+      <c r="D73" s="116"/>
+      <c r="E73" s="115" t="s">
         <v>252</v>
       </c>
-      <c r="F73" s="101"/>
+      <c r="F73" s="116"/>
       <c r="G73" s="69"/>
-      <c r="H73" s="148" t="s">
-        <v>517</v>
-      </c>
-      <c r="I73" s="108" t="s">
-        <v>506</v>
-      </c>
-      <c r="J73" s="101"/>
+      <c r="H73" s="105" t="s">
+        <v>515</v>
+      </c>
+      <c r="I73" s="115" t="s">
+        <v>504</v>
+      </c>
+      <c r="J73" s="116"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -5555,16 +5576,16 @@
       <c r="Y73" s="9"/>
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="134"/>
-      <c r="E74" s="115" t="s">
-        <v>571</v>
-      </c>
-      <c r="F74" s="116"/>
+      <c r="A74" s="118"/>
+      <c r="E74" s="145" t="s">
+        <v>568</v>
+      </c>
+      <c r="F74" s="146"/>
       <c r="G74" s="69"/>
-      <c r="I74" s="108" t="s">
+      <c r="I74" s="115" t="s">
         <v>218</v>
       </c>
-      <c r="J74" s="101"/>
+      <c r="J74" s="116"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -5582,19 +5603,19 @@
       <c r="Y74" s="9"/>
     </row>
     <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="134"/>
+      <c r="A75" s="118"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="108"/>
-      <c r="D75" s="101"/>
-      <c r="E75" s="113" t="s">
+      <c r="C75" s="115"/>
+      <c r="D75" s="116"/>
+      <c r="E75" s="133" t="s">
         <v>249</v>
       </c>
-      <c r="F75" s="114"/>
+      <c r="F75" s="134"/>
       <c r="G75" s="69"/>
-      <c r="I75" s="106" t="s">
-        <v>451</v>
-      </c>
-      <c r="J75" s="107"/>
+      <c r="I75" s="119" t="s">
+        <v>450</v>
+      </c>
+      <c r="J75" s="120"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -5612,17 +5633,17 @@
       <c r="Y75" s="9"/>
     </row>
     <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="134"/>
+      <c r="A76" s="118"/>
       <c r="B76" s="6"/>
       <c r="C76" s="70"/>
       <c r="D76" s="71"/>
-      <c r="E76" s="108" t="s">
-        <v>431</v>
-      </c>
-      <c r="F76" s="101"/>
+      <c r="E76" s="115" t="s">
+        <v>430</v>
+      </c>
+      <c r="F76" s="116"/>
       <c r="G76" s="69"/>
       <c r="J76" s="91" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
@@ -5667,7 +5688,7 @@
       <c r="Y77" s="9"/>
     </row>
     <row r="78" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="98" t="s">
+      <c r="A78" s="130" t="s">
         <v>55</v>
       </c>
       <c r="B78" s="12"/>
@@ -5675,19 +5696,19 @@
         <v>341</v>
       </c>
       <c r="D78" s="69" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G78" s="102" t="s">
-        <v>423</v>
+      <c r="G78" s="156" t="s">
+        <v>422</v>
       </c>
       <c r="H78" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="69" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -5708,9 +5729,9 @@
       <c r="AA78" s="9"/>
     </row>
     <row r="79" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="99"/>
+      <c r="A79" s="131"/>
       <c r="C79" s="84" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D79" s="69" t="s">
         <v>58</v>
@@ -5721,7 +5742,7 @@
       <c r="F79" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="G79" s="103"/>
+      <c r="G79" s="122"/>
       <c r="H79" s="4" t="s">
         <v>374</v>
       </c>
@@ -5747,7 +5768,7 @@
       <c r="AA79" s="9"/>
     </row>
     <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="99"/>
+      <c r="A80" s="131"/>
       <c r="C80" s="2" t="s">
         <v>62</v>
       </c>
@@ -5760,7 +5781,7 @@
       <c r="F80" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G80" s="103"/>
+      <c r="G80" s="122"/>
       <c r="H80" s="4" t="s">
         <v>375</v>
       </c>
@@ -5787,17 +5808,17 @@
       <c r="Y80" s="9"/>
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="99"/>
-      <c r="C81" s="141" t="s">
+      <c r="A81" s="131"/>
+      <c r="C81" s="98" t="s">
         <v>288</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E81" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="G81" s="103"/>
+      <c r="G81" s="122"/>
       <c r="H81" s="4" t="s">
         <v>376</v>
       </c>
@@ -5805,7 +5826,7 @@
         <v>49</v>
       </c>
       <c r="J81" s="69" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
@@ -5824,25 +5845,25 @@
       <c r="Y81" s="9"/>
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="99"/>
+      <c r="A82" s="131"/>
       <c r="C82" s="5" t="s">
         <v>292</v>
       </c>
       <c r="D82" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E82" s="145" t="s">
+      <c r="E82" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="F82" s="141" t="s">
-        <v>578</v>
-      </c>
-      <c r="G82" s="103"/>
+      <c r="F82" s="98" t="s">
+        <v>575</v>
+      </c>
+      <c r="G82" s="122"/>
       <c r="H82" s="4" t="s">
         <v>377</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -5860,8 +5881,8 @@
       <c r="Y82" s="9"/>
     </row>
     <row r="83" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="99"/>
-      <c r="D83" s="141" t="s">
+      <c r="A83" s="131"/>
+      <c r="D83" s="98" t="s">
         <v>287</v>
       </c>
       <c r="E83" s="23" t="s">
@@ -5870,11 +5891,11 @@
       <c r="F83" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="G83" s="103"/>
+      <c r="G83" s="122"/>
       <c r="H83" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="I83" s="141" t="s">
+        <v>562</v>
+      </c>
+      <c r="I83" s="98" t="s">
         <v>285</v>
       </c>
       <c r="J83" s="69" t="s">
@@ -5897,20 +5918,20 @@
       <c r="Y83" s="9"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="99"/>
+      <c r="A84" s="131"/>
       <c r="C84" s="4" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="G84" s="103"/>
+      <c r="G84" s="122"/>
       <c r="H84" s="73" t="s">
         <v>397</v>
       </c>
@@ -5937,7 +5958,7 @@
       <c r="Y84" s="9"/>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="99"/>
+      <c r="A85" s="131"/>
       <c r="C85" s="4" t="s">
         <v>393</v>
       </c>
@@ -5945,12 +5966,12 @@
         <v>358</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G85" s="103"/>
+      <c r="G85" s="122"/>
       <c r="H85" s="4" t="s">
         <v>398</v>
       </c>
@@ -5958,7 +5979,7 @@
         <v>411</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
@@ -5977,17 +5998,17 @@
       <c r="Y85" s="9"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="99"/>
+      <c r="A86" s="131"/>
       <c r="C86" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="E86" s="149" t="s">
-        <v>572</v>
+        <v>546</v>
+      </c>
+      <c r="E86" s="106" t="s">
+        <v>569</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="G86" s="103"/>
+        <v>537</v>
+      </c>
+      <c r="G86" s="122"/>
       <c r="H86" s="2" t="s">
         <v>378</v>
       </c>
@@ -6016,19 +6037,19 @@
       <c r="AA86" s="31"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="99"/>
+      <c r="A87" s="131"/>
       <c r="E87" s="73" t="s">
         <v>394</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="G87" s="103"/>
+      <c r="G87" s="122"/>
       <c r="H87" s="2" t="s">
         <v>379</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>301</v>
@@ -6051,15 +6072,15 @@
       <c r="AA87" s="31"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="99"/>
+      <c r="A88" s="131"/>
       <c r="C88" s="2"/>
       <c r="E88" s="89" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="G88" s="103"/>
+      <c r="G88" s="122"/>
       <c r="H88" s="1" t="s">
         <v>380</v>
       </c>
@@ -6081,10 +6102,10 @@
       <c r="AA88" s="17"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="99"/>
+      <c r="A89" s="131"/>
       <c r="B89" s="29"/>
       <c r="G89" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>381</v>
@@ -6113,19 +6134,19 @@
       <c r="AA89" s="17"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="99"/>
-      <c r="C90" s="106" t="s">
-        <v>502</v>
-      </c>
-      <c r="D90" s="107"/>
+      <c r="A90" s="131"/>
+      <c r="C90" s="119" t="s">
+        <v>500</v>
+      </c>
+      <c r="D90" s="120"/>
       <c r="G90" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>382</v>
       </c>
       <c r="I90" s="89" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K90" s="16"/>
       <c r="L90" s="16"/>
@@ -6146,11 +6167,11 @@
       <c r="AA90" s="17"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="99"/>
-      <c r="C91" s="106" t="s">
+      <c r="A91" s="131"/>
+      <c r="C91" s="119" t="s">
         <v>251</v>
       </c>
-      <c r="D91" s="152"/>
+      <c r="D91" s="155"/>
       <c r="H91" s="1" t="s">
         <v>383</v>
       </c>
@@ -6176,11 +6197,11 @@
       <c r="AA91" s="17"/>
     </row>
     <row r="92" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="99"/>
+      <c r="A92" s="131"/>
       <c r="E92" s="61"/>
       <c r="G92" s="32"/>
       <c r="H92" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J92" s="69"/>
       <c r="K92" s="16"/>
@@ -6202,13 +6223,13 @@
       <c r="AA92" s="17"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="99"/>
+      <c r="A93" s="131"/>
       <c r="C93" s="85" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G93" s="32"/>
       <c r="H93" s="78" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J93" s="69"/>
       <c r="K93" s="9"/>
@@ -6228,22 +6249,22 @@
       <c r="Y93" s="9"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="99"/>
+      <c r="A94" s="131"/>
       <c r="B94" s="6"/>
-      <c r="C94" s="108" t="s">
+      <c r="C94" s="115" t="s">
         <v>204</v>
       </c>
-      <c r="D94" s="101"/>
-      <c r="E94" s="108" t="s">
+      <c r="D94" s="116"/>
+      <c r="E94" s="115" t="s">
         <v>216</v>
       </c>
-      <c r="F94" s="101"/>
+      <c r="F94" s="116"/>
       <c r="G94" s="32"/>
       <c r="H94" s="69"/>
-      <c r="I94" s="108" t="s">
+      <c r="I94" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="J94" s="101"/>
+      <c r="J94" s="116"/>
       <c r="K94" s="9"/>
       <c r="L94" s="9"/>
       <c r="M94" s="9"/>
@@ -6261,22 +6282,22 @@
       <c r="Y94" s="9"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="99"/>
+      <c r="A95" s="131"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="108" t="s">
-        <v>461</v>
-      </c>
-      <c r="D95" s="101"/>
-      <c r="E95" s="108" t="s">
+      <c r="C95" s="115" t="s">
+        <v>460</v>
+      </c>
+      <c r="D95" s="116"/>
+      <c r="E95" s="115" t="s">
         <v>225</v>
       </c>
-      <c r="F95" s="101"/>
+      <c r="F95" s="116"/>
       <c r="G95" s="32"/>
       <c r="H95" s="69"/>
-      <c r="I95" s="108" t="s">
+      <c r="I95" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="J95" s="101"/>
+      <c r="J95" s="116"/>
       <c r="K95" s="9"/>
       <c r="L95" s="9"/>
       <c r="M95" s="9"/>
@@ -6294,21 +6315,21 @@
       <c r="Y95" s="9"/>
     </row>
     <row r="96" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="99"/>
+      <c r="A96" s="131"/>
       <c r="B96" s="6"/>
-      <c r="C96" s="108" t="s">
+      <c r="C96" s="115" t="s">
         <v>199</v>
       </c>
-      <c r="D96" s="101"/>
-      <c r="E96" s="126" t="s">
-        <v>553</v>
-      </c>
-      <c r="F96" s="103"/>
+      <c r="D96" s="116"/>
+      <c r="E96" s="125" t="s">
+        <v>550</v>
+      </c>
+      <c r="F96" s="122"/>
       <c r="G96" s="32"/>
-      <c r="H96" s="108" t="s">
-        <v>563</v>
-      </c>
-      <c r="I96" s="101"/>
+      <c r="H96" s="115" t="s">
+        <v>560</v>
+      </c>
+      <c r="I96" s="116"/>
       <c r="J96" s="61"/>
       <c r="K96" s="9"/>
       <c r="L96" s="9"/>
@@ -6327,22 +6348,22 @@
       <c r="Y96" s="9"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="99"/>
+      <c r="A97" s="131"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="108" t="s">
-        <v>504</v>
-      </c>
-      <c r="D97" s="101"/>
-      <c r="E97" s="126" t="s">
-        <v>552</v>
-      </c>
-      <c r="F97" s="103"/>
+      <c r="C97" s="115" t="s">
+        <v>502</v>
+      </c>
+      <c r="D97" s="116"/>
+      <c r="E97" s="125" t="s">
+        <v>549</v>
+      </c>
+      <c r="F97" s="122"/>
       <c r="G97" s="32"/>
       <c r="H97" s="69"/>
-      <c r="I97" s="106" t="s">
-        <v>535</v>
-      </c>
-      <c r="J97" s="107"/>
+      <c r="I97" s="119" t="s">
+        <v>533</v>
+      </c>
+      <c r="J97" s="120"/>
       <c r="K97" s="9"/>
       <c r="L97" s="9"/>
       <c r="M97" s="9"/>
@@ -6360,20 +6381,20 @@
       <c r="Y97" s="9"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="99"/>
+      <c r="A98" s="131"/>
       <c r="B98" s="6"/>
-      <c r="C98" s="108" t="s">
+      <c r="C98" s="115" t="s">
         <v>223</v>
       </c>
-      <c r="D98" s="101"/>
-      <c r="E98" s="126" t="s">
+      <c r="D98" s="116"/>
+      <c r="E98" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="F98" s="103"/>
+      <c r="F98" s="122"/>
       <c r="G98" s="32"/>
       <c r="H98" s="75"/>
-      <c r="I98" s="122"/>
-      <c r="J98" s="123"/>
+      <c r="I98" s="143"/>
+      <c r="J98" s="144"/>
       <c r="K98" s="9"/>
       <c r="L98" s="9"/>
       <c r="M98" s="9"/>
@@ -6391,16 +6412,16 @@
       <c r="Y98" s="9"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="99"/>
+      <c r="A99" s="131"/>
       <c r="B99" s="6"/>
-      <c r="C99" s="113" t="s">
+      <c r="C99" s="133" t="s">
         <v>250</v>
       </c>
-      <c r="D99" s="114"/>
-      <c r="E99" s="113" t="s">
+      <c r="D99" s="134"/>
+      <c r="E99" s="133" t="s">
         <v>407</v>
       </c>
-      <c r="F99" s="114"/>
+      <c r="F99" s="134"/>
       <c r="G99" s="32"/>
       <c r="H99" s="75"/>
       <c r="J99" s="75"/>
@@ -6421,14 +6442,14 @@
       <c r="Y99" s="9"/>
     </row>
     <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="99"/>
+      <c r="A100" s="131"/>
       <c r="B100" s="6"/>
       <c r="C100" s="70"/>
       <c r="D100" s="71"/>
-      <c r="E100" s="108" t="s">
-        <v>485</v>
-      </c>
-      <c r="F100" s="101"/>
+      <c r="E100" s="115" t="s">
+        <v>484</v>
+      </c>
+      <c r="F100" s="116"/>
       <c r="G100" s="32"/>
       <c r="H100" s="75"/>
       <c r="I100" s="75"/>
@@ -6450,14 +6471,14 @@
       <c r="Y100" s="9"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="99"/>
+      <c r="A101" s="131"/>
       <c r="B101" s="6"/>
       <c r="C101" s="70"/>
       <c r="D101" s="71"/>
-      <c r="E101" s="117" t="s">
+      <c r="E101" s="148" t="s">
         <v>81</v>
       </c>
-      <c r="F101" s="117"/>
+      <c r="F101" s="148"/>
       <c r="G101" s="32"/>
       <c r="H101" s="75"/>
       <c r="J101" s="75"/>
@@ -6478,12 +6499,12 @@
       <c r="Y101" s="9"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="100"/>
+      <c r="A102" s="132"/>
       <c r="B102" s="6"/>
       <c r="C102" s="70"/>
       <c r="D102" s="71"/>
-      <c r="E102" s="108"/>
-      <c r="F102" s="101"/>
+      <c r="E102" s="115"/>
+      <c r="F102" s="116"/>
       <c r="G102" s="32"/>
       <c r="H102" s="75"/>
       <c r="J102" s="75"/>
@@ -6557,7 +6578,7 @@
       <c r="Y104" s="9"/>
     </row>
     <row r="105" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="131" t="s">
+      <c r="A105" s="127" t="s">
         <v>65</v>
       </c>
       <c r="B105" s="12"/>
@@ -6571,10 +6592,10 @@
         <v>351</v>
       </c>
       <c r="F105" s="88" t="s">
-        <v>524</v>
-      </c>
-      <c r="G105" s="155" t="s">
-        <v>537</v>
+        <v>522</v>
+      </c>
+      <c r="G105" s="109" t="s">
+        <v>534</v>
       </c>
       <c r="H105" s="34" t="s">
         <v>66</v>
@@ -6602,7 +6623,7 @@
       <c r="Y105" s="9"/>
     </row>
     <row r="106" spans="1:27" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="103"/>
+      <c r="A106" s="122"/>
       <c r="C106" s="15" t="s">
         <v>345</v>
       </c>
@@ -6615,12 +6636,12 @@
       <c r="F106" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G106" s="156" t="s">
-        <v>576</v>
+      <c r="G106" s="110" t="s">
+        <v>573</v>
       </c>
       <c r="H106" s="34"/>
       <c r="I106" s="23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J106" s="69" t="s">
         <v>68</v>
@@ -6642,7 +6663,7 @@
       <c r="Y106" s="9"/>
     </row>
     <row r="107" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="103"/>
+      <c r="A107" s="122"/>
       <c r="C107" s="69" t="s">
         <v>346</v>
       </c>
@@ -6656,10 +6677,10 @@
         <v>50</v>
       </c>
       <c r="G107" s="97" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I107" s="15" t="s">
         <v>35</v>
@@ -6684,7 +6705,7 @@
       <c r="Y107" s="9"/>
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="103"/>
+      <c r="A108" s="122"/>
       <c r="C108" s="2" t="s">
         <v>347</v>
       </c>
@@ -6697,14 +6718,14 @@
       <c r="F108" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G108" s="104" t="s">
-        <v>424</v>
+      <c r="G108" s="140" t="s">
+        <v>423</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>409</v>
       </c>
       <c r="I108" s="92" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="J108" s="69" t="s">
         <v>38</v>
@@ -6726,14 +6747,14 @@
       <c r="Y108" s="9"/>
     </row>
     <row r="109" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="103"/>
-      <c r="D109" s="141" t="s">
+      <c r="A109" s="122"/>
+      <c r="D109" s="98" t="s">
         <v>303</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="G109" s="105"/>
+        <v>446</v>
+      </c>
+      <c r="G109" s="141"/>
       <c r="H109" s="2" t="s">
         <v>410</v>
       </c>
@@ -6760,8 +6781,8 @@
       <c r="Y109" s="9"/>
     </row>
     <row r="110" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="103"/>
-      <c r="D110" s="141" t="s">
+      <c r="A110" s="122"/>
+      <c r="D110" s="98" t="s">
         <v>349</v>
       </c>
       <c r="E110" s="2" t="s">
@@ -6770,7 +6791,7 @@
       <c r="F110" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G110" s="105"/>
+      <c r="G110" s="141"/>
       <c r="I110" s="69"/>
       <c r="J110" s="69"/>
       <c r="K110" s="16"/>
@@ -6792,14 +6813,14 @@
       <c r="AA110" s="17"/>
     </row>
     <row r="111" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="103"/>
-      <c r="D111" s="141" t="s">
-        <v>446</v>
+      <c r="A111" s="122"/>
+      <c r="D111" s="98" t="s">
+        <v>445</v>
       </c>
       <c r="F111" s="69" t="s">
-        <v>539</v>
-      </c>
-      <c r="G111" s="105"/>
+        <v>536</v>
+      </c>
+      <c r="G111" s="141"/>
       <c r="H111" s="36"/>
       <c r="I111" s="4" t="s">
         <v>233</v>
@@ -6824,11 +6845,11 @@
       <c r="AA111" s="17"/>
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="103"/>
+      <c r="A112" s="122"/>
       <c r="D112" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="G112" s="105"/>
+      <c r="G112" s="141"/>
       <c r="H112" s="36"/>
       <c r="J112" s="2"/>
       <c r="K112" s="16"/>
@@ -6850,12 +6871,12 @@
       <c r="AA112" s="17"/>
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="103"/>
+      <c r="A113" s="122"/>
       <c r="C113" s="69"/>
       <c r="E113" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="G113" s="105"/>
+      <c r="G113" s="141"/>
       <c r="H113" s="34"/>
       <c r="J113" s="2"/>
       <c r="K113" s="16"/>
@@ -6877,11 +6898,11 @@
       <c r="AA113" s="17"/>
     </row>
     <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="103"/>
+      <c r="A114" s="122"/>
       <c r="E114" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="G114" s="105"/>
+        <v>547</v>
+      </c>
+      <c r="G114" s="141"/>
       <c r="H114" s="36"/>
       <c r="K114" s="16"/>
       <c r="L114" s="16"/>
@@ -6902,15 +6923,15 @@
       <c r="AA114" s="17"/>
     </row>
     <row r="115" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="103"/>
+      <c r="A115" s="122"/>
       <c r="D115" s="69"/>
       <c r="E115" s="4" t="s">
         <v>400</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="G115" s="105"/>
+        <v>438</v>
+      </c>
+      <c r="G115" s="141"/>
       <c r="H115" s="36"/>
       <c r="J115" s="69"/>
       <c r="K115" s="16"/>
@@ -6932,11 +6953,11 @@
       <c r="AA115" s="17"/>
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="103"/>
+      <c r="A116" s="122"/>
       <c r="E116" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="G116" s="105"/>
+        <v>548</v>
+      </c>
+      <c r="G116" s="141"/>
       <c r="H116" s="69" t="s">
         <v>32</v>
       </c>
@@ -6959,22 +6980,22 @@
       <c r="AA116" s="17"/>
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="103"/>
+      <c r="A117" s="122"/>
       <c r="B117" s="6"/>
-      <c r="C117" s="108"/>
-      <c r="D117" s="101"/>
-      <c r="E117" s="108" t="s">
+      <c r="C117" s="115"/>
+      <c r="D117" s="116"/>
+      <c r="E117" s="115" t="s">
         <v>208</v>
       </c>
-      <c r="F117" s="101"/>
-      <c r="G117" s="105"/>
+      <c r="F117" s="116"/>
+      <c r="G117" s="141"/>
       <c r="H117" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I117" s="108" t="s">
+      <c r="I117" s="115" t="s">
         <v>194</v>
       </c>
-      <c r="J117" s="101"/>
+      <c r="J117" s="116"/>
       <c r="K117" s="16"/>
       <c r="L117" s="16"/>
       <c r="M117" s="16"/>
@@ -6994,15 +7015,15 @@
       <c r="AA117" s="17"/>
     </row>
     <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="103"/>
+      <c r="A118" s="122"/>
       <c r="C118" s="85" t="s">
-        <v>521</v>
-      </c>
-      <c r="G118" s="105"/>
-      <c r="H118" s="115" t="s">
-        <v>459</v>
-      </c>
-      <c r="I118" s="116"/>
+        <v>519</v>
+      </c>
+      <c r="G118" s="141"/>
+      <c r="H118" s="145" t="s">
+        <v>458</v>
+      </c>
+      <c r="I118" s="146"/>
       <c r="K118" s="16"/>
       <c r="L118" s="16"/>
       <c r="M118" s="16"/>
@@ -7022,21 +7043,21 @@
       <c r="AA118" s="17"/>
     </row>
     <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="103"/>
+      <c r="A119" s="122"/>
       <c r="B119" s="6"/>
-      <c r="C119" s="108" t="s">
-        <v>458</v>
-      </c>
-      <c r="D119" s="101"/>
-      <c r="E119" s="108" t="s">
+      <c r="C119" s="115" t="s">
+        <v>457</v>
+      </c>
+      <c r="D119" s="116"/>
+      <c r="E119" s="115" t="s">
         <v>222</v>
       </c>
-      <c r="F119" s="101"/>
-      <c r="G119" s="105"/>
-      <c r="I119" s="108" t="s">
+      <c r="F119" s="116"/>
+      <c r="G119" s="141"/>
+      <c r="I119" s="115" t="s">
         <v>195</v>
       </c>
-      <c r="J119" s="101"/>
+      <c r="J119" s="116"/>
       <c r="K119" s="16"/>
       <c r="L119" s="16"/>
       <c r="M119" s="16"/>
@@ -7056,22 +7077,22 @@
       <c r="AA119" s="17"/>
     </row>
     <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="103"/>
+      <c r="A120" s="122"/>
       <c r="B120" s="6"/>
-      <c r="C120" s="108" t="s">
-        <v>464</v>
-      </c>
-      <c r="D120" s="101"/>
-      <c r="E120" s="113" t="s">
+      <c r="C120" s="115" t="s">
+        <v>463</v>
+      </c>
+      <c r="D120" s="116"/>
+      <c r="E120" s="133" t="s">
         <v>414</v>
       </c>
-      <c r="F120" s="114"/>
+      <c r="F120" s="134"/>
       <c r="G120" s="35"/>
       <c r="H120" s="36"/>
-      <c r="I120" s="108" t="s">
+      <c r="I120" s="115" t="s">
         <v>212</v>
       </c>
-      <c r="J120" s="101"/>
+      <c r="J120" s="116"/>
       <c r="K120" s="16"/>
       <c r="L120" s="16"/>
       <c r="M120" s="16"/>
@@ -7091,22 +7112,22 @@
       <c r="AA120" s="17"/>
     </row>
     <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="103"/>
+      <c r="A121" s="122"/>
       <c r="B121" s="6"/>
-      <c r="C121" s="108" t="s">
-        <v>460</v>
-      </c>
-      <c r="D121" s="101"/>
-      <c r="E121" s="106" t="s">
-        <v>536</v>
-      </c>
-      <c r="F121" s="107"/>
+      <c r="C121" s="115" t="s">
+        <v>459</v>
+      </c>
+      <c r="D121" s="116"/>
+      <c r="E121" s="161" t="s">
+        <v>577</v>
+      </c>
+      <c r="F121" s="151"/>
       <c r="G121" s="35"/>
       <c r="H121" s="36"/>
-      <c r="I121" s="108" t="s">
+      <c r="I121" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="J121" s="101"/>
+      <c r="J121" s="116"/>
       <c r="K121" s="16"/>
       <c r="L121" s="16"/>
       <c r="M121" s="16"/>
@@ -7126,16 +7147,16 @@
       <c r="AA121" s="17"/>
     </row>
     <row r="122" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="103"/>
+      <c r="A122" s="122"/>
       <c r="B122" s="6"/>
-      <c r="C122" s="108" t="s">
+      <c r="C122" s="115" t="s">
         <v>202</v>
       </c>
-      <c r="D122" s="101"/>
-      <c r="E122" s="108" t="s">
-        <v>432</v>
-      </c>
-      <c r="F122" s="101"/>
+      <c r="D122" s="116"/>
+      <c r="E122" s="115" t="s">
+        <v>431</v>
+      </c>
+      <c r="F122" s="116"/>
       <c r="G122" s="35"/>
       <c r="H122" s="36"/>
       <c r="K122" s="16"/>
@@ -7157,20 +7178,20 @@
       <c r="AA122" s="17"/>
     </row>
     <row r="123" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="103"/>
+      <c r="A123" s="122"/>
       <c r="B123" s="6"/>
-      <c r="C123" s="108" t="s">
+      <c r="C123" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="D123" s="101"/>
-      <c r="E123" s="117" t="s">
-        <v>466</v>
-      </c>
-      <c r="F123" s="103"/>
+      <c r="D123" s="116"/>
+      <c r="E123" s="148" t="s">
+        <v>465</v>
+      </c>
+      <c r="F123" s="122"/>
       <c r="G123" s="35"/>
       <c r="H123" s="36"/>
-      <c r="I123" s="106"/>
-      <c r="J123" s="107"/>
+      <c r="I123" s="119"/>
+      <c r="J123" s="120"/>
       <c r="K123" s="16"/>
       <c r="L123" s="16"/>
       <c r="M123" s="16"/>
@@ -7190,20 +7211,20 @@
       <c r="AA123" s="17"/>
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="103"/>
+      <c r="A124" s="122"/>
       <c r="B124" s="6"/>
-      <c r="C124" s="139" t="s">
-        <v>573</v>
-      </c>
-      <c r="D124" s="119"/>
+      <c r="C124" s="150" t="s">
+        <v>570</v>
+      </c>
+      <c r="D124" s="151"/>
       <c r="G124" s="35"/>
-      <c r="H124" s="144" t="s">
-        <v>427</v>
-      </c>
-      <c r="I124" s="139" t="s">
-        <v>574</v>
-      </c>
-      <c r="J124" s="116"/>
+      <c r="H124" s="101" t="s">
+        <v>426</v>
+      </c>
+      <c r="I124" s="150" t="s">
+        <v>571</v>
+      </c>
+      <c r="J124" s="146"/>
       <c r="K124" s="16"/>
       <c r="L124" s="16"/>
       <c r="M124" s="16"/>
@@ -7223,16 +7244,16 @@
       <c r="AA124" s="17"/>
     </row>
     <row r="125" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="103"/>
+      <c r="A125" s="122"/>
       <c r="B125" s="6"/>
-      <c r="C125" s="108"/>
-      <c r="D125" s="101"/>
+      <c r="C125" s="115"/>
+      <c r="D125" s="116"/>
       <c r="G125" s="35"/>
       <c r="H125" s="73"/>
-      <c r="I125" s="140" t="s">
-        <v>486</v>
-      </c>
-      <c r="J125" s="123"/>
+      <c r="I125" s="154" t="s">
+        <v>485</v>
+      </c>
+      <c r="J125" s="144"/>
       <c r="K125" s="16"/>
       <c r="L125" s="16"/>
       <c r="M125" s="16"/>
@@ -7252,10 +7273,10 @@
       <c r="AA125" s="17"/>
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="103"/>
+      <c r="A126" s="122"/>
       <c r="B126" s="6"/>
-      <c r="C126" s="108"/>
-      <c r="D126" s="101"/>
+      <c r="C126" s="115"/>
+      <c r="D126" s="116"/>
       <c r="G126" s="35"/>
       <c r="H126" s="36"/>
       <c r="K126" s="16"/>
@@ -7277,7 +7298,7 @@
       <c r="AA126" s="17"/>
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="103"/>
+      <c r="A127" s="122"/>
       <c r="B127" s="6"/>
       <c r="C127" s="70"/>
       <c r="D127" s="71"/>
@@ -7355,7 +7376,7 @@
       <c r="Y129" s="9"/>
     </row>
     <row r="130" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="98" t="s">
+      <c r="A130" s="130" t="s">
         <v>73</v>
       </c>
       <c r="B130" s="74"/>
@@ -7392,7 +7413,7 @@
       <c r="Y130" s="9"/>
     </row>
     <row r="131" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="99"/>
+      <c r="A131" s="131"/>
       <c r="C131" s="23" t="s">
         <v>309</v>
       </c>
@@ -7403,8 +7424,8 @@
         <v>67</v>
       </c>
       <c r="H131" s="11"/>
-      <c r="I131" s="127"/>
-      <c r="J131" s="103"/>
+      <c r="I131" s="149"/>
+      <c r="J131" s="122"/>
       <c r="K131" s="9"/>
       <c r="L131" s="9"/>
       <c r="M131" s="9"/>
@@ -7422,15 +7443,15 @@
       <c r="Y131" s="9"/>
     </row>
     <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="99"/>
+      <c r="A132" s="131"/>
       <c r="C132" s="23" t="s">
         <v>310</v>
       </c>
       <c r="D132" s="79" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F132" s="88" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H132" s="11"/>
       <c r="I132" s="41"/>
@@ -7452,7 +7473,7 @@
       <c r="Y132" s="9"/>
     </row>
     <row r="133" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="99"/>
+      <c r="A133" s="131"/>
       <c r="C133" s="23" t="s">
         <v>311</v>
       </c>
@@ -7482,9 +7503,9 @@
       <c r="Y133" s="9"/>
     </row>
     <row r="134" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="99"/>
+      <c r="A134" s="131"/>
       <c r="C134" s="15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>312</v>
@@ -7512,7 +7533,7 @@
       <c r="Y134" s="9"/>
     </row>
     <row r="135" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="99"/>
+      <c r="A135" s="131"/>
       <c r="C135" s="23" t="s">
         <v>264</v>
       </c>
@@ -7541,15 +7562,15 @@
       <c r="Y135" s="9"/>
     </row>
     <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="99"/>
+      <c r="A136" s="131"/>
       <c r="C136" s="4" t="s">
         <v>408</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E136" s="141" t="s">
-        <v>478</v>
+      <c r="E136" s="98" t="s">
+        <v>477</v>
       </c>
       <c r="G136" s="2"/>
       <c r="I136" s="43"/>
@@ -7571,14 +7592,14 @@
       <c r="Y136" s="9"/>
     </row>
     <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="99"/>
-      <c r="C137" s="124" t="s">
-        <v>543</v>
+      <c r="A137" s="131"/>
+      <c r="C137" s="121" t="s">
+        <v>540</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E137" s="142" t="s">
+      <c r="E137" s="99" t="s">
         <v>401</v>
       </c>
       <c r="G137" s="2"/>
@@ -7601,15 +7622,15 @@
       <c r="Y137" s="9"/>
     </row>
     <row r="138" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="99"/>
-      <c r="C138" s="103"/>
+      <c r="A138" s="131"/>
+      <c r="C138" s="122"/>
       <c r="D138" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E138" s="108" t="s">
+      <c r="E138" s="115" t="s">
         <v>201</v>
       </c>
-      <c r="F138" s="101"/>
+      <c r="F138" s="116"/>
       <c r="G138" s="2"/>
       <c r="H138" s="43"/>
       <c r="I138" s="43"/>
@@ -7631,14 +7652,14 @@
       <c r="Y138" s="9"/>
     </row>
     <row r="139" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="99"/>
+      <c r="A139" s="131"/>
       <c r="C139" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="F139" s="126" t="s">
-        <v>492</v>
-      </c>
-      <c r="G139" s="103"/>
+      <c r="F139" s="125" t="s">
+        <v>490</v>
+      </c>
+      <c r="G139" s="122"/>
       <c r="H139" s="43"/>
       <c r="I139" s="43"/>
       <c r="J139" s="11"/>
@@ -7659,14 +7680,14 @@
       <c r="Y139" s="9"/>
     </row>
     <row r="140" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="99"/>
+      <c r="A140" s="131"/>
       <c r="C140" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="F140" s="118" t="s">
+      <c r="F140" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="G140" s="103"/>
+      <c r="G140" s="122"/>
       <c r="H140" s="43"/>
       <c r="I140" s="43"/>
       <c r="J140" s="11"/>
@@ -7687,15 +7708,15 @@
       <c r="Y140" s="9"/>
     </row>
     <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="99"/>
-      <c r="C141" s="150" t="s">
+      <c r="A141" s="131"/>
+      <c r="C141" s="107" t="s">
         <v>404</v>
       </c>
       <c r="E141" s="61"/>
-      <c r="F141" s="118" t="s">
+      <c r="F141" s="126" t="s">
         <v>79</v>
       </c>
-      <c r="G141" s="103"/>
+      <c r="G141" s="122"/>
       <c r="H141" s="43"/>
       <c r="I141" s="43"/>
       <c r="J141" s="11"/>
@@ -7716,9 +7737,9 @@
       <c r="Y141" s="9"/>
     </row>
     <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="99"/>
+      <c r="A142" s="131"/>
       <c r="E142" s="85" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G142" s="35"/>
       <c r="H142" s="43"/>
@@ -7741,12 +7762,12 @@
       <c r="Y142" s="9"/>
     </row>
     <row r="143" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="99"/>
+      <c r="A143" s="131"/>
       <c r="C143" s="2"/>
-      <c r="D143" s="108" t="s">
+      <c r="D143" s="115" t="s">
         <v>209</v>
       </c>
-      <c r="E143" s="101"/>
+      <c r="E143" s="116"/>
       <c r="H143" s="43"/>
       <c r="I143" s="43"/>
       <c r="J143" s="11"/>
@@ -7767,16 +7788,16 @@
       <c r="Y143" s="9"/>
     </row>
     <row r="144" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="99"/>
+      <c r="A144" s="131"/>
       <c r="C144" s="2"/>
-      <c r="D144" s="108" t="s">
+      <c r="D144" s="115" t="s">
         <v>196</v>
       </c>
-      <c r="E144" s="101"/>
-      <c r="F144" s="113" t="s">
+      <c r="E144" s="116"/>
+      <c r="F144" s="133" t="s">
         <v>248</v>
       </c>
-      <c r="G144" s="114"/>
+      <c r="G144" s="134"/>
       <c r="H144" s="43"/>
       <c r="I144" s="43"/>
       <c r="J144" s="11"/>
@@ -7797,16 +7818,16 @@
       <c r="Y144" s="9"/>
     </row>
     <row r="145" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="99"/>
+      <c r="A145" s="131"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="120" t="s">
+      <c r="D145" s="152" t="s">
         <v>197</v>
       </c>
-      <c r="E145" s="121"/>
-      <c r="F145" s="113" t="s">
-        <v>417</v>
-      </c>
-      <c r="G145" s="114"/>
+      <c r="E145" s="153"/>
+      <c r="F145" s="159" t="s">
+        <v>576</v>
+      </c>
+      <c r="G145" s="160"/>
       <c r="H145" s="43"/>
       <c r="I145" s="43"/>
       <c r="J145" s="11"/>
@@ -7827,16 +7848,16 @@
       <c r="Y145" s="9"/>
     </row>
     <row r="146" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="99"/>
+      <c r="A146" s="131"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="108" t="s">
+      <c r="D146" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="E146" s="101"/>
-      <c r="F146" s="137" t="s">
-        <v>488</v>
-      </c>
-      <c r="G146" s="138"/>
+      <c r="E146" s="116"/>
+      <c r="F146" s="135" t="s">
+        <v>486</v>
+      </c>
+      <c r="G146" s="136"/>
       <c r="H146" s="43"/>
       <c r="I146" s="43"/>
       <c r="J146" s="11"/>
@@ -7857,12 +7878,12 @@
       <c r="Y146" s="9"/>
     </row>
     <row r="147" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="99"/>
+      <c r="A147" s="131"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="108" t="s">
+      <c r="D147" s="115" t="s">
         <v>220</v>
       </c>
-      <c r="E147" s="101"/>
+      <c r="E147" s="116"/>
       <c r="H147" s="43"/>
       <c r="I147" s="43"/>
       <c r="J147" s="11"/>
@@ -7883,12 +7904,12 @@
       <c r="Y147" s="9"/>
     </row>
     <row r="148" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="99"/>
+      <c r="A148" s="131"/>
       <c r="C148" s="2"/>
-      <c r="D148" s="106" t="s">
-        <v>487</v>
-      </c>
-      <c r="E148" s="107"/>
+      <c r="D148" s="162" t="s">
+        <v>578</v>
+      </c>
+      <c r="E148" s="163"/>
       <c r="H148" s="43"/>
       <c r="I148" s="43"/>
       <c r="J148" s="11"/>
@@ -7909,12 +7930,12 @@
       <c r="Y148" s="9"/>
     </row>
     <row r="149" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="99"/>
+      <c r="A149" s="131"/>
       <c r="C149" s="2"/>
-      <c r="D149" s="126" t="s">
-        <v>555</v>
-      </c>
-      <c r="E149" s="103"/>
+      <c r="D149" s="125" t="s">
+        <v>552</v>
+      </c>
+      <c r="E149" s="122"/>
       <c r="F149" s="2"/>
       <c r="G149" s="35"/>
       <c r="H149" s="11"/>
@@ -7937,12 +7958,12 @@
       <c r="Y149" s="9"/>
     </row>
     <row r="150" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="99"/>
+      <c r="A150" s="131"/>
       <c r="C150" s="2"/>
-      <c r="D150" s="126" t="s">
-        <v>554</v>
-      </c>
-      <c r="E150" s="103"/>
+      <c r="D150" s="125" t="s">
+        <v>551</v>
+      </c>
+      <c r="E150" s="122"/>
       <c r="F150" s="2"/>
       <c r="G150" s="32"/>
       <c r="H150" s="11"/>
@@ -7965,12 +7986,12 @@
       <c r="Y150" s="9"/>
     </row>
     <row r="151" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="99"/>
+      <c r="A151" s="131"/>
       <c r="C151" s="2"/>
-      <c r="D151" s="126" t="s">
+      <c r="D151" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E151" s="103"/>
+      <c r="E151" s="122"/>
       <c r="F151" s="2"/>
       <c r="G151" s="32"/>
       <c r="H151" s="11"/>
@@ -7993,12 +8014,12 @@
       <c r="Y151" s="9"/>
     </row>
     <row r="152" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="100"/>
+      <c r="A152" s="132"/>
       <c r="C152" s="2"/>
-      <c r="E152" s="108" t="s">
-        <v>513</v>
-      </c>
-      <c r="F152" s="101"/>
+      <c r="E152" s="115" t="s">
+        <v>511</v>
+      </c>
+      <c r="F152" s="116"/>
       <c r="G152" s="32"/>
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
@@ -8185,10 +8206,10 @@
     <row r="158" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="9"/>
       <c r="B158" s="9"/>
-      <c r="C158" s="151" t="s">
+      <c r="C158" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="D158" s="151" t="s">
+      <c r="D158" s="108" t="s">
         <v>89</v>
       </c>
       <c r="E158" s="53" t="s">
@@ -8492,7 +8513,7 @@
         <v>148</v>
       </c>
       <c r="H166" s="59" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I166" s="59" t="s">
         <v>149</v>
@@ -8832,10 +8853,10 @@
       </c>
       <c r="F175" s="13"/>
       <c r="G175" s="58" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H175" s="58" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I175" s="58" t="s">
         <v>173</v>
@@ -8865,10 +8886,10 @@
       <c r="E176" s="13"/>
       <c r="F176" s="13"/>
       <c r="G176" s="58" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H176" s="58" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I176" s="58" t="s">
         <v>174</v>
@@ -9307,7 +9328,7 @@
       <c r="C192" s="58"/>
       <c r="D192" s="58"/>
       <c r="E192" s="58"/>
-      <c r="F192" s="125"/>
+      <c r="F192" s="147"/>
       <c r="J192" s="13"/>
       <c r="K192" s="9"/>
       <c r="L192" s="9"/>
@@ -9331,7 +9352,7 @@
       <c r="C193" s="58"/>
       <c r="D193" s="58"/>
       <c r="E193" s="58"/>
-      <c r="F193" s="103"/>
+      <c r="F193" s="122"/>
       <c r="J193" s="13"/>
       <c r="K193" s="9"/>
       <c r="L193" s="9"/>
@@ -9382,7 +9403,7 @@
       <c r="C195" s="58"/>
       <c r="D195" s="58"/>
       <c r="E195" s="58"/>
-      <c r="F195" s="125"/>
+      <c r="F195" s="147"/>
       <c r="G195" s="9"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
@@ -9409,7 +9430,7 @@
       <c r="C196" s="58"/>
       <c r="D196" s="58"/>
       <c r="E196" s="58"/>
-      <c r="F196" s="103"/>
+      <c r="F196" s="122"/>
       <c r="G196" s="9"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
@@ -12983,6 +13004,113 @@
     <row r="1060" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="A130:A152"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="G78:G88"/>
+    <mergeCell ref="G37:G55"/>
+    <mergeCell ref="G57:G68"/>
+    <mergeCell ref="I123:J123"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="I124:J124"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G108:G119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="E138:F138"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="I97:J97"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="I125:J125"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="F192:F193"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="F139:G139"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="I131:J131"/>
+    <mergeCell ref="I120:J120"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="I117:J117"/>
+    <mergeCell ref="I119:J119"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A3:A28"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G5:G28"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="A30:A52"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I49:J49"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="E152:F152"/>
     <mergeCell ref="A54:A76"/>
@@ -13007,113 +13135,6 @@
     <mergeCell ref="C123:D123"/>
     <mergeCell ref="E119:F119"/>
     <mergeCell ref="F145:G145"/>
-    <mergeCell ref="F146:G146"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:A28"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G5:G28"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A30:A52"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="F192:F193"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="F139:G139"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="I131:J131"/>
-    <mergeCell ref="I120:J120"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="I117:J117"/>
-    <mergeCell ref="I119:J119"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="I124:J124"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="F141:G141"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="G108:G119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="E138:F138"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="I97:J97"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="H118:I118"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="I125:J125"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A130:A152"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="G78:G88"/>
-    <mergeCell ref="G37:G55"/>
-    <mergeCell ref="G57:G68"/>
-    <mergeCell ref="I123:J123"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="I95:J95"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="E76:F76"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
update: add btech-62-sem2/4 tt
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 62 (btech-62)/4/1.xlsx
+++ b/raw/time_tables/B.Tech 62 (btech-62)/4/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\TT_27 jan\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fileserver2\time table\JIIT Time Table EVEN 2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13067FA-8708-4617-90FC-E59BC59324A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDEA5A-07E4-4219-BF81-1D59F9A2AAF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IV" sheetId="1" r:id="rId1"/>
@@ -1156,9 +1156,6 @@
     <t>LA5,A6(15B11EC611))-G4/RRP</t>
   </si>
   <si>
-    <t>LB14,B16 (CS221)-G7/TKT</t>
-  </si>
-  <si>
     <t>LC1-C3(BT411)-G8/NDH, RD</t>
   </si>
   <si>
@@ -1552,9 +1549,6 @@
     <t>PB9,B10(CS224)-CL19,20/ATI,PRK,AMT</t>
   </si>
   <si>
-    <t>PB14,B16(CS222)-CL10,11/PU,DL,SOS</t>
-  </si>
-  <si>
     <t>LG1,G2 (CS222)-G8/AKM</t>
   </si>
   <si>
@@ -1562,9 +1556,6 @@
   </si>
   <si>
     <t>PB3,B4(CS224)-CL09,10/DEP,ALK,SLK</t>
-  </si>
-  <si>
-    <t>PG1,G2(CS221)-CL10,11/VRN,SHV,DL,RJM</t>
   </si>
   <si>
     <t>PB(25B16CS213)-CL17,18/HN,VIK</t>
@@ -2057,9 +2048,6 @@
     <t>PB1,B2(CS224)-CL02,03/SLK,ATI,SHG</t>
   </si>
   <si>
-    <t>PB5,B6(CS222)-CL05,06/SYN,NIY</t>
-  </si>
-  <si>
     <t>PB14(CS224)-CL14/AKM,ATI</t>
   </si>
   <si>
@@ -2067,9 +2055,6 @@
   </si>
   <si>
     <t>PB1,B2,B4(CS221)-CL10,11,12/AST,TRN,TAJ,RJM,KJ</t>
-  </si>
-  <si>
-    <t>PB3,B14(CS221)-CL02,03/TRN,KJ,MKT</t>
   </si>
   <si>
     <t>PMinor(24B15CS245)-CL01/NET</t>
@@ -2110,6 +2095,21 @@
   </si>
   <si>
     <t>PB8(CS221)-CL02/VRN,KJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>PB5,B6(CS222)-CL05,06/SYN,NIY,PU</t>
+  </si>
+  <si>
+    <t>PB14(CS222)-CL10,11/DL,SOS</t>
+  </si>
+  <si>
+    <t>PG1,G2(CS221)-CL10,11/VRN,SHV,DL</t>
+  </si>
+  <si>
+    <t>PB3,B14(CS221)-CL02,03/TRN,KJ,,RJM,MKT</t>
   </si>
 </sst>
 </file>
@@ -2443,7 +2443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2765,10 +2765,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2811,6 +2811,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2862,18 +2868,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -2882,21 +2903,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3120,10 +3126,10 @@
   <dimension ref="A1:AA1060"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B135" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D148" sqref="D148:E148"/>
+      <selection pane="bottomRight" activeCell="I124" sqref="I124:J124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3144,17 +3150,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
       <c r="J1" s="134"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
@@ -3174,7 +3180,7 @@
     </row>
     <row r="2" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>1</v>
@@ -3229,7 +3235,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="96" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="I3" s="69" t="s">
         <v>15</v>
@@ -3256,22 +3262,22 @@
     <row r="4" spans="1:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="122"/>
       <c r="C4" s="77" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F4" s="121" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I4" s="69" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K4" s="71"/>
       <c r="L4" s="9"/>
@@ -3292,7 +3298,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="122"/>
       <c r="C5" s="93" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>318</v>
@@ -3301,8 +3307,8 @@
         <v>247</v>
       </c>
       <c r="F5" s="122"/>
-      <c r="G5" s="140" t="s">
-        <v>423</v>
+      <c r="G5" s="142" t="s">
+        <v>422</v>
       </c>
       <c r="H5" s="94" t="s">
         <v>323</v>
@@ -3311,7 +3317,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -3332,10 +3338,10 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="122"/>
       <c r="C6" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>321</v>
@@ -3343,7 +3349,7 @@
       <c r="F6" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="141"/>
+      <c r="G6" s="143"/>
       <c r="H6" s="2" t="s">
         <v>262</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>25</v>
@@ -3380,7 +3386,7 @@
       <c r="F7" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="141"/>
+      <c r="G7" s="143"/>
       <c r="H7" s="2" t="s">
         <v>263</v>
       </c>
@@ -3410,15 +3416,15 @@
         <v>229</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E8" s="98" t="s">
         <v>253</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>509</v>
-      </c>
-      <c r="G8" s="141"/>
+        <v>506</v>
+      </c>
+      <c r="G8" s="143"/>
       <c r="H8" s="2" t="s">
         <v>264</v>
       </c>
@@ -3452,7 +3458,7 @@
       <c r="F9" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="G9" s="141"/>
+      <c r="G9" s="143"/>
       <c r="H9" s="2" t="s">
         <v>265</v>
       </c>
@@ -3484,7 +3490,7 @@
       <c r="F10" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="G10" s="141"/>
+      <c r="G10" s="143"/>
       <c r="H10" s="2" t="s">
         <v>325</v>
       </c>
@@ -3515,9 +3521,9 @@
         <v>256</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="G11" s="141"/>
+        <v>411</v>
+      </c>
+      <c r="G11" s="143"/>
       <c r="H11" s="69"/>
       <c r="K11" s="9"/>
       <c r="L11" s="16"/>
@@ -3544,14 +3550,14 @@
         <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="G12" s="141"/>
+        <v>414</v>
+      </c>
+      <c r="G12" s="143"/>
       <c r="H12" s="4" t="s">
         <v>236</v>
       </c>
       <c r="I12" s="99" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J12" s="69"/>
       <c r="K12" s="9"/>
@@ -3575,20 +3581,20 @@
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="122"/>
       <c r="C13" s="67" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E13" s="69" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="86" t="s">
-        <v>487</v>
-      </c>
-      <c r="G13" s="141"/>
+        <v>484</v>
+      </c>
+      <c r="G13" s="143"/>
       <c r="H13" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J13" s="69"/>
       <c r="K13" s="9"/>
@@ -3612,20 +3618,20 @@
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="122"/>
       <c r="C14" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E14" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="141"/>
+      <c r="G14" s="143"/>
       <c r="H14" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I14" s="125" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="J14" s="122"/>
       <c r="K14" s="9"/>
@@ -3657,12 +3663,12 @@
       <c r="F15" s="69" t="s">
         <v>259</v>
       </c>
-      <c r="G15" s="141"/>
+      <c r="G15" s="143"/>
       <c r="H15" s="85" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I15" s="125" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="J15" s="122"/>
       <c r="K15" s="9"/>
@@ -3687,12 +3693,12 @@
       <c r="A16" s="122"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F16" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="G16" s="141"/>
+      <c r="G16" s="143"/>
       <c r="I16" s="125" t="s">
         <v>27</v>
       </c>
@@ -3719,12 +3725,12 @@
       <c r="A17" s="122"/>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E17" s="96" t="s">
-        <v>574</v>
-      </c>
-      <c r="G17" s="141"/>
+        <v>569</v>
+      </c>
+      <c r="G17" s="143"/>
       <c r="H17" s="72"/>
       <c r="I17" s="115" t="s">
         <v>343</v>
@@ -3751,7 +3757,7 @@
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="122"/>
       <c r="C18" s="4"/>
-      <c r="G18" s="141"/>
+      <c r="G18" s="143"/>
       <c r="I18" s="115" t="s">
         <v>187</v>
       </c>
@@ -3778,10 +3784,10 @@
       <c r="A19" s="122"/>
       <c r="C19" s="4"/>
       <c r="E19" s="100" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F19" s="69"/>
-      <c r="G19" s="141"/>
+      <c r="G19" s="143"/>
       <c r="I19" s="115" t="s">
         <v>213</v>
       </c>
@@ -3813,7 +3819,7 @@
       <c r="F20" s="69" t="s">
         <v>257</v>
       </c>
-      <c r="G20" s="141"/>
+      <c r="G20" s="143"/>
       <c r="I20" s="115" t="s">
         <v>206</v>
       </c>
@@ -3843,9 +3849,9 @@
         <v>235</v>
       </c>
       <c r="F21" s="69" t="s">
-        <v>555</v>
-      </c>
-      <c r="G21" s="141"/>
+        <v>552</v>
+      </c>
+      <c r="G21" s="143"/>
       <c r="H21" s="115" t="s">
         <v>200</v>
       </c>
@@ -3875,7 +3881,7 @@
         <v>239</v>
       </c>
       <c r="F22" s="69"/>
-      <c r="G22" s="141"/>
+      <c r="G22" s="143"/>
       <c r="H22" s="72"/>
       <c r="I22" s="115" t="s">
         <v>217</v>
@@ -3906,7 +3912,7 @@
         <v>245</v>
       </c>
       <c r="F23" s="69"/>
-      <c r="G23" s="141"/>
+      <c r="G23" s="143"/>
       <c r="H23" s="72"/>
       <c r="I23" s="115" t="s">
         <v>226</v>
@@ -3933,7 +3939,7 @@
       <c r="A24" s="122"/>
       <c r="C24" s="4"/>
       <c r="F24" s="69"/>
-      <c r="G24" s="141"/>
+      <c r="G24" s="143"/>
       <c r="H24" s="72"/>
       <c r="I24" s="133"/>
       <c r="J24" s="134"/>
@@ -3958,10 +3964,10 @@
       <c r="A25" s="122"/>
       <c r="C25" s="4"/>
       <c r="F25" s="69"/>
-      <c r="G25" s="141"/>
+      <c r="G25" s="143"/>
       <c r="H25" s="72"/>
       <c r="I25" s="115" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J25" s="116"/>
       <c r="K25" s="9"/>
@@ -3985,10 +3991,10 @@
       <c r="A26" s="122"/>
       <c r="C26" s="4"/>
       <c r="F26" s="69"/>
-      <c r="G26" s="141"/>
+      <c r="G26" s="143"/>
       <c r="H26" s="72"/>
       <c r="I26" s="115" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="J26" s="116"/>
       <c r="K26" s="9"/>
@@ -4010,9 +4016,9 @@
       <c r="A27" s="122"/>
       <c r="C27" s="4"/>
       <c r="F27" s="69"/>
-      <c r="G27" s="141"/>
+      <c r="G27" s="143"/>
       <c r="H27" s="115" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="I27" s="116"/>
       <c r="K27" s="9"/>
@@ -4034,7 +4040,7 @@
       <c r="A28" s="122"/>
       <c r="C28" s="4"/>
       <c r="F28" s="69"/>
-      <c r="G28" s="142"/>
+      <c r="G28" s="144"/>
       <c r="H28" s="72"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -4118,7 +4124,7 @@
     <row r="31" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="131"/>
       <c r="C31" s="69" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D31" s="69" t="s">
         <v>32</v>
@@ -4130,7 +4136,7 @@
         <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I31" s="69" t="s">
         <v>33</v>
@@ -4166,7 +4172,7 @@
       </c>
       <c r="F32" s="122"/>
       <c r="G32" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>279</v>
@@ -4205,13 +4211,13 @@
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>334</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -4231,22 +4237,22 @@
     <row r="34" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="131"/>
       <c r="C34" s="23" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D34" s="98" t="s">
         <v>329</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F34" s="69" t="s">
         <v>332</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I34" s="98" t="s">
         <v>22</v>
@@ -4283,10 +4289,10 @@
         <v>273</v>
       </c>
       <c r="F35" s="121" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I35" s="98" t="s">
         <v>283</v>
@@ -4318,13 +4324,13 @@
       </c>
       <c r="F36" s="122"/>
       <c r="G36" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>280</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
@@ -4355,14 +4361,14 @@
       <c r="F37" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G37" s="140" t="s">
-        <v>423</v>
+      <c r="G37" s="142" t="s">
+        <v>422</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>281</v>
       </c>
       <c r="I37" s="101" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
@@ -4387,12 +4393,12 @@
         <v>39</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="G38" s="141"/>
+        <v>412</v>
+      </c>
+      <c r="G38" s="143"/>
       <c r="H38" s="1" t="s">
         <v>282</v>
       </c>
@@ -4418,17 +4424,17 @@
       <c r="A39" s="131"/>
       <c r="D39" s="69"/>
       <c r="E39" s="24" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="G39" s="141"/>
+        <v>415</v>
+      </c>
+      <c r="G39" s="143"/>
       <c r="H39" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I39" s="73" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J39" s="72" t="s">
         <v>230</v>
@@ -4454,12 +4460,12 @@
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="131"/>
       <c r="E40" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F40" s="86" t="s">
-        <v>487</v>
-      </c>
-      <c r="G40" s="141"/>
+        <v>484</v>
+      </c>
+      <c r="G40" s="143"/>
       <c r="J40" s="72" t="s">
         <v>232</v>
       </c>
@@ -4487,13 +4493,13 @@
       <c r="F41" s="69" t="s">
         <v>258</v>
       </c>
-      <c r="G41" s="141"/>
+      <c r="G41" s="143"/>
       <c r="H41" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="72" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
@@ -4516,12 +4522,12 @@
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="131"/>
       <c r="D42" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F42" s="69" t="s">
         <v>276</v>
       </c>
-      <c r="G42" s="141"/>
+      <c r="G42" s="143"/>
       <c r="H42" s="1" t="s">
         <v>333</v>
       </c>
@@ -4554,7 +4560,7 @@
       <c r="F43" s="69" t="s">
         <v>277</v>
       </c>
-      <c r="G43" s="141"/>
+      <c r="G43" s="143"/>
       <c r="J43" s="69" t="s">
         <v>278</v>
       </c>
@@ -4578,15 +4584,15 @@
       <c r="A44" s="131"/>
       <c r="B44" s="6"/>
       <c r="C44" s="113" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D44" s="114"/>
       <c r="E44" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G44" s="141"/>
+      <c r="G44" s="143"/>
       <c r="H44" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I44" s="115" t="s">
         <v>205</v>
@@ -4616,11 +4622,11 @@
       </c>
       <c r="D45" s="116"/>
       <c r="F45" s="79" t="s">
-        <v>512</v>
-      </c>
-      <c r="G45" s="141"/>
+        <v>509</v>
+      </c>
+      <c r="G45" s="143"/>
       <c r="H45" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I45" s="115" t="s">
         <v>210</v>
@@ -4646,13 +4652,13 @@
       <c r="A46" s="131"/>
       <c r="B46" s="6"/>
       <c r="C46" s="123" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D46" s="124"/>
       <c r="E46" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G46" s="141"/>
+      <c r="G46" s="143"/>
       <c r="I46" s="115" t="s">
         <v>190</v>
       </c>
@@ -4681,11 +4687,11 @@
       </c>
       <c r="D47" s="116"/>
       <c r="E47" s="99" t="s">
-        <v>387</v>
-      </c>
-      <c r="G47" s="141"/>
+        <v>386</v>
+      </c>
+      <c r="G47" s="143"/>
       <c r="I47" s="115" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="J47" s="116"/>
       <c r="K47" s="9"/>
@@ -4707,18 +4713,18 @@
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="131"/>
       <c r="C48" s="115" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D48" s="116"/>
       <c r="E48" s="99" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F48" s="69"/>
-      <c r="G48" s="141"/>
-      <c r="I48" s="145" t="s">
-        <v>566</v>
-      </c>
-      <c r="J48" s="146"/>
+      <c r="G48" s="143"/>
+      <c r="I48" s="147" t="s">
+        <v>563</v>
+      </c>
+      <c r="J48" s="148"/>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
@@ -4738,19 +4744,19 @@
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="131"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="119" t="s">
-        <v>514</v>
-      </c>
-      <c r="D49" s="120"/>
+      <c r="C49" s="157" t="s">
+        <v>511</v>
+      </c>
+      <c r="D49" s="158"/>
       <c r="E49" s="115" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F49" s="116"/>
-      <c r="G49" s="141"/>
-      <c r="I49" s="145" t="s">
-        <v>567</v>
-      </c>
-      <c r="J49" s="146"/>
+      <c r="G49" s="143"/>
+      <c r="I49" s="147" t="s">
+        <v>575</v>
+      </c>
+      <c r="J49" s="148"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
@@ -4770,15 +4776,15 @@
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="131"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="115" t="s">
-        <v>481</v>
-      </c>
-      <c r="D50" s="116"/>
+      <c r="C50" s="161" t="s">
+        <v>576</v>
+      </c>
+      <c r="D50" s="162"/>
       <c r="E50" s="69"/>
       <c r="F50" s="69"/>
-      <c r="G50" s="141"/>
+      <c r="G50" s="143"/>
       <c r="I50" s="115" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J50" s="116"/>
       <c r="K50" s="9"/>
@@ -4801,12 +4807,12 @@
       <c r="A51" s="131"/>
       <c r="B51" s="6"/>
       <c r="C51" s="112" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D51" s="111"/>
       <c r="E51" s="69"/>
       <c r="F51" s="69"/>
-      <c r="G51" s="141"/>
+      <c r="G51" s="143"/>
       <c r="I51" s="70"/>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -4832,10 +4838,10 @@
       <c r="D52" s="116"/>
       <c r="E52" s="69"/>
       <c r="F52" s="69"/>
-      <c r="G52" s="141"/>
+      <c r="G52" s="143"/>
       <c r="H52" s="25"/>
-      <c r="I52" s="143"/>
-      <c r="J52" s="144"/>
+      <c r="I52" s="145"/>
+      <c r="J52" s="146"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
@@ -4859,7 +4865,7 @@
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="141"/>
+      <c r="G53" s="143"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
@@ -4884,7 +4890,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="27"/>
-      <c r="G54" s="141"/>
+      <c r="G54" s="143"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -4903,7 +4909,7 @@
     </row>
     <row r="55" spans="1:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="118"/>
-      <c r="G55" s="141"/>
+      <c r="G55" s="143"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -4957,8 +4963,8 @@
       <c r="F57" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="140" t="s">
-        <v>423</v>
+      <c r="G57" s="142" t="s">
+        <v>422</v>
       </c>
       <c r="H57" s="28" t="s">
         <v>10</v>
@@ -4985,7 +4991,7 @@
     <row r="58" spans="1:27" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="118"/>
       <c r="C58" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D58" s="69" t="s">
         <v>49</v>
@@ -4993,9 +4999,9 @@
       <c r="E58" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G58" s="141"/>
+      <c r="G58" s="143"/>
       <c r="H58" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I58" s="69" t="s">
         <v>51</v>
@@ -5022,26 +5028,26 @@
     <row r="59" spans="1:27" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="118"/>
       <c r="C59" s="24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D59" s="98" t="s">
         <v>284</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F59" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="G59" s="141"/>
+      <c r="G59" s="143"/>
       <c r="H59" s="23" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K59" s="80"/>
       <c r="L59" s="80"/>
@@ -5064,7 +5070,7 @@
     <row r="60" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="118"/>
       <c r="C60" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D60" s="69" t="s">
         <v>32</v>
@@ -5073,15 +5079,15 @@
       <c r="F60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G60" s="141"/>
+      <c r="G60" s="143"/>
       <c r="H60" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I60" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J60" s="98" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="K60" s="80"/>
       <c r="L60" s="80"/>
@@ -5104,7 +5110,7 @@
     <row r="61" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="118"/>
       <c r="C61" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D61" s="98" t="s">
         <v>285</v>
@@ -5115,9 +5121,9 @@
       <c r="F61" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G61" s="141"/>
+      <c r="G61" s="143"/>
       <c r="H61" s="4" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="I61" s="98" t="s">
         <v>290</v>
@@ -5146,26 +5152,26 @@
     <row r="62" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="118"/>
       <c r="C62" s="23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D62" s="98" t="s">
         <v>286</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F62" s="88" t="s">
-        <v>522</v>
-      </c>
-      <c r="G62" s="141"/>
+        <v>519</v>
+      </c>
+      <c r="G62" s="143"/>
       <c r="H62" s="23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I62" s="69" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K62" s="80"/>
       <c r="L62" s="80"/>
@@ -5197,12 +5203,12 @@
       <c r="F63" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="G63" s="141"/>
+      <c r="G63" s="143"/>
       <c r="H63" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K63" s="80"/>
       <c r="L63" s="80"/>
@@ -5225,17 +5231,17 @@
     <row r="64" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="118"/>
       <c r="C64" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D64" s="69" t="s">
         <v>337</v>
       </c>
-      <c r="G64" s="141"/>
+      <c r="G64" s="143"/>
       <c r="H64" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J64" s="23" t="s">
         <v>291</v>
@@ -5267,11 +5273,11 @@
         <v>25</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>543</v>
-      </c>
-      <c r="G65" s="141"/>
+        <v>540</v>
+      </c>
+      <c r="G65" s="143"/>
       <c r="H65" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I65" s="23"/>
       <c r="K65" s="80"/>
@@ -5296,21 +5302,21 @@
       <c r="A66" s="118"/>
       <c r="B66" s="82"/>
       <c r="C66" s="103" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D66" s="98" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E66" s="41"/>
       <c r="F66" s="23" t="s">
-        <v>542</v>
-      </c>
-      <c r="G66" s="141"/>
+        <v>539</v>
+      </c>
+      <c r="G66" s="143"/>
       <c r="H66" s="23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K66" s="80"/>
       <c r="L66" s="80"/>
@@ -5333,23 +5339,23 @@
     <row r="67" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="118"/>
       <c r="C67" s="102" t="s">
+        <v>538</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>435</v>
+      </c>
+      <c r="F67" s="23" t="s">
         <v>541</v>
       </c>
-      <c r="D67" s="23" t="s">
-        <v>436</v>
-      </c>
-      <c r="F67" s="23" t="s">
-        <v>544</v>
-      </c>
-      <c r="G67" s="141"/>
+      <c r="G67" s="143"/>
       <c r="H67" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I67" s="69" t="s">
         <v>45</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K67" s="80"/>
       <c r="L67" s="80"/>
@@ -5372,23 +5378,23 @@
     <row r="68" spans="1:27" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="118"/>
       <c r="C68" s="90" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D68" s="67" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F68" s="104" t="s">
-        <v>405</v>
-      </c>
-      <c r="G68" s="141"/>
+        <v>404</v>
+      </c>
+      <c r="G68" s="143"/>
       <c r="H68" s="23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="J68" s="104" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K68" s="80"/>
       <c r="L68" s="80"/>
@@ -5417,7 +5423,7 @@
       <c r="D69" s="129"/>
       <c r="G69" s="69"/>
       <c r="H69" s="23" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
@@ -5442,11 +5448,11 @@
         <v>191</v>
       </c>
       <c r="D70" s="116"/>
-      <c r="G70" s="157" t="s">
-        <v>494</v>
+      <c r="G70" s="164" t="s">
+        <v>491</v>
       </c>
       <c r="H70" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I70" s="115" t="s">
         <v>192</v>
@@ -5476,12 +5482,12 @@
       </c>
       <c r="D71" s="116"/>
       <c r="E71" s="115" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F71" s="116"/>
-      <c r="G71" s="158"/>
+      <c r="G71" s="165"/>
       <c r="H71" s="23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I71" s="115" t="s">
         <v>207</v>
@@ -5507,7 +5513,7 @@
       <c r="A72" s="118"/>
       <c r="B72" s="83"/>
       <c r="C72" s="123" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D72" s="124"/>
       <c r="E72" s="115" t="s">
@@ -5515,10 +5521,10 @@
       </c>
       <c r="F72" s="116"/>
       <c r="G72" s="95" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I72" s="115" t="s">
         <v>214</v>
@@ -5553,10 +5559,10 @@
       <c r="F73" s="116"/>
       <c r="G73" s="69"/>
       <c r="H73" s="105" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I73" s="115" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="J73" s="116"/>
       <c r="K73" s="9"/>
@@ -5577,10 +5583,10 @@
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="118"/>
-      <c r="E74" s="145" t="s">
-        <v>568</v>
-      </c>
-      <c r="F74" s="146"/>
+      <c r="E74" s="147" t="s">
+        <v>564</v>
+      </c>
+      <c r="F74" s="148"/>
       <c r="G74" s="69"/>
       <c r="I74" s="115" t="s">
         <v>218</v>
@@ -5612,10 +5618,10 @@
       </c>
       <c r="F75" s="134"/>
       <c r="G75" s="69"/>
-      <c r="I75" s="119" t="s">
-        <v>450</v>
-      </c>
-      <c r="J75" s="120"/>
+      <c r="I75" s="157" t="s">
+        <v>449</v>
+      </c>
+      <c r="J75" s="158"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -5638,12 +5644,12 @@
       <c r="C76" s="70"/>
       <c r="D76" s="71"/>
       <c r="E76" s="115" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F76" s="116"/>
       <c r="G76" s="69"/>
       <c r="J76" s="91" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
@@ -5696,19 +5702,19 @@
         <v>341</v>
       </c>
       <c r="D78" s="69" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G78" s="156" t="s">
-        <v>422</v>
+      <c r="G78" s="163" t="s">
+        <v>421</v>
       </c>
       <c r="H78" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="69" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -5731,7 +5737,7 @@
     <row r="79" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="131"/>
       <c r="C79" s="84" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D79" s="69" t="s">
         <v>58</v>
@@ -5744,7 +5750,7 @@
       </c>
       <c r="G79" s="122"/>
       <c r="H79" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I79" s="69" t="s">
         <v>33</v>
@@ -5783,7 +5789,7 @@
       </c>
       <c r="G80" s="122"/>
       <c r="H80" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I80" s="15" t="s">
         <v>59</v>
@@ -5813,20 +5819,20 @@
         <v>288</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E81" s="24" t="s">
         <v>293</v>
       </c>
       <c r="G81" s="122"/>
       <c r="H81" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I81" s="69" t="s">
         <v>49</v>
       </c>
       <c r="J81" s="69" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
@@ -5856,14 +5862,14 @@
         <v>253</v>
       </c>
       <c r="F82" s="98" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="G82" s="122"/>
       <c r="H82" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -5893,7 +5899,7 @@
       </c>
       <c r="G83" s="122"/>
       <c r="H83" s="4" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I83" s="98" t="s">
         <v>285</v>
@@ -5920,20 +5926,20 @@
     <row r="84" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="131"/>
       <c r="C84" s="4" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>296</v>
       </c>
       <c r="G84" s="122"/>
       <c r="H84" s="73" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>298</v>
@@ -5960,26 +5966,26 @@
     <row r="85" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="131"/>
       <c r="C85" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>297</v>
       </c>
       <c r="G85" s="122"/>
       <c r="H85" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
@@ -6000,17 +6006,17 @@
     <row r="86" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="131"/>
       <c r="C86" s="4" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E86" s="106" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="G86" s="122"/>
       <c r="H86" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>291</v>
@@ -6039,17 +6045,17 @@
     <row r="87" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="131"/>
       <c r="E87" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>394</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>395</v>
       </c>
       <c r="G87" s="122"/>
       <c r="H87" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>301</v>
@@ -6075,14 +6081,14 @@
       <c r="A88" s="131"/>
       <c r="C88" s="2"/>
       <c r="E88" s="89" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>242</v>
       </c>
       <c r="G88" s="122"/>
       <c r="H88" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L88" s="16"/>
       <c r="M88" s="16"/>
@@ -6105,10 +6111,10 @@
       <c r="A89" s="131"/>
       <c r="B89" s="29"/>
       <c r="G89" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I89" s="73" t="s">
         <v>231</v>
@@ -6135,18 +6141,18 @@
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="131"/>
-      <c r="C90" s="119" t="s">
-        <v>500</v>
-      </c>
-      <c r="D90" s="120"/>
+      <c r="C90" s="157" t="s">
+        <v>497</v>
+      </c>
+      <c r="D90" s="158"/>
       <c r="G90" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I90" s="89" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K90" s="16"/>
       <c r="L90" s="16"/>
@@ -6168,15 +6174,15 @@
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="131"/>
-      <c r="C91" s="119" t="s">
+      <c r="C91" s="157" t="s">
         <v>251</v>
       </c>
-      <c r="D91" s="155"/>
+      <c r="D91" s="160"/>
       <c r="H91" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I91" s="73" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K91" s="16"/>
       <c r="L91" s="16"/>
@@ -6201,7 +6207,7 @@
       <c r="E92" s="61"/>
       <c r="G92" s="32"/>
       <c r="H92" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J92" s="69"/>
       <c r="K92" s="16"/>
@@ -6225,11 +6231,11 @@
     <row r="93" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="131"/>
       <c r="C93" s="85" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="G93" s="32"/>
       <c r="H93" s="78" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="J93" s="69"/>
       <c r="K93" s="9"/>
@@ -6285,7 +6291,7 @@
       <c r="A95" s="131"/>
       <c r="B95" s="6"/>
       <c r="C95" s="115" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D95" s="116"/>
       <c r="E95" s="115" t="s">
@@ -6322,12 +6328,12 @@
       </c>
       <c r="D96" s="116"/>
       <c r="E96" s="125" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F96" s="122"/>
       <c r="G96" s="32"/>
       <c r="H96" s="115" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="I96" s="116"/>
       <c r="J96" s="61"/>
@@ -6351,19 +6357,19 @@
       <c r="A97" s="131"/>
       <c r="B97" s="6"/>
       <c r="C97" s="115" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D97" s="116"/>
       <c r="E97" s="125" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F97" s="122"/>
       <c r="G97" s="32"/>
       <c r="H97" s="69"/>
-      <c r="I97" s="119" t="s">
-        <v>533</v>
-      </c>
-      <c r="J97" s="120"/>
+      <c r="I97" s="157" t="s">
+        <v>530</v>
+      </c>
+      <c r="J97" s="158"/>
       <c r="K97" s="9"/>
       <c r="L97" s="9"/>
       <c r="M97" s="9"/>
@@ -6393,8 +6399,8 @@
       <c r="F98" s="122"/>
       <c r="G98" s="32"/>
       <c r="H98" s="75"/>
-      <c r="I98" s="143"/>
-      <c r="J98" s="144"/>
+      <c r="I98" s="145"/>
+      <c r="J98" s="146"/>
       <c r="K98" s="9"/>
       <c r="L98" s="9"/>
       <c r="M98" s="9"/>
@@ -6419,7 +6425,7 @@
       </c>
       <c r="D99" s="134"/>
       <c r="E99" s="133" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F99" s="134"/>
       <c r="G99" s="32"/>
@@ -6447,7 +6453,7 @@
       <c r="C100" s="70"/>
       <c r="D100" s="71"/>
       <c r="E100" s="115" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F100" s="116"/>
       <c r="G100" s="32"/>
@@ -6475,10 +6481,10 @@
       <c r="B101" s="6"/>
       <c r="C101" s="70"/>
       <c r="D101" s="71"/>
-      <c r="E101" s="148" t="s">
+      <c r="E101" s="150" t="s">
         <v>81</v>
       </c>
-      <c r="F101" s="148"/>
+      <c r="F101" s="150"/>
       <c r="G101" s="32"/>
       <c r="H101" s="75"/>
       <c r="J101" s="75"/>
@@ -6589,13 +6595,13 @@
         <v>17</v>
       </c>
       <c r="E105" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F105" s="88" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="G105" s="109" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="H105" s="34" t="s">
         <v>66</v>
@@ -6637,11 +6643,11 @@
         <v>44</v>
       </c>
       <c r="G106" s="110" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="H106" s="34"/>
       <c r="I106" s="23" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J106" s="69" t="s">
         <v>68</v>
@@ -6677,10 +6683,10 @@
         <v>50</v>
       </c>
       <c r="G107" s="97" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I107" s="15" t="s">
         <v>35</v>
@@ -6718,14 +6724,14 @@
       <c r="F108" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G108" s="140" t="s">
-        <v>423</v>
+      <c r="G108" s="142" t="s">
+        <v>422</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I108" s="92" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="J108" s="69" t="s">
         <v>38</v>
@@ -6752,11 +6758,11 @@
         <v>303</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="G109" s="141"/>
+        <v>445</v>
+      </c>
+      <c r="G109" s="143"/>
       <c r="H109" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>304</v>
@@ -6783,7 +6789,7 @@
     <row r="110" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="122"/>
       <c r="D110" s="98" t="s">
-        <v>349</v>
+        <v>574</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>307</v>
@@ -6791,7 +6797,7 @@
       <c r="F110" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G110" s="141"/>
+      <c r="G110" s="143"/>
       <c r="I110" s="69"/>
       <c r="J110" s="69"/>
       <c r="K110" s="16"/>
@@ -6815,12 +6821,12 @@
     <row r="111" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="122"/>
       <c r="D111" s="98" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F111" s="69" t="s">
-        <v>536</v>
-      </c>
-      <c r="G111" s="141"/>
+        <v>533</v>
+      </c>
+      <c r="G111" s="143"/>
       <c r="H111" s="36"/>
       <c r="I111" s="4" t="s">
         <v>233</v>
@@ -6847,9 +6853,9 @@
     <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="122"/>
       <c r="D112" s="23" t="s">
-        <v>350</v>
-      </c>
-      <c r="G112" s="141"/>
+        <v>349</v>
+      </c>
+      <c r="G112" s="143"/>
       <c r="H112" s="36"/>
       <c r="J112" s="2"/>
       <c r="K112" s="16"/>
@@ -6874,9 +6880,9 @@
       <c r="A113" s="122"/>
       <c r="C113" s="69"/>
       <c r="E113" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="G113" s="141"/>
+        <v>398</v>
+      </c>
+      <c r="G113" s="143"/>
       <c r="H113" s="34"/>
       <c r="J113" s="2"/>
       <c r="K113" s="16"/>
@@ -6900,9 +6906,9 @@
     <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="122"/>
       <c r="E114" s="4" t="s">
-        <v>547</v>
-      </c>
-      <c r="G114" s="141"/>
+        <v>544</v>
+      </c>
+      <c r="G114" s="143"/>
       <c r="H114" s="36"/>
       <c r="K114" s="16"/>
       <c r="L114" s="16"/>
@@ -6926,12 +6932,12 @@
       <c r="A115" s="122"/>
       <c r="D115" s="69"/>
       <c r="E115" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="G115" s="141"/>
+        <v>437</v>
+      </c>
+      <c r="G115" s="143"/>
       <c r="H115" s="36"/>
       <c r="J115" s="69"/>
       <c r="K115" s="16"/>
@@ -6955,9 +6961,9 @@
     <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="122"/>
       <c r="E116" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="G116" s="141"/>
+        <v>545</v>
+      </c>
+      <c r="G116" s="143"/>
       <c r="H116" s="69" t="s">
         <v>32</v>
       </c>
@@ -6988,7 +6994,7 @@
         <v>208</v>
       </c>
       <c r="F117" s="116"/>
-      <c r="G117" s="141"/>
+      <c r="G117" s="143"/>
       <c r="H117" s="15" t="s">
         <v>71</v>
       </c>
@@ -7017,13 +7023,13 @@
     <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="122"/>
       <c r="C118" s="85" t="s">
-        <v>519</v>
-      </c>
-      <c r="G118" s="141"/>
-      <c r="H118" s="145" t="s">
-        <v>458</v>
-      </c>
-      <c r="I118" s="146"/>
+        <v>516</v>
+      </c>
+      <c r="G118" s="143"/>
+      <c r="H118" s="147" t="s">
+        <v>457</v>
+      </c>
+      <c r="I118" s="148"/>
       <c r="K118" s="16"/>
       <c r="L118" s="16"/>
       <c r="M118" s="16"/>
@@ -7046,14 +7052,14 @@
       <c r="A119" s="122"/>
       <c r="B119" s="6"/>
       <c r="C119" s="115" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D119" s="116"/>
       <c r="E119" s="115" t="s">
         <v>222</v>
       </c>
       <c r="F119" s="116"/>
-      <c r="G119" s="141"/>
+      <c r="G119" s="143"/>
       <c r="I119" s="115" t="s">
         <v>195</v>
       </c>
@@ -7080,11 +7086,11 @@
       <c r="A120" s="122"/>
       <c r="B120" s="6"/>
       <c r="C120" s="115" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D120" s="116"/>
       <c r="E120" s="133" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F120" s="134"/>
       <c r="G120" s="35"/>
@@ -7115,13 +7121,13 @@
       <c r="A121" s="122"/>
       <c r="B121" s="6"/>
       <c r="C121" s="115" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D121" s="116"/>
-      <c r="E121" s="161" t="s">
-        <v>577</v>
-      </c>
-      <c r="F121" s="151"/>
+      <c r="E121" s="154" t="s">
+        <v>572</v>
+      </c>
+      <c r="F121" s="153"/>
       <c r="G121" s="35"/>
       <c r="H121" s="36"/>
       <c r="I121" s="115" t="s">
@@ -7154,7 +7160,7 @@
       </c>
       <c r="D122" s="116"/>
       <c r="E122" s="115" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F122" s="116"/>
       <c r="G122" s="35"/>
@@ -7184,14 +7190,14 @@
         <v>221</v>
       </c>
       <c r="D123" s="116"/>
-      <c r="E123" s="148" t="s">
-        <v>465</v>
+      <c r="E123" s="150" t="s">
+        <v>464</v>
       </c>
       <c r="F123" s="122"/>
       <c r="G123" s="35"/>
       <c r="H123" s="36"/>
-      <c r="I123" s="119"/>
-      <c r="J123" s="120"/>
+      <c r="I123" s="157"/>
+      <c r="J123" s="158"/>
       <c r="K123" s="16"/>
       <c r="L123" s="16"/>
       <c r="M123" s="16"/>
@@ -7213,18 +7219,18 @@
     <row r="124" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="122"/>
       <c r="B124" s="6"/>
-      <c r="C124" s="150" t="s">
-        <v>570</v>
-      </c>
-      <c r="D124" s="151"/>
+      <c r="C124" s="152" t="s">
+        <v>566</v>
+      </c>
+      <c r="D124" s="153"/>
       <c r="G124" s="35"/>
       <c r="H124" s="101" t="s">
-        <v>426</v>
-      </c>
-      <c r="I124" s="150" t="s">
-        <v>571</v>
-      </c>
-      <c r="J124" s="146"/>
+        <v>425</v>
+      </c>
+      <c r="I124" s="152" t="s">
+        <v>578</v>
+      </c>
+      <c r="J124" s="148"/>
       <c r="K124" s="16"/>
       <c r="L124" s="16"/>
       <c r="M124" s="16"/>
@@ -7250,10 +7256,10 @@
       <c r="D125" s="116"/>
       <c r="G125" s="35"/>
       <c r="H125" s="73"/>
-      <c r="I125" s="154" t="s">
-        <v>485</v>
-      </c>
-      <c r="J125" s="144"/>
+      <c r="I125" s="159" t="s">
+        <v>577</v>
+      </c>
+      <c r="J125" s="146"/>
       <c r="K125" s="16"/>
       <c r="L125" s="16"/>
       <c r="M125" s="16"/>
@@ -7424,7 +7430,7 @@
         <v>67</v>
       </c>
       <c r="H131" s="11"/>
-      <c r="I131" s="149"/>
+      <c r="I131" s="151"/>
       <c r="J131" s="122"/>
       <c r="K131" s="9"/>
       <c r="L131" s="9"/>
@@ -7448,10 +7454,10 @@
         <v>310</v>
       </c>
       <c r="D132" s="79" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F132" s="88" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="H132" s="11"/>
       <c r="I132" s="41"/>
@@ -7505,7 +7511,7 @@
     <row r="134" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="131"/>
       <c r="C134" s="15" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>312</v>
@@ -7564,13 +7570,13 @@
     <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="131"/>
       <c r="C136" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>313</v>
       </c>
       <c r="E136" s="98" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G136" s="2"/>
       <c r="I136" s="43"/>
@@ -7594,13 +7600,13 @@
     <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="131"/>
       <c r="C137" s="121" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>314</v>
       </c>
       <c r="E137" s="99" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G137" s="2"/>
       <c r="I137" s="43"/>
@@ -7657,7 +7663,7 @@
         <v>243</v>
       </c>
       <c r="F139" s="125" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="G139" s="122"/>
       <c r="H139" s="43"/>
@@ -7710,7 +7716,7 @@
     <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="131"/>
       <c r="C141" s="107" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E141" s="61"/>
       <c r="F141" s="126" t="s">
@@ -7739,7 +7745,7 @@
     <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="131"/>
       <c r="E142" s="85" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="G142" s="35"/>
       <c r="H142" s="43"/>
@@ -7820,14 +7826,14 @@
     <row r="145" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="131"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="152" t="s">
+      <c r="D145" s="155" t="s">
         <v>197</v>
       </c>
-      <c r="E145" s="153"/>
-      <c r="F145" s="159" t="s">
-        <v>576</v>
-      </c>
-      <c r="G145" s="160"/>
+      <c r="E145" s="156"/>
+      <c r="F145" s="135" t="s">
+        <v>571</v>
+      </c>
+      <c r="G145" s="136"/>
       <c r="H145" s="43"/>
       <c r="I145" s="43"/>
       <c r="J145" s="11"/>
@@ -7854,10 +7860,10 @@
         <v>198</v>
       </c>
       <c r="E146" s="116"/>
-      <c r="F146" s="135" t="s">
-        <v>486</v>
-      </c>
-      <c r="G146" s="136"/>
+      <c r="F146" s="137" t="s">
+        <v>483</v>
+      </c>
+      <c r="G146" s="138"/>
       <c r="H146" s="43"/>
       <c r="I146" s="43"/>
       <c r="J146" s="11"/>
@@ -7906,10 +7912,10 @@
     <row r="148" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="131"/>
       <c r="C148" s="2"/>
-      <c r="D148" s="162" t="s">
-        <v>578</v>
-      </c>
-      <c r="E148" s="163"/>
+      <c r="D148" s="119" t="s">
+        <v>573</v>
+      </c>
+      <c r="E148" s="120"/>
       <c r="H148" s="43"/>
       <c r="I148" s="43"/>
       <c r="J148" s="11"/>
@@ -7933,7 +7939,7 @@
       <c r="A149" s="131"/>
       <c r="C149" s="2"/>
       <c r="D149" s="125" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E149" s="122"/>
       <c r="F149" s="2"/>
@@ -7961,7 +7967,7 @@
       <c r="A150" s="131"/>
       <c r="C150" s="2"/>
       <c r="D150" s="125" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E150" s="122"/>
       <c r="F150" s="2"/>
@@ -8017,7 +8023,7 @@
       <c r="A152" s="132"/>
       <c r="C152" s="2"/>
       <c r="E152" s="115" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F152" s="116"/>
       <c r="G152" s="32"/>
@@ -8513,7 +8519,7 @@
         <v>148</v>
       </c>
       <c r="H166" s="59" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I166" s="59" t="s">
         <v>149</v>
@@ -8853,10 +8859,10 @@
       </c>
       <c r="F175" s="13"/>
       <c r="G175" s="58" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H175" s="58" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I175" s="58" t="s">
         <v>173</v>
@@ -8886,10 +8892,10 @@
       <c r="E176" s="13"/>
       <c r="F176" s="13"/>
       <c r="G176" s="58" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H176" s="58" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I176" s="58" t="s">
         <v>174</v>
@@ -9328,7 +9334,7 @@
       <c r="C192" s="58"/>
       <c r="D192" s="58"/>
       <c r="E192" s="58"/>
-      <c r="F192" s="147"/>
+      <c r="F192" s="149"/>
       <c r="J192" s="13"/>
       <c r="K192" s="9"/>
       <c r="L192" s="9"/>
@@ -9403,7 +9409,7 @@
       <c r="C195" s="58"/>
       <c r="D195" s="58"/>
       <c r="E195" s="58"/>
-      <c r="F195" s="147"/>
+      <c r="F195" s="149"/>
       <c r="G195" s="9"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>

</xml_diff>